<commit_message>
added absquant workflow diagrams, expanded example worksheet to support diagrams, fixed typo in calc_cell_counts
</commit_message>
<xml_diff>
--- a/docs/absolute_quant_example.xlsx
+++ b/docs/absolute_quant_example.xlsx
@@ -1,26 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abirmingham/Work/Repositories/pysyndna/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abirmingham/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F3AF709-F60E-344F-B55B-82DFFC4BA8FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:2001_{B806CE7F-E384-A04D-B7E0-583EA7BFBFCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4700" yWindow="11020" windowWidth="31480" windowHeight="15160" xr2:uid="{E184B90C-6432-8947-B7A0-BE1974B73180}"/>
+    <workbookView xWindow="1440" yWindow="940" windowWidth="26580" windowHeight="15160" firstSheet="1" activeTab="2" xr2:uid="{E184B90C-6432-8947-B7A0-BE1974B73180}"/>
   </bookViews>
   <sheets>
     <sheet name="full_calcs on correct masses " sheetId="16" r:id="rId1"/>
     <sheet name="linear regressions counts" sheetId="17" r:id="rId2"/>
-    <sheet name="full_calcs on Zaramela masses " sheetId="1" r:id="rId3"/>
-    <sheet name="linear regressions CPMs" sheetId="2" r:id="rId4"/>
-    <sheet name="zaramela linear reg CPM&amp;counts " sheetId="15" r:id="rId5"/>
-    <sheet name="syndna_saliva_analysis_ex1" sheetId="14" r:id="rId6"/>
+    <sheet name="diagrm artifacts from linregcts" sheetId="19" r:id="rId3"/>
+    <sheet name="full_calcs on Zaramela masses " sheetId="1" r:id="rId4"/>
+    <sheet name="linear regressions CPMs" sheetId="2" r:id="rId5"/>
+    <sheet name="zaramela linear reg CPM&amp;counts " sheetId="15" r:id="rId6"/>
+    <sheet name="syndna_saliva_analysis_ex1" sheetId="14" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2115,7 +2117,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -2137,7 +2139,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1410" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1593" uniqueCount="309">
   <si>
     <t>variable name</t>
   </si>
@@ -2968,21 +2970,118 @@
   </si>
   <si>
     <t>ogu_cells_per_g_gdna * gdna_mass_to_sample_surface_area_ratio</t>
+  </si>
+  <si>
+    <t>read_counts</t>
+  </si>
+  <si>
+    <t>sampleA</t>
+  </si>
+  <si>
+    <t>sampleA:</t>
+  </si>
+  <si>
+    <t>slope: 1.24487652379132</t>
+  </si>
+  <si>
+    <t>intercept: -7.35593916054843</t>
+  </si>
+  <si>
+    <t>rvalue: 0.986503097515657</t>
+  </si>
+  <si>
+    <t>pvalue: 1.42844356065977E-07</t>
+  </si>
+  <si>
+    <t>stderr: 0.073657952553024</t>
+  </si>
+  <si>
+    <t>intercept_stderr: 0.271274537363401</t>
+  </si>
+  <si>
+    <t>OGU_ID</t>
+  </si>
+  <si>
+    <t>G100014425</t>
+  </si>
+  <si>
+    <t>*THESE ARE FAKE. t is not possible to match up all of these species with lineage values in the "lineages.txt" file from http://ftp.microbio.me/pub/wol2/taxonomy/ , and where it is, the lengths in the lengths.map file don't exactly match the lengths used in the Zaramela calcs (and thus in the test calcs).  I picked the closest OGU id I could find and replaced the leftmost zero with a 1 to indicate it is a dummy</t>
+  </si>
+  <si>
+    <t>G100179635</t>
+  </si>
+  <si>
+    <t>G100026325</t>
+  </si>
+  <si>
+    <t>G100185145</t>
+  </si>
+  <si>
+    <t>G100027165</t>
+  </si>
+  <si>
+    <t>G101485215</t>
+  </si>
+  <si>
+    <t>OGU_id</t>
+  </si>
+  <si>
+    <t>G101488575</t>
+  </si>
+  <si>
+    <t>&lt;- this one is made up, just to have something to throw out in illustration for having low overall OGU genome coverage</t>
+  </si>
+  <si>
+    <t>coverage_percent</t>
+  </si>
+  <si>
+    <t>These OGU coverage percentages are MADE UP (kinda have to be since the ogu ids are made up) ... just shows G101488575 as having &lt;1% coverage, for use in illustration</t>
+  </si>
+  <si>
+    <t>gdna_ng</t>
+  </si>
+  <si>
+    <t>length_in_bp</t>
+  </si>
+  <si>
+    <t>&lt;-for Lactobacillus gasseri, from full_calcs on correct masses sheet, truncated to integer</t>
+  </si>
+  <si>
+    <t>&lt;-for Ruminococcus albus, from full_calcs on correct masses sheet</t>
+  </si>
+  <si>
+    <t>&lt;-for Leptolyngbya valderiana, from full_calcs on correct masses sheet</t>
+  </si>
+  <si>
+    <t>made up value</t>
+  </si>
+  <si>
+    <t>num_genomes</t>
+  </si>
+  <si>
+    <t>num_genomes_per_g_gdna</t>
+  </si>
+  <si>
+    <t>num_genomes_per_g_sample</t>
+  </si>
+  <si>
+    <t>num_cells_per_g_sample</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="6">
+  <numFmts count="7">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.00000000E+00"/>
     <numFmt numFmtId="166" formatCode="0.000E+00"/>
     <numFmt numFmtId="167" formatCode="0.0000000000E+00"/>
     <numFmt numFmtId="168" formatCode="0.000000000000000E+00"/>
     <numFmt numFmtId="169" formatCode="0.0"/>
+    <numFmt numFmtId="171" formatCode="0.000000E+00"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3039,6 +3138,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -3078,7 +3183,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -3186,12 +3291,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3242,17 +3362,17 @@
     <xf numFmtId="166" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3274,6 +3394,1099 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'diagrm artifacts from linregcts'!$I$17:$I$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>4.9691129189016641</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.181557773862786</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.3886339693517891</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.4885507165004443</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.8864907251724818</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.173186268412274</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.0314084642516241</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.5036545192429593</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.4039265648312682</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.3753508093107225</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'diagrm artifacts from linregcts'!$J$17:$J$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>-0.94884313458608482</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-1.9488431345860848</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-2.9488431345860846</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-3.9488431345860846</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-4.9488431345860846</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-4.9488431345860846</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-3.9488431345860846</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-2.9488431345860846</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-1.9488431345860848</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-0.94884313458608482</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-C89A-D242-9DD4-C182935FE840}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1853351567"/>
+        <c:axId val="1660587999"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1853351567"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>log10(syndna</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> read</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t> counts)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1660587999"/>
+        <c:crossesAt val="-6"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1660587999"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>log10(syndna ng)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1853351567"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>539750</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B255ED9-38DC-EB45-8691-A9E5E0B00A4F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3575,9 +4788,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA83768D-892A-3A42-8EA4-41D4B20C5948}">
   <dimension ref="A1:M106"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D107" sqref="D107"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5250,23 +6463,23 @@
       <c r="B48" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="C48" s="46" t="b">
-        <v>1</v>
-      </c>
-      <c r="D48" s="46" t="s">
+      <c r="C48" t="b">
+        <v>1</v>
+      </c>
+      <c r="D48" t="s">
         <v>98</v>
       </c>
-      <c r="E48" s="46" t="s">
+      <c r="E48" t="s">
         <v>13</v>
       </c>
-      <c r="F48" s="46" t="s">
+      <c r="F48" t="s">
         <v>99</v>
       </c>
-      <c r="G48" s="49">
+      <c r="G48" s="27">
         <f>G47*10^9</f>
         <v>5438449731907.9639</v>
       </c>
-      <c r="H48" s="49">
+      <c r="H48" s="27">
         <f>H47*10^9</f>
         <v>4698653063541.4355</v>
       </c>
@@ -5274,7 +6487,7 @@
         <f>I47*10^9</f>
         <v>5438449731907.9639</v>
       </c>
-      <c r="J48" s="49">
+      <c r="J48" s="27">
         <f>J47*10^9</f>
         <v>4698653063541.4355</v>
       </c>
@@ -5289,23 +6502,23 @@
       <c r="B49" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="C49" s="46" t="b">
-        <v>1</v>
-      </c>
-      <c r="D49" s="46" t="s">
+      <c r="C49" t="b">
+        <v>1</v>
+      </c>
+      <c r="D49" t="s">
         <v>101</v>
       </c>
-      <c r="E49" s="46" t="s">
+      <c r="E49" t="s">
         <v>13</v>
       </c>
-      <c r="F49" s="46" t="s">
+      <c r="F49" t="s">
         <v>102</v>
       </c>
-      <c r="G49" s="47">
+      <c r="G49" s="4">
         <f>G48*G$29</f>
         <v>39084741.271463379</v>
       </c>
-      <c r="H49" s="47">
+      <c r="H49" s="4">
         <f>H48*H29</f>
         <v>22304970.753461108</v>
       </c>
@@ -5313,7 +6526,7 @@
         <f>I48*I29</f>
         <v>82077956.670073092</v>
       </c>
-      <c r="J49" s="47">
+      <c r="J49" s="4">
         <f>J48*J29</f>
         <v>15613479.527422776</v>
       </c>
@@ -5328,31 +6541,31 @@
       <c r="B50" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="C50" s="46" t="b">
-        <v>1</v>
-      </c>
-      <c r="D50" s="48" t="s">
+      <c r="C50" t="b">
+        <v>1</v>
+      </c>
+      <c r="D50" t="s">
         <v>270</v>
       </c>
       <c r="E50" t="s">
         <v>13</v>
       </c>
-      <c r="F50" s="48" t="s">
+      <c r="F50" t="s">
         <v>271</v>
       </c>
-      <c r="G50" s="47">
+      <c r="G50" s="4">
         <f>G48*G$30</f>
         <v>5438.4497319079646</v>
       </c>
-      <c r="H50" s="47">
+      <c r="H50" s="4">
         <f>H48*H30</f>
         <v>4385.409525972007</v>
       </c>
-      <c r="I50" s="47">
+      <c r="I50" s="4">
         <f>I48*I30</f>
         <v>11420.744437006726</v>
       </c>
-      <c r="J50" s="47">
+      <c r="J50" s="4">
         <f>J48*J30</f>
         <v>3069.7866681804048</v>
       </c>
@@ -5370,13 +6583,13 @@
       <c r="C51" s="13" t="b">
         <v>1</v>
       </c>
-      <c r="D51" s="50" t="s">
+      <c r="D51" s="13" t="s">
         <v>272</v>
       </c>
       <c r="E51" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F51" s="50" t="s">
+      <c r="F51" s="13" t="s">
         <v>273</v>
       </c>
       <c r="G51" s="36">
@@ -5403,14 +6616,10 @@
       </c>
     </row>
     <row r="52" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B52" s="46"/>
-      <c r="C52" s="46"/>
-      <c r="D52" s="48"/>
-      <c r="F52" s="48"/>
-      <c r="G52" s="47"/>
-      <c r="H52" s="47"/>
-      <c r="I52" s="47"/>
-      <c r="J52" s="47"/>
+      <c r="G52" s="4"/>
+      <c r="H52" s="4"/>
+      <c r="I52" s="4"/>
+      <c r="J52" s="4"/>
     </row>
     <row r="53" spans="2:13" x14ac:dyDescent="0.2">
       <c r="G53" s="4" t="s">
@@ -5624,19 +6833,19 @@
       </c>
     </row>
     <row r="60" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B60" s="46" t="s">
+      <c r="B60" t="s">
         <v>82</v>
       </c>
-      <c r="C60" s="46" t="b">
-        <v>1</v>
-      </c>
-      <c r="D60" s="48" t="s">
+      <c r="C60" t="b">
+        <v>1</v>
+      </c>
+      <c r="D60" t="s">
         <v>270</v>
       </c>
-      <c r="E60" s="46" t="s">
+      <c r="E60" t="s">
         <v>13</v>
       </c>
-      <c r="F60" s="48" t="s">
+      <c r="F60" t="s">
         <v>271</v>
       </c>
       <c r="G60" s="4">
@@ -5644,32 +6853,32 @@
         <v>2859.9177577571454</v>
       </c>
       <c r="H60" s="4">
-        <f t="shared" ref="H60:J60" si="0">H58*H$30</f>
+        <f>H58*H$30</f>
         <v>2306.7771489585143</v>
       </c>
       <c r="I60" s="4">
-        <f t="shared" si="0"/>
+        <f>I58*I$30</f>
         <v>6005.8272912900047</v>
       </c>
       <c r="J60" s="4">
-        <f t="shared" si="0"/>
+        <f>J58*J$30</f>
         <v>1614.74400427096</v>
       </c>
     </row>
     <row r="61" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B61" s="46" t="s">
+      <c r="B61" t="s">
         <v>82</v>
       </c>
-      <c r="C61" s="46" t="b">
-        <v>1</v>
-      </c>
-      <c r="D61" s="48" t="s">
+      <c r="C61" t="b">
+        <v>1</v>
+      </c>
+      <c r="D61" t="s">
         <v>272</v>
       </c>
-      <c r="E61" s="46" t="s">
+      <c r="E61" t="s">
         <v>13</v>
       </c>
-      <c r="F61" s="48" t="s">
+      <c r="F61" t="s">
         <v>273</v>
       </c>
       <c r="G61" s="4">
@@ -5677,15 +6886,15 @@
         <v>142995.88788785727</v>
       </c>
       <c r="H61" s="4">
-        <f t="shared" ref="H61:J61" si="1">H58*H$31</f>
+        <f>H58*H$31</f>
         <v>57669.428723962861</v>
       </c>
       <c r="I61" s="4">
-        <f t="shared" si="1"/>
+        <f>I58*I$31</f>
         <v>300291.36456450023</v>
       </c>
       <c r="J61" s="4">
-        <f t="shared" si="1"/>
+        <f>J58*J$31</f>
         <v>40368.600106774</v>
       </c>
     </row>
@@ -5877,31 +7086,31 @@
       <c r="B69" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="C69" s="46" t="b">
-        <v>1</v>
-      </c>
-      <c r="D69" s="46" t="s">
+      <c r="C69" t="b">
+        <v>1</v>
+      </c>
+      <c r="D69" t="s">
         <v>101</v>
       </c>
-      <c r="E69" s="46" t="s">
+      <c r="E69" t="s">
         <v>13</v>
       </c>
-      <c r="F69" s="46" t="s">
+      <c r="F69" t="s">
         <v>102</v>
       </c>
-      <c r="G69" s="51">
+      <c r="G69" s="46">
         <f>G68*G$29</f>
         <v>8324307.6720339339</v>
       </c>
-      <c r="H69" s="51">
+      <c r="H69" s="46">
         <f>H68*H$29</f>
         <v>4717478.5789171578</v>
       </c>
-      <c r="I69" s="51">
+      <c r="I69" s="46">
         <f>I68*I$29</f>
         <v>17481046.111271258</v>
       </c>
-      <c r="J69" s="51">
+      <c r="J69" s="46">
         <f>J68*J$29</f>
         <v>3302235.005242011</v>
       </c>
@@ -5910,32 +7119,32 @@
       <c r="B70" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="C70" s="46" t="b">
-        <v>1</v>
-      </c>
-      <c r="D70" s="48" t="s">
+      <c r="C70" t="b">
+        <v>1</v>
+      </c>
+      <c r="D70" t="s">
         <v>270</v>
       </c>
       <c r="E70" t="s">
         <v>13</v>
       </c>
-      <c r="F70" s="48" t="s">
+      <c r="F70" t="s">
         <v>271</v>
       </c>
-      <c r="G70" s="47">
+      <c r="G70" s="4">
         <f>G68*G$30</f>
         <v>1158.2865167984608</v>
       </c>
-      <c r="H70" s="47">
-        <f t="shared" ref="H70:J70" si="2">H68*H$30</f>
+      <c r="H70" s="4">
+        <f>H68*H$30</f>
         <v>927.50964469845724</v>
       </c>
-      <c r="I70" s="47">
-        <f t="shared" si="2"/>
+      <c r="I70" s="4">
+        <f>I68*I$30</f>
         <v>2432.4016852767677</v>
       </c>
-      <c r="J70" s="47">
-        <f t="shared" si="2"/>
+      <c r="J70" s="4">
+        <f>J68*J$30</f>
         <v>649.25675128891999</v>
       </c>
     </row>
@@ -5946,13 +7155,13 @@
       <c r="C71" s="13" t="b">
         <v>1</v>
       </c>
-      <c r="D71" s="50" t="s">
+      <c r="D71" s="13" t="s">
         <v>272</v>
       </c>
       <c r="E71" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F71" s="50" t="s">
+      <c r="F71" s="13" t="s">
         <v>273</v>
       </c>
       <c r="G71" s="36">
@@ -5960,28 +7169,23 @@
         <v>57914.32583992304</v>
       </c>
       <c r="H71" s="36">
-        <f t="shared" ref="H71:J71" si="3">H68*H$31</f>
+        <f>H68*H$31</f>
         <v>23187.741117461428</v>
       </c>
       <c r="I71" s="36">
-        <f t="shared" si="3"/>
+        <f>I68*I$31</f>
         <v>121620.08426383838</v>
       </c>
       <c r="J71" s="36">
-        <f t="shared" si="3"/>
+        <f>J68*J$31</f>
         <v>16231.418782223</v>
       </c>
     </row>
     <row r="72" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B72" s="46"/>
-      <c r="C72" s="46"/>
-      <c r="D72" s="46"/>
-      <c r="E72" s="46"/>
-      <c r="F72" s="46"/>
-      <c r="G72" s="47"/>
-      <c r="H72" s="47"/>
-      <c r="I72" s="47"/>
-      <c r="J72" s="47"/>
+      <c r="G72" s="4"/>
+      <c r="H72" s="4"/>
+      <c r="I72" s="4"/>
+      <c r="J72" s="4"/>
     </row>
     <row r="73" spans="2:12" x14ac:dyDescent="0.2">
       <c r="G73" s="4"/>
@@ -6216,31 +7420,31 @@
       <c r="B82" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="C82" s="52" t="b">
-        <v>1</v>
-      </c>
-      <c r="D82" s="52" t="s">
+      <c r="C82" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="D82" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="E82" s="52" t="s">
+      <c r="E82" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="F82" s="52" t="s">
+      <c r="F82" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="G82" s="53">
+      <c r="G82" s="39">
         <f>G81*G$29</f>
         <v>39085654.849706717</v>
       </c>
-      <c r="H82" s="53">
+      <c r="H82" s="39">
         <f>H81*H$29</f>
         <v>22305492.116410837</v>
       </c>
-      <c r="I82" s="53">
+      <c r="I82" s="39">
         <f>I81*I$29</f>
         <v>82079875.184384093</v>
       </c>
-      <c r="J82" s="53">
+      <c r="J82" s="39">
         <f>J81*J$29</f>
         <v>15613844.481487585</v>
       </c>
@@ -6252,29 +7456,29 @@
       <c r="C83" s="19" t="b">
         <v>1</v>
       </c>
-      <c r="D83" s="52" t="s">
+      <c r="D83" s="19" t="s">
         <v>270</v>
       </c>
       <c r="E83" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="F83" s="52" t="s">
+      <c r="F83" s="19" t="s">
         <v>271</v>
       </c>
-      <c r="G83" s="53">
+      <c r="G83" s="39">
         <f>G81*G$30</f>
         <v>5438.5768518322857</v>
       </c>
-      <c r="H83" s="53">
-        <f t="shared" ref="H83:J83" si="4">H81*H$30</f>
+      <c r="H83" s="39">
+        <f>H81*H$30</f>
         <v>4385.5120318246927</v>
       </c>
-      <c r="I83" s="53">
-        <f t="shared" si="4"/>
+      <c r="I83" s="39">
+        <f>I81*I$30</f>
         <v>11421.011388847799</v>
       </c>
-      <c r="J83" s="53">
-        <f t="shared" si="4"/>
+      <c r="J83" s="39">
+        <f>J81*J$30</f>
         <v>3069.8584222772852</v>
       </c>
     </row>
@@ -6299,28 +7503,23 @@
         <v>271928.84259161429</v>
       </c>
       <c r="H84" s="38">
-        <f t="shared" ref="H84:J84" si="5">H81*H$31</f>
+        <f>H81*H$31</f>
         <v>109637.80079561732</v>
       </c>
       <c r="I84" s="38">
-        <f t="shared" si="5"/>
+        <f>I81*I$31</f>
         <v>571050.56944239</v>
       </c>
       <c r="J84" s="38">
-        <f t="shared" si="5"/>
+        <f>J81*J$31</f>
         <v>76746.460556932128</v>
       </c>
     </row>
     <row r="85" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B85" s="48"/>
-      <c r="C85" s="48"/>
-      <c r="D85" s="48"/>
-      <c r="E85" s="54"/>
-      <c r="F85" s="48"/>
-      <c r="G85" s="55"/>
-      <c r="H85" s="55"/>
-      <c r="I85" s="55"/>
-      <c r="J85" s="55"/>
+      <c r="G85" s="4"/>
+      <c r="H85" s="4"/>
+      <c r="I85" s="4"/>
+      <c r="J85" s="4"/>
     </row>
     <row r="86" spans="2:12" x14ac:dyDescent="0.2">
       <c r="G86" s="4" t="s">
@@ -6554,15 +7753,15 @@
         <v>2859.9846063163582</v>
       </c>
       <c r="H93" s="39">
-        <f t="shared" ref="H93:J93" si="6">H91*H$30</f>
+        <f>H91*H$30</f>
         <v>2306.8310682463734</v>
       </c>
       <c r="I93" s="39">
-        <f t="shared" si="6"/>
+        <f>I91*I$30</f>
         <v>6005.967673264352</v>
       </c>
       <c r="J93" s="39">
-        <f t="shared" si="6"/>
+        <f>J91*J$30</f>
         <v>1614.7817477724611</v>
       </c>
     </row>
@@ -6587,28 +7786,23 @@
         <v>142999.2303158179</v>
       </c>
       <c r="H94" s="39">
-        <f t="shared" ref="H94:J94" si="7">H91*H$31</f>
+        <f>H91*H$31</f>
         <v>57670.776706159326</v>
       </c>
       <c r="I94" s="39">
-        <f t="shared" si="7"/>
+        <f>I91*I$31</f>
         <v>300298.3836632176</v>
       </c>
       <c r="J94" s="39">
-        <f t="shared" si="7"/>
+        <f>J91*J$31</f>
         <v>40369.543694311527</v>
       </c>
     </row>
     <row r="95" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B95" s="48"/>
-      <c r="C95" s="48"/>
-      <c r="D95" s="48"/>
-      <c r="E95" s="54"/>
-      <c r="F95" s="48"/>
-      <c r="G95" s="55"/>
-      <c r="H95" s="55"/>
-      <c r="I95" s="55"/>
-      <c r="J95" s="55"/>
+      <c r="G95" s="4"/>
+      <c r="H95" s="4"/>
+      <c r="I95" s="4"/>
+      <c r="J95" s="4"/>
     </row>
     <row r="96" spans="2:12" x14ac:dyDescent="0.2">
       <c r="G96" s="4" t="s">
@@ -6792,31 +7986,31 @@
       <c r="B102" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="C102" s="52" t="b">
-        <v>1</v>
-      </c>
-      <c r="D102" s="52" t="s">
+      <c r="C102" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="D102" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="E102" s="52" t="s">
+      <c r="E102" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="F102" s="52" t="s">
+      <c r="F102" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="G102" s="56">
+      <c r="G102" s="47">
         <f>G101*G$29</f>
         <v>8324502.2468509236</v>
       </c>
-      <c r="H102" s="56">
+      <c r="H102" s="47">
         <f>H101*H$29</f>
         <v>4717588.8466496002</v>
       </c>
-      <c r="I102" s="56">
+      <c r="I102" s="47">
         <f>I101*I$29</f>
         <v>17481454.718386941</v>
       </c>
-      <c r="J102" s="56">
+      <c r="J102" s="47">
         <f>J101*J$29</f>
         <v>3302312.1926547205</v>
       </c>
@@ -6828,29 +8022,29 @@
       <c r="C103" s="19" t="b">
         <v>1</v>
       </c>
-      <c r="D103" s="52" t="s">
+      <c r="D103" s="19" t="s">
         <v>270</v>
       </c>
       <c r="E103" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="F103" s="52" t="s">
+      <c r="F103" s="19" t="s">
         <v>271</v>
       </c>
-      <c r="G103" s="53">
+      <c r="G103" s="39">
         <f>G101*G$30</f>
         <v>1158.3135909283353</v>
       </c>
-      <c r="H103" s="53">
-        <f t="shared" ref="H103:J103" si="8">H101*H$30</f>
+      <c r="H103" s="39">
+        <f>H101*H$30</f>
         <v>927.53132458181619</v>
       </c>
-      <c r="I103" s="53">
-        <f t="shared" si="8"/>
+      <c r="I103" s="39">
+        <f>I101*I$30</f>
         <v>2432.4585409495044</v>
       </c>
-      <c r="J103" s="53">
-        <f t="shared" si="8"/>
+      <c r="J103" s="39">
+        <f>J101*J$30</f>
         <v>649.27192720727123</v>
       </c>
     </row>
@@ -6875,15 +8069,15 @@
         <v>57915.679546416766</v>
       </c>
       <c r="H104" s="38">
-        <f t="shared" ref="H104:J104" si="9">H101*H$31</f>
+        <f>H101*H$31</f>
         <v>23188.283114545404</v>
       </c>
       <c r="I104" s="38">
-        <f t="shared" si="9"/>
+        <f>I101*I$31</f>
         <v>121622.9270474752</v>
       </c>
       <c r="J104" s="38">
-        <f t="shared" si="9"/>
+        <f>J101*J$31</f>
         <v>16231.798180181782</v>
       </c>
     </row>
@@ -6901,11 +8095,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFC0DD12-9F50-4C4C-88FA-79E5E161A3E2}">
   <dimension ref="A1:M146"/>
   <sheetViews>
-    <sheetView topLeftCell="A113" workbookViewId="0">
-      <selection activeCell="O140" sqref="O140"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J40" sqref="J40:J48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="11" max="11" width="23.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -7795,7 +8992,7 @@
         <v>93024</v>
       </c>
       <c r="M43">
-        <f t="shared" ref="M43:M54" si="4">10^($B$57*LOG10(L43)+$B$56)</f>
+        <f>10^($B$57*LOG10(L43)+$B$56)</f>
         <v>6.7506893569518861E-2</v>
       </c>
     </row>
@@ -7813,7 +9010,7 @@
         <v>86188</v>
       </c>
       <c r="M44">
-        <f t="shared" si="4"/>
+        <f>10^($B$57*LOG10(L44)+$B$56)</f>
         <v>6.1387888964041307E-2</v>
       </c>
     </row>
@@ -7831,7 +9028,7 @@
         <v>45441</v>
       </c>
       <c r="M45">
-        <f t="shared" si="4"/>
+        <f>10^($B$57*LOG10(L45)+$B$56)</f>
         <v>2.7669949480603664E-2</v>
       </c>
     </row>
@@ -7849,7 +9046,7 @@
         <v>31185</v>
       </c>
       <c r="M46">
-        <f t="shared" si="4"/>
+        <f>10^($B$57*LOG10(L46)+$B$56)</f>
         <v>1.731683029216274E-2</v>
       </c>
     </row>
@@ -7867,7 +9064,7 @@
         <v>24929</v>
       </c>
       <c r="M47">
-        <f t="shared" si="4"/>
+        <f>10^($B$57*LOG10(L47)+$B$56)</f>
         <v>1.3104350443761088E-2</v>
       </c>
     </row>
@@ -7879,7 +9076,7 @@
         <v>1975</v>
       </c>
       <c r="M48">
-        <f t="shared" si="4"/>
+        <f>10^($B$57*LOG10(L48)+$B$56)</f>
         <v>5.5800097113146443E-4</v>
       </c>
     </row>
@@ -7894,7 +9091,7 @@
         <v>26130</v>
       </c>
       <c r="M49">
-        <f t="shared" si="4"/>
+        <f>10^($B$57*LOG10(L49)+$B$56)</f>
         <v>1.3894854164478233E-2</v>
       </c>
     </row>
@@ -7922,7 +9119,7 @@
         <v>22303</v>
       </c>
       <c r="M50">
-        <f t="shared" si="4"/>
+        <f>10^($B$57*LOG10(L50)+$B$56)</f>
         <v>1.1408701284690223E-2</v>
       </c>
     </row>
@@ -7952,7 +9149,7 @@
         <v>19783</v>
       </c>
       <c r="M51">
-        <f t="shared" si="4"/>
+        <f>10^($B$57*LOG10(L51)+$B$56)</f>
         <v>9.8268443584452556E-3</v>
       </c>
     </row>
@@ -7976,7 +9173,7 @@
         <v>14478</v>
       </c>
       <c r="M52">
-        <f t="shared" si="4"/>
+        <f>10^($B$57*LOG10(L52)+$B$56)</f>
         <v>6.6623779084662204E-3</v>
       </c>
     </row>
@@ -8000,7 +9197,7 @@
         <v>12145</v>
       </c>
       <c r="M53">
-        <f t="shared" si="4"/>
+        <f>10^($B$57*LOG10(L53)+$B$56)</f>
         <v>5.3534213285283943E-3</v>
       </c>
     </row>
@@ -8012,7 +9209,7 @@
         <v>14609</v>
       </c>
       <c r="M54">
-        <f t="shared" si="4"/>
+        <f>10^($B$57*LOG10(L54)+$B$56)</f>
         <v>6.7375052531226162E-3</v>
       </c>
     </row>
@@ -8159,7 +9356,7 @@
         <v>93024</v>
       </c>
       <c r="M66">
-        <f t="shared" ref="M66:M77" si="5">10^($B$80*LOG10(L66)+$B$79)</f>
+        <f t="shared" ref="M66:M77" si="4">10^($B$80*LOG10(L66)+$B$79)</f>
         <v>5.5539298723601756E-2</v>
       </c>
     </row>
@@ -8177,7 +9374,7 @@
         <v>86188</v>
       </c>
       <c r="M67">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>5.0497812064730196E-2</v>
       </c>
     </row>
@@ -8195,7 +9392,7 @@
         <v>45441</v>
       </c>
       <c r="M68">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2.2733948133172519E-2</v>
       </c>
     </row>
@@ -8213,7 +9410,7 @@
         <v>31185</v>
       </c>
       <c r="M69">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.4217626083413358E-2</v>
       </c>
     </row>
@@ -8231,7 +9428,7 @@
         <v>24929</v>
       </c>
       <c r="M70">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.075452217344529E-2</v>
       </c>
     </row>
@@ -8243,7 +9440,7 @@
         <v>1975</v>
       </c>
       <c r="M71">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>4.5576142039897643E-4</v>
       </c>
     </row>
@@ -8258,7 +9455,7 @@
         <v>0</v>
       </c>
       <c r="M72" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>#NUM!</v>
       </c>
     </row>
@@ -8286,7 +9483,7 @@
         <v>22303</v>
       </c>
       <c r="M73">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>9.3609693069967321E-3</v>
       </c>
     </row>
@@ -8316,7 +9513,7 @@
         <v>197830</v>
       </c>
       <c r="M74">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.14228522207085967</v>
       </c>
     </row>
@@ -8340,7 +9537,7 @@
         <v>14478</v>
       </c>
       <c r="M75">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>5.4621119181234735E-3</v>
       </c>
     </row>
@@ -8364,7 +9561,7 @@
         <v>100</v>
       </c>
       <c r="M76">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.1052930563393005E-5</v>
       </c>
     </row>
@@ -8376,7 +9573,7 @@
         <v>14609</v>
       </c>
       <c r="M77">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>5.5237983062126324E-3</v>
       </c>
     </row>
@@ -8444,7 +9641,7 @@
         <v>1.24675913604407</v>
       </c>
       <c r="C80" s="30">
-        <v>7.3657952553023986E-2</v>
+        <v>7.3657952553024E-2</v>
       </c>
       <c r="D80" s="30">
         <v>16.92633439880872</v>
@@ -8558,19 +9755,19 @@
         <v>0.1</v>
       </c>
       <c r="G87">
-        <f t="shared" ref="G87:G103" si="6">F87/(2*(1+0.1+0.01+0.001+0.0001))</f>
+        <f t="shared" ref="G87:G103" si="5">F87/(2*(1+0.1+0.01+0.001+0.0001))</f>
         <v>4.5000450004500051E-2</v>
       </c>
       <c r="H87">
-        <f t="shared" ref="H87:H103" si="7">E87*G87</f>
+        <f t="shared" ref="H87:H103" si="6">E87*G87</f>
         <v>1.1250112501125013E-2</v>
       </c>
       <c r="I87">
-        <f t="shared" ref="I87:I103" si="8">LOG10(C87)</f>
+        <f t="shared" ref="I87:I103" si="7">LOG10(C87)</f>
         <v>4.181557773862786</v>
       </c>
       <c r="J87" s="2">
-        <f t="shared" ref="J87:J103" si="9">LOG10(H87)</f>
+        <f t="shared" ref="J87:J103" si="8">LOG10(H87)</f>
         <v>-1.9488431345860848</v>
       </c>
     </row>
@@ -8594,19 +9791,19 @@
         <v>0.01</v>
       </c>
       <c r="G88">
+        <f t="shared" si="5"/>
+        <v>4.5000450004500049E-3</v>
+      </c>
+      <c r="H88">
         <f t="shared" si="6"/>
-        <v>4.5000450004500049E-3</v>
-      </c>
-      <c r="H88">
+        <v>1.1250112501125012E-3</v>
+      </c>
+      <c r="I88">
         <f t="shared" si="7"/>
-        <v>1.1250112501125012E-3</v>
-      </c>
-      <c r="I88">
+        <v>3.3886339693517891</v>
+      </c>
+      <c r="J88" s="2">
         <f t="shared" si="8"/>
-        <v>3.3886339693517891</v>
-      </c>
-      <c r="J88" s="2">
-        <f t="shared" si="9"/>
         <v>-2.9488431345860846</v>
       </c>
     </row>
@@ -8630,19 +9827,19 @@
         <v>1E-3</v>
       </c>
       <c r="G89">
+        <f t="shared" si="5"/>
+        <v>4.5000450004500047E-4</v>
+      </c>
+      <c r="H89">
         <f t="shared" si="6"/>
-        <v>4.5000450004500047E-4</v>
-      </c>
-      <c r="H89">
+        <v>1.1250112501125012E-4</v>
+      </c>
+      <c r="I89">
         <f t="shared" si="7"/>
-        <v>1.1250112501125012E-4</v>
-      </c>
-      <c r="I89">
+        <v>2.4885507165004443</v>
+      </c>
+      <c r="J89" s="2">
         <f t="shared" si="8"/>
-        <v>2.4885507165004443</v>
-      </c>
-      <c r="J89" s="2">
-        <f t="shared" si="9"/>
         <v>-3.9488431345860846</v>
       </c>
     </row>
@@ -8666,19 +9863,19 @@
         <v>1E-4</v>
       </c>
       <c r="G90">
+        <f t="shared" si="5"/>
+        <v>4.5000450004500049E-5</v>
+      </c>
+      <c r="H90">
         <f t="shared" si="6"/>
-        <v>4.5000450004500049E-5</v>
-      </c>
-      <c r="H90">
+        <v>1.1250112501125012E-5</v>
+      </c>
+      <c r="I90">
         <f t="shared" si="7"/>
-        <v>1.1250112501125012E-5</v>
-      </c>
-      <c r="I90">
+        <v>2.173186268412274</v>
+      </c>
+      <c r="J90" s="2">
         <f t="shared" si="8"/>
-        <v>2.173186268412274</v>
-      </c>
-      <c r="J90" s="2">
-        <f t="shared" si="9"/>
         <v>-4.9488431345860846</v>
       </c>
     </row>
@@ -8702,19 +9899,19 @@
         <v>1E-3</v>
       </c>
       <c r="G91">
+        <f t="shared" si="5"/>
+        <v>4.5000450004500047E-4</v>
+      </c>
+      <c r="H91">
         <f t="shared" si="6"/>
-        <v>4.5000450004500047E-4</v>
-      </c>
-      <c r="H91">
+        <v>1.1250112501125012E-4</v>
+      </c>
+      <c r="I91">
         <f t="shared" si="7"/>
-        <v>1.1250112501125012E-4</v>
-      </c>
-      <c r="I91">
+        <v>3.0314084642516241</v>
+      </c>
+      <c r="J91" s="2">
         <f t="shared" si="8"/>
-        <v>3.0314084642516241</v>
-      </c>
-      <c r="J91" s="2">
-        <f t="shared" si="9"/>
         <v>-3.9488431345860846</v>
       </c>
     </row>
@@ -8738,19 +9935,19 @@
         <v>0.01</v>
       </c>
       <c r="G92">
+        <f t="shared" si="5"/>
+        <v>4.5000450004500049E-3</v>
+      </c>
+      <c r="H92">
         <f t="shared" si="6"/>
-        <v>4.5000450004500049E-3</v>
-      </c>
-      <c r="H92">
+        <v>1.1250112501125012E-3</v>
+      </c>
+      <c r="I92">
         <f t="shared" si="7"/>
-        <v>1.1250112501125012E-3</v>
-      </c>
-      <c r="I92">
+        <v>3.5036545192429593</v>
+      </c>
+      <c r="J92" s="2">
         <f t="shared" si="8"/>
-        <v>3.5036545192429593</v>
-      </c>
-      <c r="J92" s="2">
-        <f t="shared" si="9"/>
         <v>-2.9488431345860846</v>
       </c>
     </row>
@@ -8774,19 +9971,19 @@
         <v>0.1</v>
       </c>
       <c r="G93">
+        <f t="shared" si="5"/>
+        <v>4.5000450004500051E-2</v>
+      </c>
+      <c r="H93">
         <f t="shared" si="6"/>
-        <v>4.5000450004500051E-2</v>
-      </c>
-      <c r="H93">
+        <v>1.1250112501125013E-2</v>
+      </c>
+      <c r="I93">
         <f t="shared" si="7"/>
-        <v>1.1250112501125013E-2</v>
-      </c>
-      <c r="I93">
+        <v>4.4039265648312682</v>
+      </c>
+      <c r="J93" s="2">
         <f t="shared" si="8"/>
-        <v>4.4039265648312682</v>
-      </c>
-      <c r="J93" s="2">
-        <f t="shared" si="9"/>
         <v>-1.9488431345860848</v>
       </c>
     </row>
@@ -8810,19 +10007,19 @@
         <v>1</v>
       </c>
       <c r="G94">
+        <f t="shared" si="5"/>
+        <v>0.45000450004500048</v>
+      </c>
+      <c r="H94">
         <f t="shared" si="6"/>
-        <v>0.45000450004500048</v>
-      </c>
-      <c r="H94">
+        <v>0.11250112501125012</v>
+      </c>
+      <c r="I94">
         <f t="shared" si="7"/>
-        <v>0.11250112501125012</v>
-      </c>
-      <c r="I94">
+        <v>5.3753508093107225</v>
+      </c>
+      <c r="J94" s="2">
         <f t="shared" si="8"/>
-        <v>5.3753508093107225</v>
-      </c>
-      <c r="J94" s="2">
-        <f t="shared" si="9"/>
         <v>-0.94884313458608482</v>
       </c>
     </row>
@@ -8846,19 +10043,19 @@
         <v>1</v>
       </c>
       <c r="G95">
+        <f t="shared" si="5"/>
+        <v>0.45000450004500048</v>
+      </c>
+      <c r="H95">
         <f t="shared" si="6"/>
-        <v>0.45000450004500048</v>
-      </c>
-      <c r="H95">
+        <v>9.0000900009000101E-2</v>
+      </c>
+      <c r="I95">
         <f t="shared" si="7"/>
-        <v>9.0000900009000101E-2</v>
-      </c>
-      <c r="I95">
+        <v>4.958549549834224</v>
+      </c>
+      <c r="J95" s="2">
         <f t="shared" si="8"/>
-        <v>4.958549549834224</v>
-      </c>
-      <c r="J95" s="2">
-        <f t="shared" si="9"/>
         <v>-1.0457531475941411</v>
       </c>
     </row>
@@ -8882,19 +10079,19 @@
         <v>0.1</v>
       </c>
       <c r="G96">
+        <f t="shared" si="5"/>
+        <v>4.5000450004500051E-2</v>
+      </c>
+      <c r="H96">
         <f t="shared" si="6"/>
-        <v>4.5000450004500051E-2</v>
-      </c>
-      <c r="H96">
+        <v>9.0000900009000098E-3</v>
+      </c>
+      <c r="I96">
         <f t="shared" si="7"/>
-        <v>9.0000900009000098E-3</v>
-      </c>
-      <c r="I96">
+        <v>4.1761491611265491</v>
+      </c>
+      <c r="J96" s="2">
         <f t="shared" si="8"/>
-        <v>4.1761491611265491</v>
-      </c>
-      <c r="J96" s="2">
-        <f t="shared" si="9"/>
         <v>-2.0457531475941413</v>
       </c>
     </row>
@@ -8918,19 +10115,19 @@
         <v>0.01</v>
       </c>
       <c r="G97">
+        <f t="shared" si="5"/>
+        <v>4.5000450004500049E-3</v>
+      </c>
+      <c r="H97">
         <f t="shared" si="6"/>
-        <v>4.5000450004500049E-3</v>
-      </c>
-      <c r="H97">
+        <v>9.0000900009000104E-4</v>
+      </c>
+      <c r="I97">
         <f t="shared" si="7"/>
-        <v>9.0000900009000104E-4</v>
-      </c>
-      <c r="I97">
+        <v>3.3839947894417328</v>
+      </c>
+      <c r="J97" s="2">
         <f t="shared" si="8"/>
-        <v>3.3839947894417328</v>
-      </c>
-      <c r="J97" s="2">
-        <f t="shared" si="9"/>
         <v>-3.0457531475941413</v>
       </c>
     </row>
@@ -8954,19 +10151,19 @@
         <v>1E-3</v>
       </c>
       <c r="G98">
+        <f t="shared" si="5"/>
+        <v>4.5000450004500047E-4</v>
+      </c>
+      <c r="H98">
         <f t="shared" si="6"/>
-        <v>4.5000450004500047E-4</v>
-      </c>
-      <c r="H98">
+        <v>9.0000900009000099E-5</v>
+      </c>
+      <c r="I98">
         <f t="shared" si="7"/>
-        <v>9.0000900009000099E-5</v>
-      </c>
-      <c r="I98">
+        <v>2.4712917110589387</v>
+      </c>
+      <c r="J98" s="2">
         <f t="shared" si="8"/>
-        <v>2.4712917110589387</v>
-      </c>
-      <c r="J98" s="2">
-        <f t="shared" si="9"/>
         <v>-4.0457531475941408</v>
       </c>
     </row>
@@ -8990,19 +10187,19 @@
         <v>1E-4</v>
       </c>
       <c r="G99">
+        <f t="shared" si="5"/>
+        <v>4.5000450004500049E-5</v>
+      </c>
+      <c r="H99">
         <f t="shared" si="6"/>
-        <v>4.5000450004500049E-5</v>
-      </c>
-      <c r="H99">
+        <v>9.0000900009000095E-6</v>
+      </c>
+      <c r="I99">
         <f t="shared" si="7"/>
-        <v>9.0000900009000095E-6</v>
-      </c>
-      <c r="I99">
+        <v>2.1702617153949575</v>
+      </c>
+      <c r="J99" s="2">
         <f t="shared" si="8"/>
-        <v>2.1702617153949575</v>
-      </c>
-      <c r="J99" s="2">
-        <f t="shared" si="9"/>
         <v>-5.0457531475941408</v>
       </c>
     </row>
@@ -9026,19 +10223,19 @@
         <v>1E-3</v>
       </c>
       <c r="G100">
+        <f t="shared" si="5"/>
+        <v>4.5000450004500047E-4</v>
+      </c>
+      <c r="H100">
         <f t="shared" si="6"/>
-        <v>4.5000450004500047E-4</v>
-      </c>
-      <c r="H100">
+        <v>9.0000900009000099E-5</v>
+      </c>
+      <c r="I100">
         <f t="shared" si="7"/>
-        <v>9.0000900009000099E-5</v>
-      </c>
-      <c r="I100">
+        <v>3.024895960107485</v>
+      </c>
+      <c r="J100" s="2">
         <f t="shared" si="8"/>
-        <v>3.024895960107485</v>
-      </c>
-      <c r="J100" s="2">
-        <f t="shared" si="9"/>
         <v>-4.0457531475941408</v>
       </c>
     </row>
@@ -9062,19 +10259,19 @@
         <v>0.01</v>
       </c>
       <c r="G101">
+        <f t="shared" si="5"/>
+        <v>4.5000450004500049E-3</v>
+      </c>
+      <c r="H101">
         <f t="shared" si="6"/>
-        <v>4.5000450004500049E-3</v>
-      </c>
-      <c r="H101">
+        <v>9.0000900009000104E-4</v>
+      </c>
+      <c r="I101">
         <f t="shared" si="7"/>
-        <v>9.0000900009000104E-4</v>
-      </c>
-      <c r="I101">
+        <v>3.4954055631461931</v>
+      </c>
+      <c r="J101" s="2">
         <f t="shared" si="8"/>
-        <v>3.4954055631461931</v>
-      </c>
-      <c r="J101" s="2">
-        <f t="shared" si="9"/>
         <v>-3.0457531475941413</v>
       </c>
     </row>
@@ -9098,19 +10295,19 @@
         <v>0.1</v>
       </c>
       <c r="G102">
+        <f t="shared" si="5"/>
+        <v>4.5000450004500051E-2</v>
+      </c>
+      <c r="H102">
         <f t="shared" si="6"/>
-        <v>4.5000450004500051E-2</v>
-      </c>
-      <c r="H102">
+        <v>9.0000900009000098E-3</v>
+      </c>
+      <c r="I102">
         <f t="shared" si="7"/>
-        <v>9.0000900009000098E-3</v>
-      </c>
-      <c r="I102">
+        <v>4.3954312402469178</v>
+      </c>
+      <c r="J102" s="2">
         <f t="shared" si="8"/>
-        <v>4.3954312402469178</v>
-      </c>
-      <c r="J102" s="2">
-        <f t="shared" si="9"/>
         <v>-2.0457531475941413</v>
       </c>
     </row>
@@ -9134,19 +10331,19 @@
         <v>1</v>
       </c>
       <c r="G103">
+        <f t="shared" si="5"/>
+        <v>0.45000450004500048</v>
+      </c>
+      <c r="H103">
         <f t="shared" si="6"/>
-        <v>0.45000450004500048</v>
-      </c>
-      <c r="H103">
+        <v>9.0000900009000101E-2</v>
+      </c>
+      <c r="I103">
         <f t="shared" si="7"/>
-        <v>9.0000900009000101E-2</v>
-      </c>
-      <c r="I103">
+        <v>5.3634201711470348</v>
+      </c>
+      <c r="J103" s="2">
         <f t="shared" si="8"/>
-        <v>5.3634201711470348</v>
-      </c>
-      <c r="J103" s="2">
-        <f t="shared" si="9"/>
         <v>-1.0457531475941411</v>
       </c>
     </row>
@@ -9209,7 +10406,7 @@
         <v>93024</v>
       </c>
       <c r="M109">
-        <f t="shared" ref="M109:M120" si="10">10^($B$123*LOG10(L109)+$B$122)</f>
+        <f t="shared" ref="M109:M120" si="9">10^($B$123*LOG10(L109)+$B$122)</f>
         <v>6.8694072413691618E-2</v>
       </c>
     </row>
@@ -9227,7 +10424,7 @@
         <v>86188</v>
       </c>
       <c r="M110">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>6.2413516819281277E-2</v>
       </c>
     </row>
@@ -9245,7 +10442,7 @@
         <v>45441</v>
       </c>
       <c r="M111">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>2.7929156677989907E-2</v>
       </c>
     </row>
@@ -9263,7 +10460,7 @@
         <v>31185</v>
       </c>
       <c r="M112">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>1.7404729442059844E-2</v>
       </c>
     </row>
@@ -9281,7 +10478,7 @@
         <v>24929</v>
       </c>
       <c r="M113">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>1.3137531319523383E-2</v>
       </c>
     </row>
@@ -9293,7 +10490,7 @@
         <v>1975</v>
       </c>
       <c r="M114">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>5.4358832056686452E-4</v>
       </c>
     </row>
@@ -9308,7 +10505,7 @@
         <v>26130</v>
       </c>
       <c r="M115">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>1.3937457137122871E-2</v>
       </c>
     </row>
@@ -9336,7 +10533,7 @@
         <v>22303</v>
       </c>
       <c r="M116">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>1.1423188046374242E-2</v>
       </c>
     </row>
@@ -9366,7 +10563,7 @@
         <v>19783</v>
       </c>
       <c r="M117">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>9.825979039056295E-3</v>
       </c>
     </row>
@@ -9390,7 +10587,7 @@
         <v>14478</v>
       </c>
       <c r="M118">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>6.6382932210282009E-3</v>
       </c>
     </row>
@@ -9414,7 +10611,7 @@
         <v>12145</v>
       </c>
       <c r="M119">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>5.3234707867863395E-3</v>
       </c>
     </row>
@@ -9426,7 +10623,7 @@
         <v>14609</v>
       </c>
       <c r="M120">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>6.7138334227200775E-3</v>
       </c>
     </row>
@@ -9574,7 +10771,7 @@
         <v>93024</v>
       </c>
       <c r="M132">
-        <f t="shared" ref="M132:M143" si="11">10^($B$146*LOG10(L132)+$B$145)</f>
+        <f t="shared" ref="M132:M143" si="10">10^($B$146*LOG10(L132)+$B$145)</f>
         <v>5.6415301020446777E-2</v>
       </c>
     </row>
@@ -9592,7 +10789,7 @@
         <v>86188</v>
       </c>
       <c r="M133">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>5.1254925559760744E-2</v>
       </c>
     </row>
@@ -9610,7 +10807,7 @@
         <v>45441</v>
       </c>
       <c r="M134">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>2.2926683046415791E-2</v>
       </c>
     </row>
@@ -9628,7 +10825,7 @@
         <v>31185</v>
       </c>
       <c r="M135">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>1.4283959522586398E-2</v>
       </c>
     </row>
@@ -9646,7 +10843,7 @@
         <v>24929</v>
       </c>
       <c r="M136">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>1.0780388040473274E-2</v>
       </c>
     </row>
@@ -9658,7 +10855,7 @@
         <v>1975</v>
       </c>
       <c r="M137">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>4.4535192393756743E-4</v>
       </c>
     </row>
@@ -9673,7 +10870,7 @@
         <v>0</v>
       </c>
       <c r="M138" t="e">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>#NUM!</v>
       </c>
     </row>
@@ -9701,7 +10898,7 @@
         <v>22303</v>
       </c>
       <c r="M139">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>9.3729818674479215E-3</v>
       </c>
     </row>
@@ -9731,7 +10928,7 @@
         <v>197830</v>
       </c>
       <c r="M140">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>0.14563070898747268</v>
       </c>
     </row>
@@ -9755,7 +10952,7 @@
         <v>14478</v>
       </c>
       <c r="M141">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>5.4453993386522825E-3</v>
       </c>
     </row>
@@ -9779,7 +10976,7 @@
         <v>100</v>
       </c>
       <c r="M142">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>1.0481169495883429E-5</v>
       </c>
     </row>
@@ -9791,7 +10988,7 @@
         <v>14609</v>
       </c>
       <c r="M143">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>5.5073960193810691E-3</v>
       </c>
     </row>
@@ -9887,6 +11084,1434 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7E102CF-57E9-CF4D-8304-DA1926A37703}">
+  <dimension ref="A1:AS48"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="K16" workbookViewId="0">
+      <selection activeCell="R4" sqref="R4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="11" max="11" width="23.6640625" customWidth="1"/>
+    <col min="16" max="16" width="11.5" customWidth="1"/>
+    <col min="17" max="17" width="11" customWidth="1"/>
+    <col min="20" max="20" width="4.5" customWidth="1"/>
+    <col min="21" max="21" width="32.5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.5" customWidth="1"/>
+    <col min="23" max="23" width="15.6640625" customWidth="1"/>
+    <col min="24" max="24" width="2.33203125" customWidth="1"/>
+    <col min="25" max="25" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="1.1640625" customWidth="1"/>
+    <col min="35" max="35" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="26.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="R14" s="49" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q15" s="48" t="s">
+        <v>118</v>
+      </c>
+      <c r="R15" s="48" t="s">
+        <v>277</v>
+      </c>
+      <c r="T15" s="50" t="s">
+        <v>279</v>
+      </c>
+      <c r="U15" s="50"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>118</v>
+      </c>
+      <c r="B16" t="s">
+        <v>119</v>
+      </c>
+      <c r="C16" t="s">
+        <v>120</v>
+      </c>
+      <c r="D16" t="s">
+        <v>121</v>
+      </c>
+      <c r="E16" t="s">
+        <v>122</v>
+      </c>
+      <c r="F16" t="s">
+        <v>123</v>
+      </c>
+      <c r="G16" t="s">
+        <v>124</v>
+      </c>
+      <c r="H16" t="s">
+        <v>125</v>
+      </c>
+      <c r="I16" t="s">
+        <v>235</v>
+      </c>
+      <c r="J16" t="s">
+        <v>152</v>
+      </c>
+      <c r="Q16" s="48" t="s">
+        <v>107</v>
+      </c>
+      <c r="R16" s="48">
+        <v>93135</v>
+      </c>
+      <c r="T16" s="50"/>
+      <c r="U16" s="50" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>107</v>
+      </c>
+      <c r="B17" t="s">
+        <v>108</v>
+      </c>
+      <c r="C17">
+        <v>93135</v>
+      </c>
+      <c r="D17">
+        <v>3216923</v>
+      </c>
+      <c r="E17">
+        <v>0.25</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <f>F17/(2*(1+0.1+0.01+0.001+0.0001))</f>
+        <v>0.45000450004500048</v>
+      </c>
+      <c r="H17">
+        <f>E17*G17</f>
+        <v>0.11250112501125012</v>
+      </c>
+      <c r="I17">
+        <f>LOG10(C17)</f>
+        <v>4.9691129189016641</v>
+      </c>
+      <c r="J17" s="2">
+        <f>LOG10(H17)</f>
+        <v>-0.94884313458608482</v>
+      </c>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="Q17" s="48" t="s">
+        <v>109</v>
+      </c>
+      <c r="R17" s="48">
+        <v>15190</v>
+      </c>
+      <c r="T17" s="50"/>
+      <c r="U17" s="50" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>109</v>
+      </c>
+      <c r="B18" t="s">
+        <v>108</v>
+      </c>
+      <c r="C18">
+        <v>15190</v>
+      </c>
+      <c r="D18">
+        <v>3216923</v>
+      </c>
+      <c r="E18">
+        <v>0.25</v>
+      </c>
+      <c r="F18">
+        <v>0.1</v>
+      </c>
+      <c r="G18">
+        <f t="shared" ref="G18:G26" si="0">F18/(2*(1+0.1+0.01+0.001+0.0001))</f>
+        <v>4.5000450004500051E-2</v>
+      </c>
+      <c r="H18">
+        <f t="shared" ref="H18:H26" si="1">E18*G18</f>
+        <v>1.1250112501125013E-2</v>
+      </c>
+      <c r="I18">
+        <f t="shared" ref="I18:I26" si="2">LOG10(C18)</f>
+        <v>4.181557773862786</v>
+      </c>
+      <c r="J18" s="2">
+        <f t="shared" ref="J18:J26" si="3">LOG10(H18)</f>
+        <v>-1.9488431345860848</v>
+      </c>
+      <c r="Q18" s="48" t="s">
+        <v>110</v>
+      </c>
+      <c r="R18" s="48">
+        <v>2447</v>
+      </c>
+      <c r="T18" s="50"/>
+      <c r="U18" s="50" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>110</v>
+      </c>
+      <c r="B19" t="s">
+        <v>108</v>
+      </c>
+      <c r="C19">
+        <v>2447</v>
+      </c>
+      <c r="D19">
+        <v>3216923</v>
+      </c>
+      <c r="E19">
+        <v>0.25</v>
+      </c>
+      <c r="F19">
+        <v>0.01</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="0"/>
+        <v>4.5000450004500049E-3</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="1"/>
+        <v>1.1250112501125012E-3</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="2"/>
+        <v>3.3886339693517891</v>
+      </c>
+      <c r="J19" s="2">
+        <f t="shared" si="3"/>
+        <v>-2.9488431345860846</v>
+      </c>
+      <c r="Q19" s="48" t="s">
+        <v>111</v>
+      </c>
+      <c r="R19" s="48">
+        <v>308</v>
+      </c>
+      <c r="T19" s="50"/>
+      <c r="U19" s="50" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>111</v>
+      </c>
+      <c r="B20" t="s">
+        <v>108</v>
+      </c>
+      <c r="C20">
+        <v>308</v>
+      </c>
+      <c r="D20">
+        <v>3216923</v>
+      </c>
+      <c r="E20">
+        <v>0.25</v>
+      </c>
+      <c r="F20">
+        <v>1E-3</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="0"/>
+        <v>4.5000450004500047E-4</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="1"/>
+        <v>1.1250112501125012E-4</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="2"/>
+        <v>2.4885507165004443</v>
+      </c>
+      <c r="J20" s="2">
+        <f t="shared" si="3"/>
+        <v>-3.9488431345860846</v>
+      </c>
+      <c r="Q20" s="48" t="s">
+        <v>153</v>
+      </c>
+      <c r="R20" s="48">
+        <v>77</v>
+      </c>
+      <c r="T20" s="50"/>
+      <c r="U20" s="50" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>153</v>
+      </c>
+      <c r="B21" t="s">
+        <v>108</v>
+      </c>
+      <c r="C21">
+        <v>77</v>
+      </c>
+      <c r="D21">
+        <v>3216923</v>
+      </c>
+      <c r="E21">
+        <v>0.25</v>
+      </c>
+      <c r="F21">
+        <v>1E-4</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="0"/>
+        <v>4.5000450004500049E-5</v>
+      </c>
+      <c r="H21">
+        <f>E21*G21</f>
+        <v>1.1250112501125012E-5</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="2"/>
+        <v>1.8864907251724818</v>
+      </c>
+      <c r="J21" s="2">
+        <f>LOG10(H21)</f>
+        <v>-4.9488431345860846</v>
+      </c>
+      <c r="Q21" s="48" t="s">
+        <v>112</v>
+      </c>
+      <c r="R21" s="48">
+        <v>149</v>
+      </c>
+      <c r="T21" s="50"/>
+      <c r="U21" s="50" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>112</v>
+      </c>
+      <c r="B22" t="s">
+        <v>108</v>
+      </c>
+      <c r="C22">
+        <v>149</v>
+      </c>
+      <c r="D22">
+        <v>3216923</v>
+      </c>
+      <c r="E22">
+        <v>0.25</v>
+      </c>
+      <c r="F22">
+        <v>1E-4</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="0"/>
+        <v>4.5000450004500049E-5</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="1"/>
+        <v>1.1250112501125012E-5</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="2"/>
+        <v>2.173186268412274</v>
+      </c>
+      <c r="J22" s="2">
+        <f t="shared" si="3"/>
+        <v>-4.9488431345860846</v>
+      </c>
+      <c r="Q22" s="48" t="s">
+        <v>113</v>
+      </c>
+      <c r="R22" s="48">
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>113</v>
+      </c>
+      <c r="B23" t="s">
+        <v>108</v>
+      </c>
+      <c r="C23">
+        <v>1075</v>
+      </c>
+      <c r="D23">
+        <v>3216923</v>
+      </c>
+      <c r="E23">
+        <v>0.25</v>
+      </c>
+      <c r="F23">
+        <v>1E-3</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="0"/>
+        <v>4.5000450004500047E-4</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="1"/>
+        <v>1.1250112501125012E-4</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="2"/>
+        <v>3.0314084642516241</v>
+      </c>
+      <c r="J23" s="2">
+        <f t="shared" si="3"/>
+        <v>-3.9488431345860846</v>
+      </c>
+      <c r="Q23" s="48" t="s">
+        <v>114</v>
+      </c>
+      <c r="R23" s="48">
+        <v>3189</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>114</v>
+      </c>
+      <c r="B24" t="s">
+        <v>108</v>
+      </c>
+      <c r="C24">
+        <v>3189</v>
+      </c>
+      <c r="D24">
+        <v>3216923</v>
+      </c>
+      <c r="E24">
+        <v>0.25</v>
+      </c>
+      <c r="F24">
+        <v>0.01</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="0"/>
+        <v>4.5000450004500049E-3</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="1"/>
+        <v>1.1250112501125012E-3</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="2"/>
+        <v>3.5036545192429593</v>
+      </c>
+      <c r="J24" s="2">
+        <f t="shared" si="3"/>
+        <v>-2.9488431345860846</v>
+      </c>
+      <c r="Q24" s="48" t="s">
+        <v>115</v>
+      </c>
+      <c r="R24" s="48">
+        <v>25347</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>115</v>
+      </c>
+      <c r="B25" t="s">
+        <v>108</v>
+      </c>
+      <c r="C25">
+        <v>25347</v>
+      </c>
+      <c r="D25">
+        <v>3216923</v>
+      </c>
+      <c r="E25">
+        <v>0.25</v>
+      </c>
+      <c r="F25">
+        <v>0.1</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="0"/>
+        <v>4.5000450004500051E-2</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="1"/>
+        <v>1.1250112501125013E-2</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="2"/>
+        <v>4.4039265648312682</v>
+      </c>
+      <c r="J25" s="2">
+        <f t="shared" si="3"/>
+        <v>-1.9488431345860848</v>
+      </c>
+      <c r="Q25" s="48" t="s">
+        <v>116</v>
+      </c>
+      <c r="R25" s="48">
+        <v>237329</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>116</v>
+      </c>
+      <c r="B26" t="s">
+        <v>108</v>
+      </c>
+      <c r="C26">
+        <v>237329</v>
+      </c>
+      <c r="D26">
+        <v>3216923</v>
+      </c>
+      <c r="E26">
+        <v>0.25</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="0"/>
+        <v>0.45000450004500048</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="1"/>
+        <v>0.11250112501125012</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="2"/>
+        <v>5.3753508093107225</v>
+      </c>
+      <c r="J26" s="2">
+        <f t="shared" si="3"/>
+        <v>-0.94884313458608482</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>238</v>
+      </c>
+      <c r="K29" t="s">
+        <v>246</v>
+      </c>
+      <c r="V29" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>126</v>
+      </c>
+      <c r="J30" t="s">
+        <v>288</v>
+      </c>
+      <c r="K30" t="s">
+        <v>248</v>
+      </c>
+      <c r="P30" s="48"/>
+      <c r="Q30" s="48" t="s">
+        <v>278</v>
+      </c>
+      <c r="V30" s="48" t="s">
+        <v>294</v>
+      </c>
+      <c r="W30" s="48" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J31" t="s">
+        <v>286</v>
+      </c>
+      <c r="K31" t="str" cm="1">
+        <f t="array" ref="K31:K44">syndna_saliva_analysis_ex1!D7:D20</f>
+        <v>Species</v>
+      </c>
+      <c r="L31" t="str" cm="1">
+        <f t="array" ref="L31:L44">syndna_saliva_analysis_ex1!E7:E20</f>
+        <v>RawCounts</v>
+      </c>
+      <c r="M31" t="s">
+        <v>247</v>
+      </c>
+      <c r="P31" s="48" t="s">
+        <v>294</v>
+      </c>
+      <c r="Q31" s="48" t="s">
+        <v>277</v>
+      </c>
+      <c r="V31" s="48" t="s">
+        <v>287</v>
+      </c>
+      <c r="W31" s="48">
+        <v>10.29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A32" s="32" t="s">
+        <v>127</v>
+      </c>
+      <c r="B32" s="32"/>
+      <c r="J32" t="s">
+        <v>287</v>
+      </c>
+      <c r="K32" t="str">
+        <v>Lactobacillus gasseri</v>
+      </c>
+      <c r="L32">
+        <v>79950</v>
+      </c>
+      <c r="M32">
+        <f>10^($B$47*LOG10(L32)+$B$46)</f>
+        <v>5.5906776314467152E-2</v>
+      </c>
+      <c r="P32" s="48" t="s">
+        <v>287</v>
+      </c>
+      <c r="Q32" s="48">
+        <v>79950</v>
+      </c>
+      <c r="V32" s="48" t="s">
+        <v>289</v>
+      </c>
+      <c r="W32" s="48">
+        <v>1.19</v>
+      </c>
+    </row>
+    <row r="33" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>128</v>
+      </c>
+      <c r="B33">
+        <v>0.98650309751565701</v>
+      </c>
+      <c r="J33" t="s">
+        <v>289</v>
+      </c>
+      <c r="K33" t="str">
+        <v>Ruminococcus albus</v>
+      </c>
+      <c r="L33">
+        <v>93024</v>
+      </c>
+      <c r="M33">
+        <f>10^($B$47*LOG10(L33)+$B$46)</f>
+        <v>6.7506893569518861E-2</v>
+      </c>
+      <c r="P33" s="48" t="s">
+        <v>289</v>
+      </c>
+      <c r="Q33" s="48">
+        <v>93024</v>
+      </c>
+      <c r="V33" s="48" t="s">
+        <v>290</v>
+      </c>
+      <c r="W33" s="48">
+        <v>7.24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>129</v>
+      </c>
+      <c r="B34">
+        <v>0.97318836140798681</v>
+      </c>
+      <c r="J34" t="s">
+        <v>290</v>
+      </c>
+      <c r="K34" t="str">
+        <v>Escherichia coli</v>
+      </c>
+      <c r="L34">
+        <v>86188</v>
+      </c>
+      <c r="M34">
+        <f>10^($B$47*LOG10(L34)+$B$46)</f>
+        <v>6.1387888964041307E-2</v>
+      </c>
+      <c r="P34" s="48" t="s">
+        <v>290</v>
+      </c>
+      <c r="Q34" s="48">
+        <v>86188</v>
+      </c>
+      <c r="V34" s="48" t="s">
+        <v>291</v>
+      </c>
+      <c r="W34" s="48">
+        <v>92.65</v>
+      </c>
+    </row>
+    <row r="35" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>130</v>
+      </c>
+      <c r="B35">
+        <v>0.96983690658398514</v>
+      </c>
+      <c r="K35" t="str">
+        <v>Tyzzerella nexilis</v>
+      </c>
+      <c r="L35">
+        <v>45441</v>
+      </c>
+      <c r="M35">
+        <f>10^($B$47*LOG10(L35)+$B$46)</f>
+        <v>2.7669949480603664E-2</v>
+      </c>
+      <c r="P35" s="48" t="s">
+        <v>291</v>
+      </c>
+      <c r="Q35" s="48">
+        <v>31185</v>
+      </c>
+      <c r="V35" s="48" t="s">
+        <v>292</v>
+      </c>
+      <c r="W35" s="48">
+        <v>3.58</v>
+      </c>
+    </row>
+    <row r="36" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>131</v>
+      </c>
+      <c r="B36">
+        <v>0.25889978076474535</v>
+      </c>
+      <c r="J36" t="s">
+        <v>291</v>
+      </c>
+      <c r="K36" t="str">
+        <v>Prevotella sp. oral taxon 299</v>
+      </c>
+      <c r="L36">
+        <v>31185</v>
+      </c>
+      <c r="M36">
+        <f>10^($B$47*LOG10(L36)+$B$46)</f>
+        <v>1.731683029216274E-2</v>
+      </c>
+      <c r="P36" s="48" t="s">
+        <v>292</v>
+      </c>
+      <c r="Q36" s="48">
+        <v>24929</v>
+      </c>
+      <c r="V36" s="48" t="s">
+        <v>293</v>
+      </c>
+      <c r="W36" s="48">
+        <v>4.24</v>
+      </c>
+    </row>
+    <row r="37" spans="1:45" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="30" t="s">
+        <v>132</v>
+      </c>
+      <c r="B37" s="30">
+        <v>10</v>
+      </c>
+      <c r="J37" t="s">
+        <v>292</v>
+      </c>
+      <c r="K37" t="str">
+        <v>Streptococcus mitis</v>
+      </c>
+      <c r="L37">
+        <v>24929</v>
+      </c>
+      <c r="M37">
+        <f>10^($B$47*LOG10(L37)+$B$46)</f>
+        <v>1.3104350443761088E-2</v>
+      </c>
+      <c r="P37" s="48" t="s">
+        <v>293</v>
+      </c>
+      <c r="Q37" s="48">
+        <v>1975</v>
+      </c>
+      <c r="V37" s="48" t="s">
+        <v>295</v>
+      </c>
+      <c r="W37" s="48">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="38" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="J38" t="s">
+        <v>293</v>
+      </c>
+      <c r="K38" t="str">
+        <v>Leptolyngbya valderiana</v>
+      </c>
+      <c r="L38">
+        <v>1975</v>
+      </c>
+      <c r="M38">
+        <f>10^($B$47*LOG10(L38)+$B$46)</f>
+        <v>5.5800097113146443E-4</v>
+      </c>
+      <c r="P38" s="48" t="s">
+        <v>295</v>
+      </c>
+      <c r="Q38" s="48">
+        <v>44001</v>
+      </c>
+      <c r="R38" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="39" spans="1:45" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>133</v>
+      </c>
+      <c r="K39" t="str">
+        <v>Neisseria subflava</v>
+      </c>
+      <c r="L39">
+        <v>26130</v>
+      </c>
+      <c r="M39">
+        <f>10^($B$47*LOG10(L39)+$B$46)</f>
+        <v>1.3894854164478233E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="A40" s="31"/>
+      <c r="B40" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="C40" s="31" t="s">
+        <v>139</v>
+      </c>
+      <c r="D40" s="31" t="s">
+        <v>140</v>
+      </c>
+      <c r="E40" s="31" t="s">
+        <v>141</v>
+      </c>
+      <c r="F40" s="31" t="s">
+        <v>142</v>
+      </c>
+      <c r="K40" t="str">
+        <v>Neisseria flavescens</v>
+      </c>
+      <c r="L40">
+        <v>22303</v>
+      </c>
+      <c r="M40">
+        <f>10^($B$47*LOG10(L40)+$B$46)</f>
+        <v>1.1408701284690223E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>134</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41">
+        <v>19.463767228159732</v>
+      </c>
+      <c r="D41">
+        <v>19.463767228159732</v>
+      </c>
+      <c r="E41">
+        <v>290.37788438574057</v>
+      </c>
+      <c r="F41">
+        <v>1.4284435606597672E-7</v>
+      </c>
+      <c r="K41" t="str">
+        <v>Fusobacterium periodonticum</v>
+      </c>
+      <c r="L41">
+        <v>19783</v>
+      </c>
+      <c r="M41">
+        <f>10^($B$47*LOG10(L41)+$B$46)</f>
+        <v>9.8268443584452556E-3</v>
+      </c>
+      <c r="P41" s="48"/>
+      <c r="Q41" s="48" t="s">
+        <v>278</v>
+      </c>
+      <c r="V41" s="51"/>
+      <c r="W41" s="51"/>
+      <c r="AI41" s="48"/>
+      <c r="AJ41" s="48" t="s">
+        <v>278</v>
+      </c>
+      <c r="AL41" s="48"/>
+      <c r="AM41" s="48" t="s">
+        <v>278</v>
+      </c>
+      <c r="AO41" s="48"/>
+      <c r="AP41" s="48" t="s">
+        <v>278</v>
+      </c>
+      <c r="AR41" s="48"/>
+      <c r="AS41" s="48" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="42" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>135</v>
+      </c>
+      <c r="B42">
+        <v>8</v>
+      </c>
+      <c r="C42">
+        <v>0.53623277184026563</v>
+      </c>
+      <c r="D42">
+        <v>6.7029096480033204E-2</v>
+      </c>
+      <c r="K42" t="str">
+        <v>Streptococcus pneumoniae</v>
+      </c>
+      <c r="L42">
+        <v>14478</v>
+      </c>
+      <c r="M42">
+        <f>10^($B$47*LOG10(L42)+$B$46)</f>
+        <v>6.6623779084662204E-3</v>
+      </c>
+      <c r="P42" s="48" t="s">
+        <v>294</v>
+      </c>
+      <c r="Q42" s="48" t="s">
+        <v>299</v>
+      </c>
+      <c r="Y42" s="48" t="s">
+        <v>294</v>
+      </c>
+      <c r="Z42" s="48" t="s">
+        <v>300</v>
+      </c>
+      <c r="AI42" s="48" t="s">
+        <v>294</v>
+      </c>
+      <c r="AJ42" s="48" t="s">
+        <v>305</v>
+      </c>
+      <c r="AL42" s="48" t="s">
+        <v>294</v>
+      </c>
+      <c r="AM42" s="48" t="s">
+        <v>306</v>
+      </c>
+      <c r="AO42" s="48" t="s">
+        <v>294</v>
+      </c>
+      <c r="AP42" s="48" t="s">
+        <v>307</v>
+      </c>
+      <c r="AR42" s="48" t="s">
+        <v>294</v>
+      </c>
+      <c r="AS42" s="48" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="43" spans="1:45" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="30" t="s">
+        <v>136</v>
+      </c>
+      <c r="B43" s="30">
+        <v>9</v>
+      </c>
+      <c r="C43" s="30">
+        <v>19.999999999999996</v>
+      </c>
+      <c r="D43" s="30"/>
+      <c r="E43" s="30"/>
+      <c r="F43" s="30"/>
+      <c r="K43" t="str">
+        <v>Haemophilus influenzae</v>
+      </c>
+      <c r="L43">
+        <v>12145</v>
+      </c>
+      <c r="M43">
+        <f>10^($B$47*LOG10(L43)+$B$46)</f>
+        <v>5.3534213285283943E-3</v>
+      </c>
+      <c r="P43" s="48" t="s">
+        <v>287</v>
+      </c>
+      <c r="Q43" s="48">
+        <f>M32</f>
+        <v>5.5906776314467152E-2</v>
+      </c>
+      <c r="Y43" s="48" t="s">
+        <v>287</v>
+      </c>
+      <c r="Z43" s="52">
+        <f>'full_calcs on correct masses '!G78</f>
+        <v>1904788.3330000001</v>
+      </c>
+      <c r="AB43" t="s">
+        <v>301</v>
+      </c>
+      <c r="AI43" s="48" t="s">
+        <v>287</v>
+      </c>
+      <c r="AJ43" s="52">
+        <f>'full_calcs on correct masses '!G79</f>
+        <v>27192.884259161423</v>
+      </c>
+      <c r="AL43" s="48" t="s">
+        <v>287</v>
+      </c>
+      <c r="AM43" s="54">
+        <f>'full_calcs on correct masses '!G81</f>
+        <v>5438576851832.2852</v>
+      </c>
+      <c r="AO43" s="48" t="s">
+        <v>287</v>
+      </c>
+      <c r="AP43" s="52">
+        <f>'full_calcs on correct masses '!$G$82</f>
+        <v>39085654.849706717</v>
+      </c>
+      <c r="AR43" s="48" t="s">
+        <v>287</v>
+      </c>
+      <c r="AS43" s="52">
+        <f>'full_calcs on correct masses '!$G$82</f>
+        <v>39085654.849706717</v>
+      </c>
+    </row>
+    <row r="44" spans="1:45" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K44" t="str">
+        <v>Veillonella dispar</v>
+      </c>
+      <c r="L44">
+        <v>14609</v>
+      </c>
+      <c r="M44">
+        <f>10^($B$47*LOG10(L44)+$B$46)</f>
+        <v>6.7375052531226162E-3</v>
+      </c>
+      <c r="P44" s="48" t="s">
+        <v>289</v>
+      </c>
+      <c r="Q44" s="48">
+        <f>M33</f>
+        <v>6.7506893569518861E-2</v>
+      </c>
+      <c r="Y44" s="48" t="s">
+        <v>289</v>
+      </c>
+      <c r="Z44" s="52">
+        <f>'full_calcs on correct masses '!G88</f>
+        <v>4373730</v>
+      </c>
+      <c r="AB44" t="s">
+        <v>302</v>
+      </c>
+      <c r="AI44" s="48" t="s">
+        <v>289</v>
+      </c>
+      <c r="AJ44" s="52">
+        <f>'full_calcs on correct masses '!G89</f>
+        <v>14299.923031581789</v>
+      </c>
+      <c r="AL44" s="48" t="s">
+        <v>289</v>
+      </c>
+      <c r="AM44" s="54">
+        <f>'full_calcs on correct masses '!G91</f>
+        <v>2859984606316.3579</v>
+      </c>
+      <c r="AO44" s="48" t="s">
+        <v>289</v>
+      </c>
+      <c r="AP44" s="52">
+        <f>'full_calcs on correct masses '!$G$92</f>
+        <v>20553974.733352304</v>
+      </c>
+      <c r="AR44" s="48" t="s">
+        <v>289</v>
+      </c>
+      <c r="AS44" s="52">
+        <f>'full_calcs on correct masses '!$G$92</f>
+        <v>20553974.733352304</v>
+      </c>
+    </row>
+    <row r="45" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="A45" s="31"/>
+      <c r="B45" s="31" t="s">
+        <v>143</v>
+      </c>
+      <c r="C45" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="D45" s="31" t="s">
+        <v>144</v>
+      </c>
+      <c r="E45" s="31" t="s">
+        <v>145</v>
+      </c>
+      <c r="F45" s="31" t="s">
+        <v>146</v>
+      </c>
+      <c r="G45" s="31" t="s">
+        <v>147</v>
+      </c>
+      <c r="H45" s="31" t="s">
+        <v>148</v>
+      </c>
+      <c r="I45" s="31" t="s">
+        <v>149</v>
+      </c>
+      <c r="P45" s="48" t="s">
+        <v>290</v>
+      </c>
+      <c r="Q45" s="48">
+        <f>M34</f>
+        <v>6.1387888964041307E-2</v>
+      </c>
+      <c r="Y45" s="48" t="s">
+        <v>290</v>
+      </c>
+      <c r="Z45" s="52">
+        <v>3489300</v>
+      </c>
+      <c r="AB45" t="s">
+        <v>304</v>
+      </c>
+      <c r="AI45" s="48" t="s">
+        <v>290</v>
+      </c>
+      <c r="AJ45" s="52">
+        <f>(Q45*6.02214076E+23)/(Z45*650*1000000000)</f>
+        <v>16299.787186793354</v>
+      </c>
+      <c r="AL45" s="48" t="s">
+        <v>290</v>
+      </c>
+      <c r="AM45" s="54">
+        <f>AJ45* 1000000000/5</f>
+        <v>3259957437358.6709</v>
+      </c>
+      <c r="AO45" s="48" t="s">
+        <v>290</v>
+      </c>
+      <c r="AP45" s="52">
+        <f>$AM$45*'full_calcs on correct masses '!$G$29</f>
+        <v>23428476.730710857</v>
+      </c>
+      <c r="AR45" s="48" t="s">
+        <v>290</v>
+      </c>
+      <c r="AS45" s="52">
+        <f>$AM$45*'full_calcs on correct masses '!$G$29</f>
+        <v>23428476.730710857</v>
+      </c>
+    </row>
+    <row r="46" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>137</v>
+      </c>
+      <c r="B46">
+        <v>-7.3559391605484281</v>
+      </c>
+      <c r="C46">
+        <v>0.27127453736340101</v>
+      </c>
+      <c r="D46">
+        <v>-27.116216774500909</v>
+      </c>
+      <c r="E46">
+        <v>3.6852336719780197E-9</v>
+      </c>
+      <c r="F46">
+        <v>-7.9814993654840283</v>
+      </c>
+      <c r="G46">
+        <v>-6.730378955612828</v>
+      </c>
+      <c r="H46">
+        <v>-7.9814993654840283</v>
+      </c>
+      <c r="I46">
+        <v>-6.730378955612828</v>
+      </c>
+      <c r="P46" s="48" t="s">
+        <v>291</v>
+      </c>
+      <c r="Q46" s="48">
+        <f>M36</f>
+        <v>1.731683029216274E-2</v>
+      </c>
+      <c r="Y46" s="48" t="s">
+        <v>291</v>
+      </c>
+      <c r="Z46" s="52">
+        <v>9202483</v>
+      </c>
+      <c r="AB46" t="s">
+        <v>304</v>
+      </c>
+      <c r="AI46" s="48" t="s">
+        <v>291</v>
+      </c>
+      <c r="AJ46" s="52">
+        <f>(Q46*6.02214076E+23)/(Z46*650*1000000000)</f>
+        <v>1743.4155799445389</v>
+      </c>
+      <c r="AL46" s="48" t="s">
+        <v>291</v>
+      </c>
+      <c r="AM46" s="54">
+        <f>AJ46* 1000000000/5</f>
+        <v>348683115988.90778</v>
+      </c>
+      <c r="AO46" s="48" t="s">
+        <v>291</v>
+      </c>
+      <c r="AP46" s="52">
+        <f>$AM$46*'full_calcs on correct masses '!$G$29</f>
+        <v>2505895.9898435902</v>
+      </c>
+      <c r="AR46" s="48" t="s">
+        <v>291</v>
+      </c>
+      <c r="AS46" s="52">
+        <f>$AM$46*'full_calcs on correct masses '!$G$29</f>
+        <v>2505895.9898435902</v>
+      </c>
+    </row>
+    <row r="47" spans="1:45" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="30" t="s">
+        <v>166</v>
+      </c>
+      <c r="B47" s="30">
+        <v>1.24487652379132</v>
+      </c>
+      <c r="C47" s="30">
+        <v>7.30540855033502E-2</v>
+      </c>
+      <c r="D47" s="30">
+        <v>17.040477821520749</v>
+      </c>
+      <c r="E47" s="44">
+        <v>1.4284435606597701E-7</v>
+      </c>
+      <c r="F47" s="30">
+        <v>1.0764135005270346</v>
+      </c>
+      <c r="G47" s="30">
+        <v>1.4133395470556032</v>
+      </c>
+      <c r="H47" s="30">
+        <v>1.0764135005270346</v>
+      </c>
+      <c r="I47" s="30">
+        <v>1.4133395470556032</v>
+      </c>
+      <c r="P47" s="48" t="s">
+        <v>292</v>
+      </c>
+      <c r="Q47" s="48">
+        <f>M37</f>
+        <v>1.3104350443761088E-2</v>
+      </c>
+      <c r="Y47" s="48" t="s">
+        <v>292</v>
+      </c>
+      <c r="Z47" s="52">
+        <v>10348543</v>
+      </c>
+      <c r="AB47" t="s">
+        <v>304</v>
+      </c>
+      <c r="AI47" s="48" t="s">
+        <v>292</v>
+      </c>
+      <c r="AJ47" s="52">
+        <f>(Q47*6.02214076E+23)/(Z47*650*1000000000)</f>
+        <v>1173.2048127369269</v>
+      </c>
+      <c r="AL47" s="48" t="s">
+        <v>292</v>
+      </c>
+      <c r="AM47" s="54">
+        <f>AJ47* 1000000000/5</f>
+        <v>234640962547.38541</v>
+      </c>
+      <c r="AO47" s="48" t="s">
+        <v>292</v>
+      </c>
+      <c r="AP47" s="52">
+        <f>$AM$47*'full_calcs on correct masses '!$G$29</f>
+        <v>1686304.3265887243</v>
+      </c>
+      <c r="AR47" s="48" t="s">
+        <v>292</v>
+      </c>
+      <c r="AS47" s="52">
+        <f>$AM$47*'full_calcs on correct masses '!$G$29</f>
+        <v>1686304.3265887243</v>
+      </c>
+    </row>
+    <row r="48" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="P48" s="48" t="s">
+        <v>293</v>
+      </c>
+      <c r="Q48" s="48">
+        <f>M38</f>
+        <v>5.5800097113146443E-4</v>
+      </c>
+      <c r="Y48" s="48" t="s">
+        <v>293</v>
+      </c>
+      <c r="Z48" s="53">
+        <f>'full_calcs on correct masses '!G98</f>
+        <v>89264</v>
+      </c>
+      <c r="AB48" t="s">
+        <v>303</v>
+      </c>
+      <c r="AI48" s="48" t="s">
+        <v>293</v>
+      </c>
+      <c r="AJ48" s="52">
+        <f>'full_calcs on correct masses '!G99</f>
+        <v>5791.5679546416768</v>
+      </c>
+      <c r="AL48" s="48" t="s">
+        <v>293</v>
+      </c>
+      <c r="AM48" s="54">
+        <f>'full_calcs on correct masses '!G101</f>
+        <v>1158313590928.3352</v>
+      </c>
+      <c r="AO48" s="48" t="s">
+        <v>293</v>
+      </c>
+      <c r="AP48" s="52">
+        <f>'full_calcs on correct masses '!$G$102</f>
+        <v>8324502.2468509236</v>
+      </c>
+      <c r="AR48" s="48" t="s">
+        <v>293</v>
+      </c>
+      <c r="AS48" s="52">
+        <f>'full_calcs on correct masses '!$G$102</f>
+        <v>8324502.2468509236</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF78FB9F-0C2A-0F43-B368-C0466A3B1D76}">
   <dimension ref="A1:M85"/>
   <sheetViews>
@@ -12566,11 +15191,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85A661CB-FE77-E747-9C39-6C6F06A92839}">
   <dimension ref="A1:M142"/>
   <sheetViews>
-    <sheetView topLeftCell="A149" workbookViewId="0">
+    <sheetView topLeftCell="A132" workbookViewId="0">
       <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
@@ -15109,11 +17734,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66BE62EB-1EB8-3046-8607-7A251B8CA1A4}">
   <dimension ref="A1:V68"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B63" sqref="A48:B63"/>
     </sheetView>
   </sheetViews>
@@ -16624,7 +19249,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C02A8AC-889E-CA4E-873C-2DEEB4CB6BC7}">
   <dimension ref="A1:P20"/>
   <sheetViews>

</xml_diff>

<commit_message>
extend example spreadsheet, correct typo in internal column name
</commit_message>
<xml_diff>
--- a/docs/absolute_quant_example.xlsx
+++ b/docs/absolute_quant_example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abirmingham/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abirmingham/Work/Repositories/pysyndna/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:2001_{B806CE7F-E384-A04D-B7E0-583EA7BFBFCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D69F5D4F-9A53-6042-AC4B-4C31DFF9C38E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="940" windowWidth="26580" windowHeight="15160" firstSheet="1" activeTab="2" xr2:uid="{E184B90C-6432-8947-B7A0-BE1974B73180}"/>
+    <workbookView xWindow="1440" yWindow="920" windowWidth="31820" windowHeight="19160" activeTab="2" xr2:uid="{E184B90C-6432-8947-B7A0-BE1974B73180}"/>
   </bookViews>
   <sheets>
     <sheet name="full_calcs on correct masses " sheetId="16" r:id="rId1"/>
@@ -22,7 +22,6 @@
     <sheet name="syndna_saliva_analysis_ex1" sheetId="14" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2117,7 +2116,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -2139,7 +2138,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1593" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1642" uniqueCount="311">
   <si>
     <t>variable name</t>
   </si>
@@ -3066,6 +3065,12 @@
   </si>
   <si>
     <t>num_cells_per_g_sample</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>* below tables are same as above except that values with asterisk are taken directly from "full calcs on correct masses" worksheet rather than calculated on this sheet. Note the match to values calculated here.</t>
   </si>
 </sst>
 </file>
@@ -3079,7 +3084,7 @@
     <numFmt numFmtId="167" formatCode="0.0000000000E+00"/>
     <numFmt numFmtId="168" formatCode="0.000000000000000E+00"/>
     <numFmt numFmtId="169" formatCode="0.0"/>
-    <numFmt numFmtId="171" formatCode="0.000000E+00"/>
+    <numFmt numFmtId="170" formatCode="0.000000E+00"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -3183,7 +3188,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -3306,12 +3311,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3369,10 +3385,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4789,8 +4806,8 @@
   <dimension ref="A1:M106"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G46" sqref="G46"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8095,7 +8112,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFC0DD12-9F50-4C4C-88FA-79E5E161A3E2}">
   <dimension ref="A1:M146"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A39" workbookViewId="0">
       <selection activeCell="J40" sqref="J40:J48"/>
     </sheetView>
   </sheetViews>
@@ -8974,7 +8991,7 @@
         <v>79950</v>
       </c>
       <c r="M42">
-        <f>10^($B$57*LOG10(L42)+$B$56)</f>
+        <f t="shared" ref="M42:M54" si="4">10^($B$57*LOG10(L42)+$B$56)</f>
         <v>5.5906776314467152E-2</v>
       </c>
     </row>
@@ -8992,7 +9009,7 @@
         <v>93024</v>
       </c>
       <c r="M43">
-        <f>10^($B$57*LOG10(L43)+$B$56)</f>
+        <f t="shared" si="4"/>
         <v>6.7506893569518861E-2</v>
       </c>
     </row>
@@ -9010,7 +9027,7 @@
         <v>86188</v>
       </c>
       <c r="M44">
-        <f>10^($B$57*LOG10(L44)+$B$56)</f>
+        <f t="shared" si="4"/>
         <v>6.1387888964041307E-2</v>
       </c>
     </row>
@@ -9028,7 +9045,7 @@
         <v>45441</v>
       </c>
       <c r="M45">
-        <f>10^($B$57*LOG10(L45)+$B$56)</f>
+        <f t="shared" si="4"/>
         <v>2.7669949480603664E-2</v>
       </c>
     </row>
@@ -9046,7 +9063,7 @@
         <v>31185</v>
       </c>
       <c r="M46">
-        <f>10^($B$57*LOG10(L46)+$B$56)</f>
+        <f t="shared" si="4"/>
         <v>1.731683029216274E-2</v>
       </c>
     </row>
@@ -9064,7 +9081,7 @@
         <v>24929</v>
       </c>
       <c r="M47">
-        <f>10^($B$57*LOG10(L47)+$B$56)</f>
+        <f t="shared" si="4"/>
         <v>1.3104350443761088E-2</v>
       </c>
     </row>
@@ -9076,7 +9093,7 @@
         <v>1975</v>
       </c>
       <c r="M48">
-        <f>10^($B$57*LOG10(L48)+$B$56)</f>
+        <f t="shared" si="4"/>
         <v>5.5800097113146443E-4</v>
       </c>
     </row>
@@ -9091,7 +9108,7 @@
         <v>26130</v>
       </c>
       <c r="M49">
-        <f>10^($B$57*LOG10(L49)+$B$56)</f>
+        <f t="shared" si="4"/>
         <v>1.3894854164478233E-2</v>
       </c>
     </row>
@@ -9119,7 +9136,7 @@
         <v>22303</v>
       </c>
       <c r="M50">
-        <f>10^($B$57*LOG10(L50)+$B$56)</f>
+        <f t="shared" si="4"/>
         <v>1.1408701284690223E-2</v>
       </c>
     </row>
@@ -9149,7 +9166,7 @@
         <v>19783</v>
       </c>
       <c r="M51">
-        <f>10^($B$57*LOG10(L51)+$B$56)</f>
+        <f t="shared" si="4"/>
         <v>9.8268443584452556E-3</v>
       </c>
     </row>
@@ -9173,7 +9190,7 @@
         <v>14478</v>
       </c>
       <c r="M52">
-        <f>10^($B$57*LOG10(L52)+$B$56)</f>
+        <f t="shared" si="4"/>
         <v>6.6623779084662204E-3</v>
       </c>
     </row>
@@ -9197,7 +9214,7 @@
         <v>12145</v>
       </c>
       <c r="M53">
-        <f>10^($B$57*LOG10(L53)+$B$56)</f>
+        <f t="shared" si="4"/>
         <v>5.3534213285283943E-3</v>
       </c>
     </row>
@@ -9209,7 +9226,7 @@
         <v>14609</v>
       </c>
       <c r="M54">
-        <f>10^($B$57*LOG10(L54)+$B$56)</f>
+        <f t="shared" si="4"/>
         <v>6.7375052531226162E-3</v>
       </c>
     </row>
@@ -9356,7 +9373,7 @@
         <v>93024</v>
       </c>
       <c r="M66">
-        <f t="shared" ref="M66:M77" si="4">10^($B$80*LOG10(L66)+$B$79)</f>
+        <f t="shared" ref="M66:M77" si="5">10^($B$80*LOG10(L66)+$B$79)</f>
         <v>5.5539298723601756E-2</v>
       </c>
     </row>
@@ -9374,7 +9391,7 @@
         <v>86188</v>
       </c>
       <c r="M67">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5.0497812064730196E-2</v>
       </c>
     </row>
@@ -9392,7 +9409,7 @@
         <v>45441</v>
       </c>
       <c r="M68">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.2733948133172519E-2</v>
       </c>
     </row>
@@ -9410,7 +9427,7 @@
         <v>31185</v>
       </c>
       <c r="M69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.4217626083413358E-2</v>
       </c>
     </row>
@@ -9428,7 +9445,7 @@
         <v>24929</v>
       </c>
       <c r="M70">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.075452217344529E-2</v>
       </c>
     </row>
@@ -9440,7 +9457,7 @@
         <v>1975</v>
       </c>
       <c r="M71">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.5576142039897643E-4</v>
       </c>
     </row>
@@ -9455,7 +9472,7 @@
         <v>0</v>
       </c>
       <c r="M72" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>#NUM!</v>
       </c>
     </row>
@@ -9483,7 +9500,7 @@
         <v>22303</v>
       </c>
       <c r="M73">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>9.3609693069967321E-3</v>
       </c>
     </row>
@@ -9513,7 +9530,7 @@
         <v>197830</v>
       </c>
       <c r="M74">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.14228522207085967</v>
       </c>
     </row>
@@ -9537,7 +9554,7 @@
         <v>14478</v>
       </c>
       <c r="M75">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5.4621119181234735E-3</v>
       </c>
     </row>
@@ -9561,7 +9578,7 @@
         <v>100</v>
       </c>
       <c r="M76">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.1052930563393005E-5</v>
       </c>
     </row>
@@ -9573,7 +9590,7 @@
         <v>14609</v>
       </c>
       <c r="M77">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5.5237983062126324E-3</v>
       </c>
     </row>
@@ -9755,19 +9772,19 @@
         <v>0.1</v>
       </c>
       <c r="G87">
-        <f t="shared" ref="G87:G103" si="5">F87/(2*(1+0.1+0.01+0.001+0.0001))</f>
+        <f t="shared" ref="G87:G103" si="6">F87/(2*(1+0.1+0.01+0.001+0.0001))</f>
         <v>4.5000450004500051E-2</v>
       </c>
       <c r="H87">
-        <f t="shared" ref="H87:H103" si="6">E87*G87</f>
+        <f t="shared" ref="H87:H103" si="7">E87*G87</f>
         <v>1.1250112501125013E-2</v>
       </c>
       <c r="I87">
-        <f t="shared" ref="I87:I103" si="7">LOG10(C87)</f>
+        <f t="shared" ref="I87:I103" si="8">LOG10(C87)</f>
         <v>4.181557773862786</v>
       </c>
       <c r="J87" s="2">
-        <f t="shared" ref="J87:J103" si="8">LOG10(H87)</f>
+        <f t="shared" ref="J87:J103" si="9">LOG10(H87)</f>
         <v>-1.9488431345860848</v>
       </c>
     </row>
@@ -9791,19 +9808,19 @@
         <v>0.01</v>
       </c>
       <c r="G88">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4.5000450004500049E-3</v>
       </c>
       <c r="H88">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.1250112501125012E-3</v>
       </c>
       <c r="I88">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3.3886339693517891</v>
       </c>
       <c r="J88" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-2.9488431345860846</v>
       </c>
     </row>
@@ -9827,19 +9844,19 @@
         <v>1E-3</v>
       </c>
       <c r="G89">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4.5000450004500047E-4</v>
       </c>
       <c r="H89">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.1250112501125012E-4</v>
       </c>
       <c r="I89">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2.4885507165004443</v>
       </c>
       <c r="J89" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-3.9488431345860846</v>
       </c>
     </row>
@@ -9863,19 +9880,19 @@
         <v>1E-4</v>
       </c>
       <c r="G90">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4.5000450004500049E-5</v>
       </c>
       <c r="H90">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.1250112501125012E-5</v>
       </c>
       <c r="I90">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2.173186268412274</v>
       </c>
       <c r="J90" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-4.9488431345860846</v>
       </c>
     </row>
@@ -9899,19 +9916,19 @@
         <v>1E-3</v>
       </c>
       <c r="G91">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4.5000450004500047E-4</v>
       </c>
       <c r="H91">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.1250112501125012E-4</v>
       </c>
       <c r="I91">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3.0314084642516241</v>
       </c>
       <c r="J91" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-3.9488431345860846</v>
       </c>
     </row>
@@ -9935,19 +9952,19 @@
         <v>0.01</v>
       </c>
       <c r="G92">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4.5000450004500049E-3</v>
       </c>
       <c r="H92">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.1250112501125012E-3</v>
       </c>
       <c r="I92">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3.5036545192429593</v>
       </c>
       <c r="J92" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-2.9488431345860846</v>
       </c>
     </row>
@@ -9971,19 +9988,19 @@
         <v>0.1</v>
       </c>
       <c r="G93">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4.5000450004500051E-2</v>
       </c>
       <c r="H93">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.1250112501125013E-2</v>
       </c>
       <c r="I93">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>4.4039265648312682</v>
       </c>
       <c r="J93" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-1.9488431345860848</v>
       </c>
     </row>
@@ -10007,19 +10024,19 @@
         <v>1</v>
       </c>
       <c r="G94">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.45000450004500048</v>
       </c>
       <c r="H94">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.11250112501125012</v>
       </c>
       <c r="I94">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5.3753508093107225</v>
       </c>
       <c r="J94" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-0.94884313458608482</v>
       </c>
     </row>
@@ -10043,19 +10060,19 @@
         <v>1</v>
       </c>
       <c r="G95">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.45000450004500048</v>
       </c>
       <c r="H95">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>9.0000900009000101E-2</v>
       </c>
       <c r="I95">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>4.958549549834224</v>
       </c>
       <c r="J95" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-1.0457531475941411</v>
       </c>
     </row>
@@ -10079,19 +10096,19 @@
         <v>0.1</v>
       </c>
       <c r="G96">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4.5000450004500051E-2</v>
       </c>
       <c r="H96">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>9.0000900009000098E-3</v>
       </c>
       <c r="I96">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>4.1761491611265491</v>
       </c>
       <c r="J96" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-2.0457531475941413</v>
       </c>
     </row>
@@ -10115,19 +10132,19 @@
         <v>0.01</v>
       </c>
       <c r="G97">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4.5000450004500049E-3</v>
       </c>
       <c r="H97">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>9.0000900009000104E-4</v>
       </c>
       <c r="I97">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3.3839947894417328</v>
       </c>
       <c r="J97" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-3.0457531475941413</v>
       </c>
     </row>
@@ -10151,19 +10168,19 @@
         <v>1E-3</v>
       </c>
       <c r="G98">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4.5000450004500047E-4</v>
       </c>
       <c r="H98">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>9.0000900009000099E-5</v>
       </c>
       <c r="I98">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2.4712917110589387</v>
       </c>
       <c r="J98" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-4.0457531475941408</v>
       </c>
     </row>
@@ -10187,19 +10204,19 @@
         <v>1E-4</v>
       </c>
       <c r="G99">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4.5000450004500049E-5</v>
       </c>
       <c r="H99">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>9.0000900009000095E-6</v>
       </c>
       <c r="I99">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2.1702617153949575</v>
       </c>
       <c r="J99" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-5.0457531475941408</v>
       </c>
     </row>
@@ -10223,19 +10240,19 @@
         <v>1E-3</v>
       </c>
       <c r="G100">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4.5000450004500047E-4</v>
       </c>
       <c r="H100">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>9.0000900009000099E-5</v>
       </c>
       <c r="I100">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3.024895960107485</v>
       </c>
       <c r="J100" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-4.0457531475941408</v>
       </c>
     </row>
@@ -10259,19 +10276,19 @@
         <v>0.01</v>
       </c>
       <c r="G101">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4.5000450004500049E-3</v>
       </c>
       <c r="H101">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>9.0000900009000104E-4</v>
       </c>
       <c r="I101">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3.4954055631461931</v>
       </c>
       <c r="J101" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-3.0457531475941413</v>
       </c>
     </row>
@@ -10295,19 +10312,19 @@
         <v>0.1</v>
       </c>
       <c r="G102">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4.5000450004500051E-2</v>
       </c>
       <c r="H102">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>9.0000900009000098E-3</v>
       </c>
       <c r="I102">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>4.3954312402469178</v>
       </c>
       <c r="J102" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-2.0457531475941413</v>
       </c>
     </row>
@@ -10331,19 +10348,19 @@
         <v>1</v>
       </c>
       <c r="G103">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.45000450004500048</v>
       </c>
       <c r="H103">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>9.0000900009000101E-2</v>
       </c>
       <c r="I103">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5.3634201711470348</v>
       </c>
       <c r="J103" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-1.0457531475941411</v>
       </c>
     </row>
@@ -10406,7 +10423,7 @@
         <v>93024</v>
       </c>
       <c r="M109">
-        <f t="shared" ref="M109:M120" si="9">10^($B$123*LOG10(L109)+$B$122)</f>
+        <f t="shared" ref="M109:M120" si="10">10^($B$123*LOG10(L109)+$B$122)</f>
         <v>6.8694072413691618E-2</v>
       </c>
     </row>
@@ -10424,7 +10441,7 @@
         <v>86188</v>
       </c>
       <c r="M110">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6.2413516819281277E-2</v>
       </c>
     </row>
@@ -10442,7 +10459,7 @@
         <v>45441</v>
       </c>
       <c r="M111">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>2.7929156677989907E-2</v>
       </c>
     </row>
@@ -10460,7 +10477,7 @@
         <v>31185</v>
       </c>
       <c r="M112">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1.7404729442059844E-2</v>
       </c>
     </row>
@@ -10478,7 +10495,7 @@
         <v>24929</v>
       </c>
       <c r="M113">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1.3137531319523383E-2</v>
       </c>
     </row>
@@ -10490,7 +10507,7 @@
         <v>1975</v>
       </c>
       <c r="M114">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.4358832056686452E-4</v>
       </c>
     </row>
@@ -10505,7 +10522,7 @@
         <v>26130</v>
       </c>
       <c r="M115">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1.3937457137122871E-2</v>
       </c>
     </row>
@@ -10533,7 +10550,7 @@
         <v>22303</v>
       </c>
       <c r="M116">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1.1423188046374242E-2</v>
       </c>
     </row>
@@ -10563,7 +10580,7 @@
         <v>19783</v>
       </c>
       <c r="M117">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>9.825979039056295E-3</v>
       </c>
     </row>
@@ -10587,7 +10604,7 @@
         <v>14478</v>
       </c>
       <c r="M118">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6.6382932210282009E-3</v>
       </c>
     </row>
@@ -10611,7 +10628,7 @@
         <v>12145</v>
       </c>
       <c r="M119">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.3234707867863395E-3</v>
       </c>
     </row>
@@ -10623,7 +10640,7 @@
         <v>14609</v>
       </c>
       <c r="M120">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6.7138334227200775E-3</v>
       </c>
     </row>
@@ -10771,7 +10788,7 @@
         <v>93024</v>
       </c>
       <c r="M132">
-        <f t="shared" ref="M132:M143" si="10">10^($B$146*LOG10(L132)+$B$145)</f>
+        <f t="shared" ref="M132:M143" si="11">10^($B$146*LOG10(L132)+$B$145)</f>
         <v>5.6415301020446777E-2</v>
       </c>
     </row>
@@ -10789,7 +10806,7 @@
         <v>86188</v>
       </c>
       <c r="M133">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>5.1254925559760744E-2</v>
       </c>
     </row>
@@ -10807,7 +10824,7 @@
         <v>45441</v>
       </c>
       <c r="M134">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>2.2926683046415791E-2</v>
       </c>
     </row>
@@ -10825,7 +10842,7 @@
         <v>31185</v>
       </c>
       <c r="M135">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.4283959522586398E-2</v>
       </c>
     </row>
@@ -10843,7 +10860,7 @@
         <v>24929</v>
       </c>
       <c r="M136">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.0780388040473274E-2</v>
       </c>
     </row>
@@ -10855,7 +10872,7 @@
         <v>1975</v>
       </c>
       <c r="M137">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>4.4535192393756743E-4</v>
       </c>
     </row>
@@ -10870,7 +10887,7 @@
         <v>0</v>
       </c>
       <c r="M138" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>#NUM!</v>
       </c>
     </row>
@@ -10898,7 +10915,7 @@
         <v>22303</v>
       </c>
       <c r="M139">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>9.3729818674479215E-3</v>
       </c>
     </row>
@@ -10928,7 +10945,7 @@
         <v>197830</v>
       </c>
       <c r="M140">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.14563070898747268</v>
       </c>
     </row>
@@ -10952,7 +10969,7 @@
         <v>14478</v>
       </c>
       <c r="M141">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>5.4453993386522825E-3</v>
       </c>
     </row>
@@ -10976,7 +10993,7 @@
         <v>100</v>
       </c>
       <c r="M142">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.0481169495883429E-5</v>
       </c>
     </row>
@@ -10988,7 +11005,7 @@
         <v>14609</v>
       </c>
       <c r="M143">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>5.5073960193810691E-3</v>
       </c>
     </row>
@@ -11085,10 +11102,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7E102CF-57E9-CF4D-8304-DA1926A37703}">
-  <dimension ref="A1:AS48"/>
+  <dimension ref="A1:AU58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K16" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+    <sheetView tabSelected="1" topLeftCell="AB29" workbookViewId="0">
+      <selection activeCell="Q43" sqref="Q43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11757,7 +11774,7 @@
         <v>79950</v>
       </c>
       <c r="M32">
-        <f>10^($B$47*LOG10(L32)+$B$46)</f>
+        <f t="shared" ref="M32:M44" si="4">10^($B$47*LOG10(L32)+$B$46)</f>
         <v>5.5906776314467152E-2</v>
       </c>
       <c r="P32" s="48" t="s">
@@ -11773,7 +11790,7 @@
         <v>1.19</v>
       </c>
     </row>
-    <row r="33" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>128</v>
       </c>
@@ -11790,7 +11807,7 @@
         <v>93024</v>
       </c>
       <c r="M33">
-        <f>10^($B$47*LOG10(L33)+$B$46)</f>
+        <f t="shared" si="4"/>
         <v>6.7506893569518861E-2</v>
       </c>
       <c r="P33" s="48" t="s">
@@ -11806,7 +11823,7 @@
         <v>7.24</v>
       </c>
     </row>
-    <row r="34" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>129</v>
       </c>
@@ -11823,7 +11840,7 @@
         <v>86188</v>
       </c>
       <c r="M34">
-        <f>10^($B$47*LOG10(L34)+$B$46)</f>
+        <f t="shared" si="4"/>
         <v>6.1387888964041307E-2</v>
       </c>
       <c r="P34" s="48" t="s">
@@ -11839,7 +11856,7 @@
         <v>92.65</v>
       </c>
     </row>
-    <row r="35" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>130</v>
       </c>
@@ -11853,7 +11870,7 @@
         <v>45441</v>
       </c>
       <c r="M35">
-        <f>10^($B$47*LOG10(L35)+$B$46)</f>
+        <f t="shared" si="4"/>
         <v>2.7669949480603664E-2</v>
       </c>
       <c r="P35" s="48" t="s">
@@ -11869,7 +11886,7 @@
         <v>3.58</v>
       </c>
     </row>
-    <row r="36" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>131</v>
       </c>
@@ -11886,7 +11903,7 @@
         <v>31185</v>
       </c>
       <c r="M36">
-        <f>10^($B$47*LOG10(L36)+$B$46)</f>
+        <f t="shared" si="4"/>
         <v>1.731683029216274E-2</v>
       </c>
       <c r="P36" s="48" t="s">
@@ -11902,7 +11919,7 @@
         <v>4.24</v>
       </c>
     </row>
-    <row r="37" spans="1:45" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:47" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="30" t="s">
         <v>132</v>
       </c>
@@ -11919,7 +11936,7 @@
         <v>24929</v>
       </c>
       <c r="M37">
-        <f>10^($B$47*LOG10(L37)+$B$46)</f>
+        <f t="shared" si="4"/>
         <v>1.3104350443761088E-2</v>
       </c>
       <c r="P37" s="48" t="s">
@@ -11935,7 +11952,7 @@
         <v>0.72</v>
       </c>
     </row>
-    <row r="38" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:47" x14ac:dyDescent="0.2">
       <c r="J38" t="s">
         <v>293</v>
       </c>
@@ -11946,7 +11963,7 @@
         <v>1975</v>
       </c>
       <c r="M38">
-        <f>10^($B$47*LOG10(L38)+$B$46)</f>
+        <f t="shared" si="4"/>
         <v>5.5800097113146443E-4</v>
       </c>
       <c r="P38" s="48" t="s">
@@ -11959,7 +11976,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="39" spans="1:45" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:47" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>133</v>
       </c>
@@ -11970,11 +11987,11 @@
         <v>26130</v>
       </c>
       <c r="M39">
-        <f>10^($B$47*LOG10(L39)+$B$46)</f>
+        <f t="shared" si="4"/>
         <v>1.3894854164478233E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A40" s="31"/>
       <c r="B40" s="31" t="s">
         <v>138</v>
@@ -11998,11 +12015,11 @@
         <v>22303</v>
       </c>
       <c r="M40">
-        <f>10^($B$47*LOG10(L40)+$B$46)</f>
+        <f t="shared" si="4"/>
         <v>1.1408701284690223E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>134</v>
       </c>
@@ -12028,15 +12045,13 @@
         <v>19783</v>
       </c>
       <c r="M41">
-        <f>10^($B$47*LOG10(L41)+$B$46)</f>
+        <f t="shared" si="4"/>
         <v>9.8268443584452556E-3</v>
       </c>
       <c r="P41" s="48"/>
       <c r="Q41" s="48" t="s">
         <v>278</v>
       </c>
-      <c r="V41" s="51"/>
-      <c r="W41" s="51"/>
       <c r="AI41" s="48"/>
       <c r="AJ41" s="48" t="s">
         <v>278</v>
@@ -12054,7 +12069,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="42" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>135</v>
       </c>
@@ -12074,7 +12089,7 @@
         <v>14478</v>
       </c>
       <c r="M42">
-        <f>10^($B$47*LOG10(L42)+$B$46)</f>
+        <f t="shared" si="4"/>
         <v>6.6623779084662204E-3</v>
       </c>
       <c r="P42" s="48" t="s">
@@ -12114,7 +12129,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="43" spans="1:45" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:47" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="30" t="s">
         <v>136</v>
       </c>
@@ -12134,7 +12149,7 @@
         <v>12145</v>
       </c>
       <c r="M43">
-        <f>10^($B$47*LOG10(L43)+$B$46)</f>
+        <f t="shared" si="4"/>
         <v>5.3534213285283943E-3</v>
       </c>
       <c r="P43" s="48" t="s">
@@ -12147,7 +12162,7 @@
       <c r="Y43" s="48" t="s">
         <v>287</v>
       </c>
-      <c r="Z43" s="52">
+      <c r="Z43" s="51">
         <f>'full_calcs on correct masses '!G78</f>
         <v>1904788.3330000001</v>
       </c>
@@ -12157,33 +12172,37 @@
       <c r="AI43" s="48" t="s">
         <v>287</v>
       </c>
-      <c r="AJ43" s="52">
-        <f>'full_calcs on correct masses '!G79</f>
+      <c r="AJ43" s="51">
+        <f>(Q43*6.02214076E+23)/(Z43*650*1000000000)</f>
         <v>27192.884259161423</v>
       </c>
       <c r="AL43" s="48" t="s">
         <v>287</v>
       </c>
-      <c r="AM43" s="54">
-        <f>'full_calcs on correct masses '!G81</f>
-        <v>5438576851832.2852</v>
-      </c>
+      <c r="AM43" s="52">
+        <f>AJ53* 1000000000/'full_calcs on correct masses '!$G$34</f>
+        <v>5438576851832.2842</v>
+      </c>
+      <c r="AN43" s="53"/>
       <c r="AO43" s="48" t="s">
         <v>287</v>
       </c>
-      <c r="AP43" s="52">
-        <f>'full_calcs on correct masses '!$G$82</f>
+      <c r="AP43" s="51">
+        <f>$AM53*'full_calcs on correct masses '!$G$29</f>
         <v>39085654.849706717</v>
       </c>
+      <c r="AQ43" s="53"/>
       <c r="AR43" s="48" t="s">
         <v>287</v>
       </c>
-      <c r="AS43" s="52">
-        <f>'full_calcs on correct masses '!$G$82</f>
+      <c r="AS43" s="51">
+        <f>$AM53*'full_calcs on correct masses '!$G$29</f>
         <v>39085654.849706717</v>
       </c>
-    </row>
-    <row r="44" spans="1:45" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AT43" s="54"/>
+      <c r="AU43" s="55"/>
+    </row>
+    <row r="44" spans="1:47" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="K44" t="str">
         <v>Veillonella dispar</v>
       </c>
@@ -12191,7 +12210,7 @@
         <v>14609</v>
       </c>
       <c r="M44">
-        <f>10^($B$47*LOG10(L44)+$B$46)</f>
+        <f t="shared" si="4"/>
         <v>6.7375052531226162E-3</v>
       </c>
       <c r="P44" s="48" t="s">
@@ -12204,7 +12223,7 @@
       <c r="Y44" s="48" t="s">
         <v>289</v>
       </c>
-      <c r="Z44" s="52">
+      <c r="Z44" s="51">
         <f>'full_calcs on correct masses '!G88</f>
         <v>4373730</v>
       </c>
@@ -12214,33 +12233,37 @@
       <c r="AI44" s="48" t="s">
         <v>289</v>
       </c>
-      <c r="AJ44" s="52">
-        <f>'full_calcs on correct masses '!G89</f>
+      <c r="AJ44" s="51">
+        <f>(Q44*6.02214076E+23)/(Z44*650*1000000000)</f>
         <v>14299.923031581789</v>
       </c>
       <c r="AL44" s="48" t="s">
         <v>289</v>
       </c>
-      <c r="AM44" s="54">
-        <f>'full_calcs on correct masses '!G91</f>
+      <c r="AM44" s="52">
+        <f>AJ54* 1000000000/'full_calcs on correct masses '!$G$34</f>
         <v>2859984606316.3579</v>
       </c>
+      <c r="AN44" s="53"/>
       <c r="AO44" s="48" t="s">
         <v>289</v>
       </c>
-      <c r="AP44" s="52">
-        <f>'full_calcs on correct masses '!$G$92</f>
+      <c r="AP44" s="51">
+        <f>$AM54*'full_calcs on correct masses '!$G$29</f>
         <v>20553974.733352304</v>
       </c>
+      <c r="AQ44" s="53"/>
       <c r="AR44" s="48" t="s">
         <v>289</v>
       </c>
-      <c r="AS44" s="52">
-        <f>'full_calcs on correct masses '!$G$92</f>
+      <c r="AS44" s="51">
+        <f>$AM54*'full_calcs on correct masses '!$G$29</f>
         <v>20553974.733352304</v>
       </c>
-    </row>
-    <row r="45" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT44" s="54"/>
+      <c r="AU44" s="55"/>
+    </row>
+    <row r="45" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A45" s="31"/>
       <c r="B45" s="31" t="s">
         <v>143</v>
@@ -12276,7 +12299,7 @@
       <c r="Y45" s="48" t="s">
         <v>290</v>
       </c>
-      <c r="Z45" s="52">
+      <c r="Z45" s="51">
         <v>3489300</v>
       </c>
       <c r="AB45" t="s">
@@ -12285,33 +12308,34 @@
       <c r="AI45" s="48" t="s">
         <v>290</v>
       </c>
-      <c r="AJ45" s="52">
+      <c r="AJ45" s="51">
         <f>(Q45*6.02214076E+23)/(Z45*650*1000000000)</f>
         <v>16299.787186793354</v>
       </c>
       <c r="AL45" s="48" t="s">
         <v>290</v>
       </c>
-      <c r="AM45" s="54">
-        <f>AJ45* 1000000000/5</f>
+      <c r="AM45" s="52">
+        <f>AJ55* 1000000000/'full_calcs on correct masses '!$G$34</f>
         <v>3259957437358.6709</v>
       </c>
       <c r="AO45" s="48" t="s">
         <v>290</v>
       </c>
-      <c r="AP45" s="52">
-        <f>$AM$45*'full_calcs on correct masses '!$G$29</f>
+      <c r="AP45" s="51">
+        <f>$AM55*'full_calcs on correct masses '!$G$29</f>
         <v>23428476.730710857</v>
       </c>
       <c r="AR45" s="48" t="s">
         <v>290</v>
       </c>
-      <c r="AS45" s="52">
-        <f>$AM$45*'full_calcs on correct masses '!$G$29</f>
+      <c r="AS45" s="51">
+        <f>$AM55*'full_calcs on correct masses '!$G$29</f>
         <v>23428476.730710857</v>
       </c>
-    </row>
-    <row r="46" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AU45" s="55"/>
+    </row>
+    <row r="46" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>137</v>
       </c>
@@ -12349,7 +12373,7 @@
       <c r="Y46" s="48" t="s">
         <v>291</v>
       </c>
-      <c r="Z46" s="52">
+      <c r="Z46" s="51">
         <v>9202483</v>
       </c>
       <c r="AB46" t="s">
@@ -12358,33 +12382,34 @@
       <c r="AI46" s="48" t="s">
         <v>291</v>
       </c>
-      <c r="AJ46" s="52">
+      <c r="AJ46" s="51">
         <f>(Q46*6.02214076E+23)/(Z46*650*1000000000)</f>
         <v>1743.4155799445389</v>
       </c>
       <c r="AL46" s="48" t="s">
         <v>291</v>
       </c>
-      <c r="AM46" s="54">
-        <f>AJ46* 1000000000/5</f>
+      <c r="AM46" s="52">
+        <f>AJ56* 1000000000/'full_calcs on correct masses '!$G$34</f>
         <v>348683115988.90778</v>
       </c>
       <c r="AO46" s="48" t="s">
         <v>291</v>
       </c>
-      <c r="AP46" s="52">
-        <f>$AM$46*'full_calcs on correct masses '!$G$29</f>
+      <c r="AP46" s="51">
+        <f>$AM56*'full_calcs on correct masses '!$G$29</f>
         <v>2505895.9898435902</v>
       </c>
       <c r="AR46" s="48" t="s">
         <v>291</v>
       </c>
-      <c r="AS46" s="52">
-        <f>$AM$46*'full_calcs on correct masses '!$G$29</f>
+      <c r="AS46" s="51">
+        <f>$AM56*'full_calcs on correct masses '!$G$29</f>
         <v>2505895.9898435902</v>
       </c>
-    </row>
-    <row r="47" spans="1:45" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AU46" s="55"/>
+    </row>
+    <row r="47" spans="1:47" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="30" t="s">
         <v>166</v>
       </c>
@@ -12422,7 +12447,7 @@
       <c r="Y47" s="48" t="s">
         <v>292</v>
       </c>
-      <c r="Z47" s="52">
+      <c r="Z47" s="51">
         <v>10348543</v>
       </c>
       <c r="AB47" t="s">
@@ -12431,33 +12456,34 @@
       <c r="AI47" s="48" t="s">
         <v>292</v>
       </c>
-      <c r="AJ47" s="52">
+      <c r="AJ47" s="51">
         <f>(Q47*6.02214076E+23)/(Z47*650*1000000000)</f>
         <v>1173.2048127369269</v>
       </c>
       <c r="AL47" s="48" t="s">
         <v>292</v>
       </c>
-      <c r="AM47" s="54">
-        <f>AJ47* 1000000000/5</f>
+      <c r="AM47" s="52">
+        <f>AJ57* 1000000000/'full_calcs on correct masses '!$G$34</f>
         <v>234640962547.38541</v>
       </c>
       <c r="AO47" s="48" t="s">
         <v>292</v>
       </c>
-      <c r="AP47" s="52">
-        <f>$AM$47*'full_calcs on correct masses '!$G$29</f>
+      <c r="AP47" s="51">
+        <f>$AM57*'full_calcs on correct masses '!$G$29</f>
         <v>1686304.3265887243</v>
       </c>
       <c r="AR47" s="48" t="s">
         <v>292</v>
       </c>
-      <c r="AS47" s="52">
-        <f>$AM$47*'full_calcs on correct masses '!$G$29</f>
+      <c r="AS47" s="51">
+        <f>$AM57*'full_calcs on correct masses '!$G$29</f>
         <v>1686304.3265887243</v>
       </c>
-    </row>
-    <row r="48" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AU47" s="55"/>
+    </row>
+    <row r="48" spans="1:47" x14ac:dyDescent="0.2">
       <c r="P48" s="48" t="s">
         <v>293</v>
       </c>
@@ -12468,7 +12494,7 @@
       <c r="Y48" s="48" t="s">
         <v>293</v>
       </c>
-      <c r="Z48" s="53">
+      <c r="Z48" s="51">
         <f>'full_calcs on correct masses '!G98</f>
         <v>89264</v>
       </c>
@@ -12478,30 +12504,299 @@
       <c r="AI48" s="48" t="s">
         <v>293</v>
       </c>
-      <c r="AJ48" s="52">
+      <c r="AJ48" s="51">
+        <f>(Q48*6.02214076E+23)/(Z48*650*1000000000)</f>
+        <v>5791.5679546416768</v>
+      </c>
+      <c r="AL48" s="48" t="s">
+        <v>293</v>
+      </c>
+      <c r="AM48" s="52">
+        <f>AJ58* 1000000000/'full_calcs on correct masses '!$G$34</f>
+        <v>1158313590928.3354</v>
+      </c>
+      <c r="AN48" s="53"/>
+      <c r="AO48" s="48" t="s">
+        <v>293</v>
+      </c>
+      <c r="AP48" s="51">
+        <f>$AM58*'full_calcs on correct masses '!$G$29</f>
+        <v>8324502.2468509236</v>
+      </c>
+      <c r="AQ48" s="53"/>
+      <c r="AR48" s="48" t="s">
+        <v>293</v>
+      </c>
+      <c r="AS48" s="51">
+        <f>$AM58*'full_calcs on correct masses '!$G$29</f>
+        <v>8324502.2468509236</v>
+      </c>
+      <c r="AT48" s="54"/>
+      <c r="AU48" s="55"/>
+    </row>
+    <row r="50" spans="35:46" x14ac:dyDescent="0.2">
+      <c r="AI50" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="51" spans="35:46" x14ac:dyDescent="0.2">
+      <c r="AI51" s="48"/>
+      <c r="AJ51" s="48" t="s">
+        <v>278</v>
+      </c>
+      <c r="AL51" s="48"/>
+      <c r="AM51" s="48" t="s">
+        <v>278</v>
+      </c>
+      <c r="AO51" s="48"/>
+      <c r="AP51" s="48" t="s">
+        <v>278</v>
+      </c>
+      <c r="AR51" s="48"/>
+      <c r="AS51" s="48" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="52" spans="35:46" x14ac:dyDescent="0.2">
+      <c r="AI52" s="48" t="s">
+        <v>294</v>
+      </c>
+      <c r="AJ52" s="48" t="s">
+        <v>305</v>
+      </c>
+      <c r="AL52" s="48" t="s">
+        <v>294</v>
+      </c>
+      <c r="AM52" s="48" t="s">
+        <v>306</v>
+      </c>
+      <c r="AO52" s="48" t="s">
+        <v>294</v>
+      </c>
+      <c r="AP52" s="48" t="s">
+        <v>307</v>
+      </c>
+      <c r="AR52" s="48" t="s">
+        <v>294</v>
+      </c>
+      <c r="AS52" s="48" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="53" spans="35:46" x14ac:dyDescent="0.2">
+      <c r="AI53" s="48" t="s">
+        <v>287</v>
+      </c>
+      <c r="AJ53" s="51">
+        <f>'full_calcs on correct masses '!G79</f>
+        <v>27192.884259161423</v>
+      </c>
+      <c r="AK53" t="s">
+        <v>309</v>
+      </c>
+      <c r="AL53" s="48" t="s">
+        <v>287</v>
+      </c>
+      <c r="AM53" s="52">
+        <f>'full_calcs on correct masses '!G81</f>
+        <v>5438576851832.2852</v>
+      </c>
+      <c r="AN53" s="53" t="s">
+        <v>309</v>
+      </c>
+      <c r="AO53" s="48" t="s">
+        <v>287</v>
+      </c>
+      <c r="AP53" s="51">
+        <f>'full_calcs on correct masses '!$G$82</f>
+        <v>39085654.849706717</v>
+      </c>
+      <c r="AQ53" s="53" t="s">
+        <v>309</v>
+      </c>
+      <c r="AR53" s="48" t="s">
+        <v>287</v>
+      </c>
+      <c r="AS53" s="51">
+        <f>'full_calcs on correct masses '!$G$82</f>
+        <v>39085654.849706717</v>
+      </c>
+      <c r="AT53" s="53" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="54" spans="35:46" x14ac:dyDescent="0.2">
+      <c r="AI54" s="48" t="s">
+        <v>289</v>
+      </c>
+      <c r="AJ54" s="51">
+        <f>'full_calcs on correct masses '!G89</f>
+        <v>14299.923031581789</v>
+      </c>
+      <c r="AK54" t="s">
+        <v>309</v>
+      </c>
+      <c r="AL54" s="48" t="s">
+        <v>289</v>
+      </c>
+      <c r="AM54" s="52">
+        <f>'full_calcs on correct masses '!G91</f>
+        <v>2859984606316.3579</v>
+      </c>
+      <c r="AN54" s="53" t="s">
+        <v>309</v>
+      </c>
+      <c r="AO54" s="48" t="s">
+        <v>289</v>
+      </c>
+      <c r="AP54" s="51">
+        <f>'full_calcs on correct masses '!$G$92</f>
+        <v>20553974.733352304</v>
+      </c>
+      <c r="AQ54" s="53" t="s">
+        <v>309</v>
+      </c>
+      <c r="AR54" s="48" t="s">
+        <v>289</v>
+      </c>
+      <c r="AS54" s="51">
+        <f>'full_calcs on correct masses '!$G$92</f>
+        <v>20553974.733352304</v>
+      </c>
+      <c r="AT54" s="53" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="55" spans="35:46" x14ac:dyDescent="0.2">
+      <c r="AI55" s="48" t="s">
+        <v>290</v>
+      </c>
+      <c r="AJ55" s="51">
+        <f>(Q45*6.02214076E+23)/(Z45*650*1000000000)</f>
+        <v>16299.787186793354</v>
+      </c>
+      <c r="AL55" s="48" t="s">
+        <v>290</v>
+      </c>
+      <c r="AM55" s="52">
+        <f>AJ55* 1000000000/'full_calcs on correct masses '!$G$34</f>
+        <v>3259957437358.6709</v>
+      </c>
+      <c r="AO55" s="48" t="s">
+        <v>290</v>
+      </c>
+      <c r="AP55" s="51">
+        <f>$AM55*'full_calcs on correct masses '!$G$29</f>
+        <v>23428476.730710857</v>
+      </c>
+      <c r="AR55" s="48" t="s">
+        <v>290</v>
+      </c>
+      <c r="AS55" s="51">
+        <f>$AM55*'full_calcs on correct masses '!$G$29</f>
+        <v>23428476.730710857</v>
+      </c>
+    </row>
+    <row r="56" spans="35:46" x14ac:dyDescent="0.2">
+      <c r="AI56" s="48" t="s">
+        <v>291</v>
+      </c>
+      <c r="AJ56" s="51">
+        <f>(Q46*6.02214076E+23)/(Z46*650*1000000000)</f>
+        <v>1743.4155799445389</v>
+      </c>
+      <c r="AL56" s="48" t="s">
+        <v>291</v>
+      </c>
+      <c r="AM56" s="52">
+        <f>AJ56* 1000000000/'full_calcs on correct masses '!$G$34</f>
+        <v>348683115988.90778</v>
+      </c>
+      <c r="AO56" s="48" t="s">
+        <v>291</v>
+      </c>
+      <c r="AP56" s="51">
+        <f>$AM56*'full_calcs on correct masses '!$G$29</f>
+        <v>2505895.9898435902</v>
+      </c>
+      <c r="AR56" s="48" t="s">
+        <v>291</v>
+      </c>
+      <c r="AS56" s="51">
+        <f>$AM56*'full_calcs on correct masses '!$G$29</f>
+        <v>2505895.9898435902</v>
+      </c>
+    </row>
+    <row r="57" spans="35:46" x14ac:dyDescent="0.2">
+      <c r="AI57" s="48" t="s">
+        <v>292</v>
+      </c>
+      <c r="AJ57" s="51">
+        <f>(Q47*6.02214076E+23)/(Z47*650*1000000000)</f>
+        <v>1173.2048127369269</v>
+      </c>
+      <c r="AL57" s="48" t="s">
+        <v>292</v>
+      </c>
+      <c r="AM57" s="52">
+        <f>AJ57* 1000000000/'full_calcs on correct masses '!$G$34</f>
+        <v>234640962547.38541</v>
+      </c>
+      <c r="AO57" s="48" t="s">
+        <v>292</v>
+      </c>
+      <c r="AP57" s="51">
+        <f>$AM57*'full_calcs on correct masses '!$G$29</f>
+        <v>1686304.3265887243</v>
+      </c>
+      <c r="AR57" s="48" t="s">
+        <v>292</v>
+      </c>
+      <c r="AS57" s="51">
+        <f>$AM57*'full_calcs on correct masses '!$G$29</f>
+        <v>1686304.3265887243</v>
+      </c>
+    </row>
+    <row r="58" spans="35:46" x14ac:dyDescent="0.2">
+      <c r="AI58" s="48" t="s">
+        <v>293</v>
+      </c>
+      <c r="AJ58" s="51">
         <f>'full_calcs on correct masses '!G99</f>
         <v>5791.5679546416768</v>
       </c>
-      <c r="AL48" s="48" t="s">
+      <c r="AK58" t="s">
+        <v>309</v>
+      </c>
+      <c r="AL58" s="48" t="s">
         <v>293</v>
       </c>
-      <c r="AM48" s="54">
+      <c r="AM58" s="52">
         <f>'full_calcs on correct masses '!G101</f>
         <v>1158313590928.3352</v>
       </c>
-      <c r="AO48" s="48" t="s">
+      <c r="AN58" s="53" t="s">
+        <v>309</v>
+      </c>
+      <c r="AO58" s="48" t="s">
         <v>293</v>
       </c>
-      <c r="AP48" s="52">
+      <c r="AP58" s="51">
         <f>'full_calcs on correct masses '!$G$102</f>
         <v>8324502.2468509236</v>
       </c>
-      <c r="AR48" s="48" t="s">
+      <c r="AQ58" s="53" t="s">
+        <v>309</v>
+      </c>
+      <c r="AR58" s="48" t="s">
         <v>293</v>
       </c>
-      <c r="AS48" s="52">
+      <c r="AS58" s="51">
         <f>'full_calcs on correct masses '!$G$102</f>
         <v>8324502.2468509236</v>
+      </c>
+      <c r="AT58" s="53" t="s">
+        <v>309</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
support for syndna_contributing_fraction, docs updaterd to include syndna_contributing_fraction, more validation of scalar inputs
</commit_message>
<xml_diff>
--- a/docs/absolute_quant_example.xlsx
+++ b/docs/absolute_quant_example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abirmingham/Work/Repositories/pysyndna/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D69F5D4F-9A53-6042-AC4B-4C31DFF9C38E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08B8B670-B01C-ED4A-AFC4-572D58FE2ABD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1440" yWindow="920" windowWidth="31820" windowHeight="19160" activeTab="2" xr2:uid="{E184B90C-6432-8947-B7A0-BE1974B73180}"/>
   </bookViews>
@@ -113,7 +113,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G45" authorId="0" shapeId="0" xr:uid="{8B693BA1-93C6-3E41-A5C5-CF1F02304C43}">
+    <comment ref="G48" authorId="0" shapeId="0" xr:uid="{8B693BA1-93C6-3E41-A5C5-CF1F02304C43}">
       <text>
         <r>
           <rPr>
@@ -147,7 +147,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H45" authorId="0" shapeId="0" xr:uid="{389FC856-0B53-7E42-8057-35738B51BD79}">
+    <comment ref="H48" authorId="0" shapeId="0" xr:uid="{389FC856-0B53-7E42-8057-35738B51BD79}">
       <text>
         <r>
           <rPr>
@@ -181,7 +181,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I45" authorId="0" shapeId="0" xr:uid="{E5043428-D5A2-ED4E-AE6C-3557D5750211}">
+    <comment ref="I48" authorId="0" shapeId="0" xr:uid="{E5043428-D5A2-ED4E-AE6C-3557D5750211}">
       <text>
         <r>
           <rPr>
@@ -215,7 +215,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J45" authorId="0" shapeId="0" xr:uid="{25613824-9549-404A-AEA0-A34323C76842}">
+    <comment ref="J48" authorId="0" shapeId="0" xr:uid="{25613824-9549-404A-AEA0-A34323C76842}">
       <text>
         <r>
           <rPr>
@@ -249,7 +249,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G55" authorId="0" shapeId="0" xr:uid="{90312B91-03B7-3C4D-8CC8-7EBA9C5C46BF}">
+    <comment ref="G58" authorId="0" shapeId="0" xr:uid="{90312B91-03B7-3C4D-8CC8-7EBA9C5C46BF}">
       <text>
         <r>
           <rPr>
@@ -283,7 +283,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H55" authorId="0" shapeId="0" xr:uid="{96A1F8F7-75D4-6E42-AEF6-CDDA9FA6F142}">
+    <comment ref="H58" authorId="0" shapeId="0" xr:uid="{96A1F8F7-75D4-6E42-AEF6-CDDA9FA6F142}">
       <text>
         <r>
           <rPr>
@@ -317,7 +317,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I55" authorId="0" shapeId="0" xr:uid="{FC742179-E8EB-DF46-B823-D00372A3AA55}">
+    <comment ref="I58" authorId="0" shapeId="0" xr:uid="{FC742179-E8EB-DF46-B823-D00372A3AA55}">
       <text>
         <r>
           <rPr>
@@ -351,7 +351,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J55" authorId="0" shapeId="0" xr:uid="{743F2A8E-D4E3-3644-984D-989C14ACE223}">
+    <comment ref="J58" authorId="0" shapeId="0" xr:uid="{743F2A8E-D4E3-3644-984D-989C14ACE223}">
       <text>
         <r>
           <rPr>
@@ -385,7 +385,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G65" authorId="0" shapeId="0" xr:uid="{C5CB71C0-F7BB-9244-AE81-E331D978D1E1}">
+    <comment ref="G68" authorId="0" shapeId="0" xr:uid="{C5CB71C0-F7BB-9244-AE81-E331D978D1E1}">
       <text>
         <r>
           <rPr>
@@ -419,7 +419,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H65" authorId="0" shapeId="0" xr:uid="{C94A0AAD-6A4B-8E46-82F9-4A776B8500FF}">
+    <comment ref="H68" authorId="0" shapeId="0" xr:uid="{C94A0AAD-6A4B-8E46-82F9-4A776B8500FF}">
       <text>
         <r>
           <rPr>
@@ -453,7 +453,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I65" authorId="0" shapeId="0" xr:uid="{07FA6B0F-C54E-5646-8FE8-2C10468245C8}">
+    <comment ref="I68" authorId="0" shapeId="0" xr:uid="{07FA6B0F-C54E-5646-8FE8-2C10468245C8}">
       <text>
         <r>
           <rPr>
@@ -487,7 +487,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J65" authorId="0" shapeId="0" xr:uid="{1E79EA93-14E0-B04C-A055-D78ED923C5A8}">
+    <comment ref="J68" authorId="0" shapeId="0" xr:uid="{1E79EA93-14E0-B04C-A055-D78ED923C5A8}">
       <text>
         <r>
           <rPr>
@@ -521,7 +521,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G78" authorId="0" shapeId="0" xr:uid="{71F67876-4BF6-B74C-B26A-D8CAA12F0C78}">
+    <comment ref="G81" authorId="0" shapeId="0" xr:uid="{71F67876-4BF6-B74C-B26A-D8CAA12F0C78}">
       <text>
         <r>
           <rPr>
@@ -555,7 +555,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H78" authorId="0" shapeId="0" xr:uid="{4D6B1231-8CC0-D04A-B5AD-19FA4DA52AA7}">
+    <comment ref="H81" authorId="0" shapeId="0" xr:uid="{4D6B1231-8CC0-D04A-B5AD-19FA4DA52AA7}">
       <text>
         <r>
           <rPr>
@@ -589,7 +589,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I78" authorId="0" shapeId="0" xr:uid="{9DEF9132-BAF9-EB48-97E0-AEDD75448B07}">
+    <comment ref="I81" authorId="0" shapeId="0" xr:uid="{9DEF9132-BAF9-EB48-97E0-AEDD75448B07}">
       <text>
         <r>
           <rPr>
@@ -623,7 +623,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J78" authorId="0" shapeId="0" xr:uid="{03F7C2E3-9A1D-C249-B6CD-319904017587}">
+    <comment ref="J81" authorId="0" shapeId="0" xr:uid="{03F7C2E3-9A1D-C249-B6CD-319904017587}">
       <text>
         <r>
           <rPr>
@@ -657,7 +657,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G88" authorId="0" shapeId="0" xr:uid="{3BD17A23-83C4-604A-AD23-1AA339A3D720}">
+    <comment ref="G91" authorId="0" shapeId="0" xr:uid="{3BD17A23-83C4-604A-AD23-1AA339A3D720}">
       <text>
         <r>
           <rPr>
@@ -691,7 +691,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H88" authorId="0" shapeId="0" xr:uid="{28047719-6EC6-1649-9D9F-E1C477BFD5C4}">
+    <comment ref="H91" authorId="0" shapeId="0" xr:uid="{28047719-6EC6-1649-9D9F-E1C477BFD5C4}">
       <text>
         <r>
           <rPr>
@@ -725,7 +725,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I88" authorId="0" shapeId="0" xr:uid="{C9FF1048-F445-8345-A48F-26C90488913A}">
+    <comment ref="I91" authorId="0" shapeId="0" xr:uid="{C9FF1048-F445-8345-A48F-26C90488913A}">
       <text>
         <r>
           <rPr>
@@ -759,7 +759,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J88" authorId="0" shapeId="0" xr:uid="{C2C3FA2E-6CBA-184E-B7B2-FE9B44C0C759}">
+    <comment ref="J91" authorId="0" shapeId="0" xr:uid="{C2C3FA2E-6CBA-184E-B7B2-FE9B44C0C759}">
       <text>
         <r>
           <rPr>
@@ -793,7 +793,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G98" authorId="0" shapeId="0" xr:uid="{143D5E85-2867-9142-85ED-6738BEE06115}">
+    <comment ref="G101" authorId="0" shapeId="0" xr:uid="{143D5E85-2867-9142-85ED-6738BEE06115}">
       <text>
         <r>
           <rPr>
@@ -827,7 +827,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H98" authorId="0" shapeId="0" xr:uid="{8F34C43E-56F7-7741-9B61-E34D065CD3D4}">
+    <comment ref="H101" authorId="0" shapeId="0" xr:uid="{8F34C43E-56F7-7741-9B61-E34D065CD3D4}">
       <text>
         <r>
           <rPr>
@@ -861,7 +861,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I98" authorId="0" shapeId="0" xr:uid="{CD6E378D-5C31-C545-A6BA-7DE0BEE69313}">
+    <comment ref="I101" authorId="0" shapeId="0" xr:uid="{CD6E378D-5C31-C545-A6BA-7DE0BEE69313}">
       <text>
         <r>
           <rPr>
@@ -895,7 +895,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J98" authorId="0" shapeId="0" xr:uid="{759259CF-9674-2B4D-ADAE-1BBF2503E222}">
+    <comment ref="J101" authorId="0" shapeId="0" xr:uid="{759259CF-9674-2B4D-ADAE-1BBF2503E222}">
       <text>
         <r>
           <rPr>
@@ -934,6 +934,105 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Birmingham, Amanda</author>
+  </authors>
+  <commentList>
+    <comment ref="E16" authorId="0" shapeId="0" xr:uid="{25A23DB9-E441-2B48-ABD9-94C8E8E6F68C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Birmingham, Amanda:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">This is (only) the portion of the syndna pool mass that can actually contribute to the read counts
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Birmingham, Amanda</author>
+  </authors>
+  <commentList>
+    <comment ref="E16" authorId="0" shapeId="0" xr:uid="{BBFF4746-A725-7F41-8854-A4F0971FA4CE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Birmingham, Amanda:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>This is (only) the portion of the syndna pool mass that can actually contribute to the read counts</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Birmingham, Amanda</author>
@@ -2138,7 +2237,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1642" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1657" uniqueCount="320">
   <si>
     <t>variable name</t>
   </si>
@@ -3071,6 +3170,33 @@
   </si>
   <si>
     <t>* below tables are same as above except that values with asterisk are taken directly from "full calcs on correct masses" worksheet rather than calculated on this sheet. Note the match to values calculated here.</t>
+  </si>
+  <si>
+    <t>syndna_factor</t>
+  </si>
+  <si>
+    <t>the factor by which the gdna mass is multiplied to get the amount of syndna pool added.  Note that the syndna amount is added *in addition* to the gdna amount, so if the gdna amount is 5 ng and the syndna factor is 1/20 (0.05) then the added syndna is 5 ng * 0.05 = 0.25 ng and the *total* amount of mass in the well after syndna addition is 5.25 ng</t>
+  </si>
+  <si>
+    <t>syndna_contributing_fraction</t>
+  </si>
+  <si>
+    <t>len(syndna insert) in bp/len(entire syndna plasmid including insert) in bp</t>
+  </si>
+  <si>
+    <t>this represents the fraction of the syndna pool mass that can actually contribute to the reads used to fit the model (since only reads hitting the insert part of the plasmid are used). A shearing factor can additionally be included here for long plasmids if found necessary in the protocol.</t>
+  </si>
+  <si>
+    <t>calc_contributing_mass_syndna_pool_ng</t>
+  </si>
+  <si>
+    <t>calc_mass_normalized_gdna_ng * syndna_factor</t>
+  </si>
+  <si>
+    <t>example3 (same as example1 except for lower vol_elute_ul, higher density_gdna_at_quantitation_ng_ul, higher syndna_factor, lower syndna_contributing_fraction)</t>
+  </si>
+  <si>
+    <t>mass_syndna_pool_ng</t>
   </si>
 </sst>
 </file>
@@ -3150,7 +3276,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3184,6 +3310,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFBAD3AA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA2A5FF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3387,9 +3519,9 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="170" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3399,6 +3531,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFA2A5FF"/>
       <color rgb="FFBAD3AA"/>
     </mruColors>
   </colors>
@@ -4506,6 +4639,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
@@ -4803,11 +4940,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA83768D-892A-3A42-8EA4-41D4B20C5948}">
-  <dimension ref="A1:M106"/>
+  <dimension ref="A1:M109"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G34" sqref="G34"/>
+      <pane ySplit="2" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="G37" sqref="G37"/>
+      <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4854,7 +4992,7 @@
         <v>79</v>
       </c>
       <c r="I3" t="s">
-        <v>177</v>
+        <v>318</v>
       </c>
       <c r="J3" t="s">
         <v>178</v>
@@ -5673,7 +5811,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" ht="14" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>4</v>
       </c>
@@ -5711,7 +5849,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" ht="1" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>4</v>
       </c>
@@ -6184,293 +6322,296 @@
         <v>51</v>
       </c>
       <c r="C37" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D37" t="s">
+        <v>311</v>
+      </c>
+      <c r="E37" t="s">
+        <v>8</v>
+      </c>
+      <c r="F37" t="s">
+        <v>46</v>
+      </c>
+      <c r="G37" s="54">
+        <v>0.05</v>
+      </c>
+      <c r="H37" s="54">
+        <v>0.05</v>
+      </c>
+      <c r="I37" s="54">
+        <v>0.125</v>
+      </c>
+      <c r="J37" s="54">
+        <v>0.05</v>
+      </c>
+      <c r="K37" t="b">
+        <v>1</v>
+      </c>
+      <c r="M37" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="2">
+        <v>9</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C38" t="b">
+        <v>1</v>
+      </c>
+      <c r="D38" t="s">
         <v>55</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E38" t="s">
         <v>13</v>
       </c>
-      <c r="F37" t="s">
+      <c r="F38" t="s">
         <v>44</v>
       </c>
-      <c r="G37">
-        <f>G34/20</f>
+      <c r="G38">
+        <f>G34*G37</f>
         <v>0.25</v>
       </c>
-      <c r="H37">
-        <f>H34/20</f>
+      <c r="H38">
+        <f t="shared" ref="H38:J38" si="0">H34*H37</f>
         <v>0.23799999999999999</v>
       </c>
-      <c r="I37">
-        <f>I34/20</f>
+      <c r="I38" s="55">
+        <f t="shared" si="0"/>
+        <v>0.625</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="0"/>
+        <v>0.23799999999999999</v>
+      </c>
+      <c r="K38" t="b">
+        <v>0</v>
+      </c>
+      <c r="L38" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A39" s="2">
+        <v>9</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C39" t="b">
+        <v>1</v>
+      </c>
+      <c r="D39" t="s">
+        <v>313</v>
+      </c>
+      <c r="E39" t="s">
+        <v>13</v>
+      </c>
+      <c r="F39" t="s">
+        <v>46</v>
+      </c>
+      <c r="G39">
+        <v>1</v>
+      </c>
+      <c r="H39">
+        <v>1</v>
+      </c>
+      <c r="I39" s="55">
+        <v>0.4</v>
+      </c>
+      <c r="J39">
+        <v>1</v>
+      </c>
+      <c r="K39" t="b">
+        <v>0</v>
+      </c>
+      <c r="L39" t="s">
+        <v>314</v>
+      </c>
+      <c r="M39" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A40" s="2">
+        <v>9</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C40" t="b">
+        <v>1</v>
+      </c>
+      <c r="D40" t="s">
+        <v>316</v>
+      </c>
+      <c r="E40" t="s">
+        <v>13</v>
+      </c>
+      <c r="F40" t="s">
+        <v>44</v>
+      </c>
+      <c r="G40">
+        <f>G39*G38</f>
         <v>0.25</v>
       </c>
-      <c r="J37">
-        <f>J34/20</f>
+      <c r="H40">
+        <f t="shared" ref="H40:J40" si="1">H39*H38</f>
         <v>0.23799999999999999</v>
       </c>
-      <c r="K37" t="b">
-        <v>0</v>
-      </c>
-      <c r="L37" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B39" s="2" t="s">
+      <c r="I40">
+        <f t="shared" si="1"/>
+        <v>0.25</v>
+      </c>
+      <c r="J40">
+        <f t="shared" si="1"/>
+        <v>0.23799999999999999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A41" s="2"/>
+      <c r="B41" s="2"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B42" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C39" t="b">
-        <v>1</v>
-      </c>
-      <c r="D39" t="s">
+      <c r="C42" t="b">
+        <v>1</v>
+      </c>
+      <c r="D42" t="s">
         <v>91</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E42" t="s">
         <v>8</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F42" t="s">
         <v>93</v>
       </c>
-      <c r="G39" s="4">
+      <c r="G42" s="4">
         <v>650</v>
       </c>
-      <c r="H39" s="4">
+      <c r="H42" s="4">
         <v>650</v>
       </c>
-      <c r="I39" s="4">
+      <c r="I42" s="4">
         <v>650</v>
       </c>
-      <c r="J39" s="4">
+      <c r="J42" s="4">
         <v>650</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B40" s="2"/>
-      <c r="G40" s="4"/>
-      <c r="H40" s="4"/>
-      <c r="I40" s="4"/>
-      <c r="J40" s="4"/>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B41" s="2"/>
-      <c r="G41" t="s">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B43" s="2"/>
+      <c r="G43" s="4"/>
+      <c r="H43" s="4"/>
+      <c r="I43" s="4"/>
+      <c r="J43" s="4"/>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B44" s="2"/>
+      <c r="G44" t="s">
         <v>255</v>
       </c>
-      <c r="H41" t="s">
+      <c r="H44" t="s">
         <v>256</v>
       </c>
-      <c r="I41" t="s">
+      <c r="I44" t="s">
         <v>177</v>
       </c>
-      <c r="J41" t="s">
+      <c r="J44" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="G42" t="s">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="G45" t="s">
         <v>195</v>
       </c>
-      <c r="H42" t="s">
+      <c r="H45" t="s">
         <v>195</v>
       </c>
-      <c r="I42" t="s">
+      <c r="I45" t="s">
         <v>195</v>
       </c>
-      <c r="J42" t="s">
+      <c r="J45" t="s">
         <v>195</v>
       </c>
-      <c r="L42" t="s">
+      <c r="L45" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B43" s="2" t="s">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B46" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C43" t="b">
-        <v>1</v>
-      </c>
-      <c r="D43" t="s">
+      <c r="C46" t="b">
+        <v>1</v>
+      </c>
+      <c r="D46" t="s">
         <v>88</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E46" t="s">
         <v>8</v>
       </c>
-      <c r="F43" t="s">
+      <c r="F46" t="s">
         <v>89</v>
       </c>
-      <c r="G43" s="43">
+      <c r="G46" s="43">
         <v>6.0220000000000003E+23</v>
       </c>
-      <c r="H43" s="43">
+      <c r="H46" s="43">
         <v>6.0220000000000003E+23</v>
       </c>
-      <c r="I43" s="43">
+      <c r="I46" s="43">
         <v>6.0220000000000003E+23</v>
       </c>
-      <c r="J43" s="43">
+      <c r="J46" s="43">
         <v>6.0220000000000003E+23</v>
       </c>
-      <c r="M43" t="s">
+      <c r="M46" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B44" s="6" t="s">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B47" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="C44" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="D44" s="7" t="s">
+      <c r="C47" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D47" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="E44" s="7" t="s">
+      <c r="E47" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F44" s="7" t="s">
+      <c r="F47" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="G44" s="7">
+      <c r="G47" s="7">
         <f>'linear regressions counts'!M42</f>
         <v>5.5906776314467152E-2</v>
       </c>
-      <c r="H44" s="7">
+      <c r="H47" s="7">
         <f>'linear regressions counts'!M65</f>
         <v>4.5983249626623479E-2</v>
       </c>
-      <c r="I44" s="7">
+      <c r="I47" s="7">
         <f>'linear regressions counts'!M42</f>
         <v>5.5906776314467152E-2</v>
       </c>
-      <c r="J44" s="7">
+      <c r="J47" s="7">
         <f>'linear regressions counts'!M65</f>
         <v>4.5983249626623479E-2</v>
       </c>
-      <c r="K44" t="b">
-        <v>1</v>
-      </c>
-      <c r="L44" t="s">
+      <c r="K47" t="b">
+        <v>1</v>
+      </c>
+      <c r="L47" t="s">
         <v>257</v>
-      </c>
-      <c r="M44" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B45" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="C45" t="b">
-        <v>1</v>
-      </c>
-      <c r="D45" t="s">
-        <v>85</v>
-      </c>
-      <c r="E45" t="s">
-        <v>8</v>
-      </c>
-      <c r="F45" t="s">
-        <v>84</v>
-      </c>
-      <c r="G45">
-        <v>1904788.3330000001</v>
-      </c>
-      <c r="H45">
-        <v>1904788.3330000001</v>
-      </c>
-      <c r="I45">
-        <v>1904788.3330000001</v>
-      </c>
-      <c r="J45">
-        <v>1904788.3330000001</v>
-      </c>
-      <c r="K45" t="b">
-        <v>1</v>
-      </c>
-      <c r="M45" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B46" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="C46" t="b">
-        <v>1</v>
-      </c>
-      <c r="D46" t="s">
-        <v>86</v>
-      </c>
-      <c r="E46" t="s">
-        <v>13</v>
-      </c>
-      <c r="F46" t="s">
-        <v>87</v>
-      </c>
-      <c r="G46" s="5">
-        <f>(G44*G$43)/(G45*G$39*10^9)</f>
-        <v>27192.248659539819</v>
-      </c>
-      <c r="H46" s="5">
-        <f>(H44*H43)/(H45*H39*10^9)</f>
-        <v>22365.588582457232</v>
-      </c>
-      <c r="I46" s="11">
-        <f>(I44*I43)/(I45*I39*10^9)</f>
-        <v>27192.248659539819</v>
-      </c>
-      <c r="J46" s="5">
-        <f>(J44*J43)/(J45*J39*10^9)</f>
-        <v>22365.588582457232</v>
-      </c>
-      <c r="K46" t="b">
-        <v>1</v>
-      </c>
-      <c r="L46" t="s">
-        <v>94</v>
-      </c>
-      <c r="M46" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B47" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="C47" t="b">
-        <v>1</v>
-      </c>
-      <c r="D47" t="s">
-        <v>95</v>
-      </c>
-      <c r="E47" t="s">
-        <v>13</v>
-      </c>
-      <c r="F47" t="s">
-        <v>96</v>
-      </c>
-      <c r="G47">
-        <f>G46/G$34</f>
-        <v>5438.4497319079637</v>
-      </c>
-      <c r="H47">
-        <f>H46/H34</f>
-        <v>4698.6530635414356</v>
-      </c>
-      <c r="I47" s="10">
-        <f>I46/I34</f>
-        <v>5438.4497319079637</v>
-      </c>
-      <c r="J47">
-        <f>J46/J34</f>
-        <v>4698.6530635414356</v>
-      </c>
-      <c r="L47" t="s">
-        <v>97</v>
       </c>
       <c r="M47" t="s">
         <v>104</v>
@@ -6484,32 +6625,28 @@
         <v>1</v>
       </c>
       <c r="D48" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="E48" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="F48" t="s">
-        <v>99</v>
-      </c>
-      <c r="G48" s="27">
-        <f>G47*10^9</f>
-        <v>5438449731907.9639</v>
-      </c>
-      <c r="H48" s="27">
-        <f>H47*10^9</f>
-        <v>4698653063541.4355</v>
-      </c>
-      <c r="I48" s="28">
-        <f>I47*10^9</f>
-        <v>5438449731907.9639</v>
-      </c>
-      <c r="J48" s="27">
-        <f>J47*10^9</f>
-        <v>4698653063541.4355</v>
-      </c>
-      <c r="L48" t="s">
-        <v>100</v>
+        <v>84</v>
+      </c>
+      <c r="G48">
+        <v>1904788.3330000001</v>
+      </c>
+      <c r="H48">
+        <v>1904788.3330000001</v>
+      </c>
+      <c r="I48">
+        <v>1904788.3330000001</v>
+      </c>
+      <c r="J48">
+        <v>1904788.3330000001</v>
+      </c>
+      <c r="K48" t="b">
+        <v>1</v>
       </c>
       <c r="M48" t="s">
         <v>104</v>
@@ -6523,35 +6660,38 @@
         <v>1</v>
       </c>
       <c r="D49" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="E49" t="s">
         <v>13</v>
       </c>
       <c r="F49" t="s">
-        <v>102</v>
-      </c>
-      <c r="G49" s="4">
-        <f>G48*G$29</f>
-        <v>39084741.271463379</v>
-      </c>
-      <c r="H49" s="4">
-        <f>H48*H29</f>
-        <v>22304970.753461108</v>
-      </c>
-      <c r="I49" s="10">
-        <f>I48*I29</f>
-        <v>82077956.670073092</v>
-      </c>
-      <c r="J49" s="4">
-        <f>J48*J29</f>
-        <v>15613479.527422776</v>
+        <v>87</v>
+      </c>
+      <c r="G49" s="5">
+        <f>(G47*G$46)/(G48*G$42*10^9)</f>
+        <v>27192.248659539819</v>
+      </c>
+      <c r="H49" s="5">
+        <f>(H47*H46)/(H48*H42*10^9)</f>
+        <v>22365.588582457232</v>
+      </c>
+      <c r="I49" s="11">
+        <f>(I47*I46)/(I48*I42*10^9)</f>
+        <v>27192.248659539819</v>
+      </c>
+      <c r="J49" s="5">
+        <f>(J47*J46)/(J48*J42*10^9)</f>
+        <v>22365.588582457232</v>
+      </c>
+      <c r="K49" t="b">
+        <v>1</v>
       </c>
       <c r="L49" t="s">
-        <v>274</v>
+        <v>94</v>
       </c>
       <c r="M49" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
     </row>
     <row r="50" spans="2:13" x14ac:dyDescent="0.2">
@@ -6562,225 +6702,247 @@
         <v>1</v>
       </c>
       <c r="D50" t="s">
-        <v>270</v>
+        <v>95</v>
       </c>
       <c r="E50" t="s">
         <v>13</v>
       </c>
       <c r="F50" t="s">
-        <v>271</v>
-      </c>
-      <c r="G50" s="4">
-        <f>G48*G$30</f>
-        <v>5438.4497319079646</v>
-      </c>
-      <c r="H50" s="4">
-        <f>H48*H30</f>
-        <v>4385.409525972007</v>
-      </c>
-      <c r="I50" s="4">
-        <f>I48*I30</f>
-        <v>11420.744437006726</v>
-      </c>
-      <c r="J50" s="4">
-        <f>J48*J30</f>
-        <v>3069.7866681804048</v>
+        <v>96</v>
+      </c>
+      <c r="G50">
+        <f>G49/G$34</f>
+        <v>5438.4497319079637</v>
+      </c>
+      <c r="H50">
+        <f>H49/H34</f>
+        <v>4698.6530635414356</v>
+      </c>
+      <c r="I50" s="10">
+        <f>I49/I34</f>
+        <v>5438.4497319079637</v>
+      </c>
+      <c r="J50">
+        <f>J49/J34</f>
+        <v>4698.6530635414356</v>
       </c>
       <c r="L50" t="s">
-        <v>275</v>
+        <v>97</v>
       </c>
       <c r="M50" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="51" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B51" s="12" t="s">
+      <c r="B51" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="C51" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="D51" s="13" t="s">
-        <v>272</v>
-      </c>
-      <c r="E51" s="13" t="s">
+      <c r="C51" t="b">
+        <v>1</v>
+      </c>
+      <c r="D51" t="s">
+        <v>98</v>
+      </c>
+      <c r="E51" t="s">
         <v>13</v>
       </c>
-      <c r="F51" s="13" t="s">
-        <v>273</v>
-      </c>
-      <c r="G51" s="36">
-        <f>G48*G$31</f>
-        <v>271922.48659539822</v>
-      </c>
-      <c r="H51" s="36">
-        <f>H48*H$31</f>
-        <v>109635.23814930016</v>
-      </c>
-      <c r="I51" s="36">
-        <f>I48*I$31</f>
-        <v>571037.22185033618</v>
-      </c>
-      <c r="J51" s="36">
-        <f>J48*J$31</f>
-        <v>76744.66670451012</v>
+      <c r="F51" t="s">
+        <v>99</v>
+      </c>
+      <c r="G51" s="27">
+        <f>G50*10^9</f>
+        <v>5438449731907.9639</v>
+      </c>
+      <c r="H51" s="27">
+        <f>H50*10^9</f>
+        <v>4698653063541.4355</v>
+      </c>
+      <c r="I51" s="28">
+        <f>I50*10^9</f>
+        <v>5438449731907.9639</v>
+      </c>
+      <c r="J51" s="27">
+        <f>J50*10^9</f>
+        <v>4698653063541.4355</v>
       </c>
       <c r="L51" t="s">
-        <v>276</v>
+        <v>100</v>
       </c>
       <c r="M51" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="52" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="G52" s="4"/>
-      <c r="H52" s="4"/>
-      <c r="I52" s="4"/>
-      <c r="J52" s="4"/>
+      <c r="B52" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C52" t="b">
+        <v>1</v>
+      </c>
+      <c r="D52" t="s">
+        <v>101</v>
+      </c>
+      <c r="E52" t="s">
+        <v>13</v>
+      </c>
+      <c r="F52" t="s">
+        <v>102</v>
+      </c>
+      <c r="G52" s="4">
+        <f>G51*G$29</f>
+        <v>39084741.271463379</v>
+      </c>
+      <c r="H52" s="4">
+        <f>H51*H29</f>
+        <v>22304970.753461108</v>
+      </c>
+      <c r="I52" s="10">
+        <f>I51*I29</f>
+        <v>82077956.670073092</v>
+      </c>
+      <c r="J52" s="4">
+        <f>J51*J29</f>
+        <v>15613479.527422776</v>
+      </c>
+      <c r="L52" t="s">
+        <v>274</v>
+      </c>
+      <c r="M52" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="53" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="G53" s="4" t="s">
+      <c r="B53" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C53" t="b">
+        <v>1</v>
+      </c>
+      <c r="D53" t="s">
+        <v>270</v>
+      </c>
+      <c r="E53" t="s">
+        <v>13</v>
+      </c>
+      <c r="F53" t="s">
+        <v>271</v>
+      </c>
+      <c r="G53" s="4">
+        <f>G51*G$30</f>
+        <v>5438.4497319079646</v>
+      </c>
+      <c r="H53" s="4">
+        <f>H51*H30</f>
+        <v>4385.409525972007</v>
+      </c>
+      <c r="I53" s="4">
+        <f>I51*I30</f>
+        <v>11420.744437006726</v>
+      </c>
+      <c r="J53" s="4">
+        <f>J51*J30</f>
+        <v>3069.7866681804048</v>
+      </c>
+      <c r="L53" t="s">
+        <v>275</v>
+      </c>
+      <c r="M53" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="54" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B54" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C54" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="D54" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="E54" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F54" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="G54" s="36">
+        <f>G51*G$31</f>
+        <v>271922.48659539822</v>
+      </c>
+      <c r="H54" s="36">
+        <f>H51*H$31</f>
+        <v>109635.23814930016</v>
+      </c>
+      <c r="I54" s="36">
+        <f>I51*I$31</f>
+        <v>571037.22185033618</v>
+      </c>
+      <c r="J54" s="36">
+        <f>J51*J$31</f>
+        <v>76744.66670451012</v>
+      </c>
+      <c r="L54" t="s">
+        <v>276</v>
+      </c>
+      <c r="M54" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="55" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="G55" s="4"/>
+      <c r="H55" s="4"/>
+      <c r="I55" s="4"/>
+      <c r="J55" s="4"/>
+    </row>
+    <row r="56" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="G56" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="H53" s="4" t="s">
+      <c r="H56" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="I53" s="4" t="s">
+      <c r="I56" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="J53" s="4" t="s">
+      <c r="J56" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="L53" s="2" t="s">
+      <c r="L56" s="2" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="54" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B54" s="2" t="s">
+    <row r="57" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B57" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C54" t="b">
-        <v>1</v>
-      </c>
-      <c r="D54" t="s">
+      <c r="C57" t="b">
+        <v>1</v>
+      </c>
+      <c r="D57" t="s">
         <v>83</v>
       </c>
-      <c r="E54" t="s">
+      <c r="E57" t="s">
         <v>13</v>
       </c>
-      <c r="F54" t="s">
+      <c r="F57" t="s">
         <v>44</v>
       </c>
-      <c r="G54">
+      <c r="G57">
         <f>'linear regressions counts'!M43</f>
         <v>6.7506893569518861E-2</v>
       </c>
-      <c r="H54">
+      <c r="H57">
         <f>'linear regressions counts'!M66</f>
         <v>5.5539298723601756E-2</v>
       </c>
-      <c r="I54">
+      <c r="I57">
         <f>'linear regressions counts'!M43</f>
         <v>6.7506893569518861E-2</v>
       </c>
-      <c r="J54">
+      <c r="J57">
         <f>'linear regressions counts'!M66</f>
         <v>5.5539298723601756E-2</v>
-      </c>
-    </row>
-    <row r="55" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B55" t="s">
-        <v>82</v>
-      </c>
-      <c r="C55" t="b">
-        <v>1</v>
-      </c>
-      <c r="D55" t="s">
-        <v>85</v>
-      </c>
-      <c r="E55" t="s">
-        <v>8</v>
-      </c>
-      <c r="F55" t="s">
-        <v>84</v>
-      </c>
-      <c r="G55">
-        <v>4373730</v>
-      </c>
-      <c r="H55">
-        <v>4373730</v>
-      </c>
-      <c r="I55">
-        <v>4373730</v>
-      </c>
-      <c r="J55">
-        <v>4373730</v>
-      </c>
-    </row>
-    <row r="56" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B56" t="s">
-        <v>82</v>
-      </c>
-      <c r="C56" t="b">
-        <v>1</v>
-      </c>
-      <c r="D56" t="s">
-        <v>86</v>
-      </c>
-      <c r="E56" t="s">
-        <v>13</v>
-      </c>
-      <c r="F56" t="s">
-        <v>87</v>
-      </c>
-      <c r="G56" s="5">
-        <f>(G54*G$43)/(G55*G$39*10^9)</f>
-        <v>14299.588788785724</v>
-      </c>
-      <c r="H56" s="5">
-        <f>(H54*H$43)/(H55*H$39*10^9)</f>
-        <v>11764.563459688423</v>
-      </c>
-      <c r="I56" s="5">
-        <f>(I54*I$43)/(I55*I$39*10^9)</f>
-        <v>14299.588788785724</v>
-      </c>
-      <c r="J56" s="5">
-        <f>(J54*J$43)/(J55*J$39*10^9)</f>
-        <v>11764.563459688423</v>
-      </c>
-    </row>
-    <row r="57" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B57" t="s">
-        <v>82</v>
-      </c>
-      <c r="C57" t="b">
-        <v>1</v>
-      </c>
-      <c r="D57" t="s">
-        <v>95</v>
-      </c>
-      <c r="E57" t="s">
-        <v>13</v>
-      </c>
-      <c r="F57" t="s">
-        <v>96</v>
-      </c>
-      <c r="G57">
-        <f>G56/G$34</f>
-        <v>2859.917757757145</v>
-      </c>
-      <c r="H57">
-        <f>H56/H$34</f>
-        <v>2471.5469453126939</v>
-      </c>
-      <c r="I57">
-        <f>I56/I$34</f>
-        <v>2859.917757757145</v>
-      </c>
-      <c r="J57">
-        <f>J56/J$34</f>
-        <v>2471.5469453126939</v>
       </c>
     </row>
     <row r="58" spans="2:13" x14ac:dyDescent="0.2">
@@ -6791,29 +6953,25 @@
         <v>1</v>
       </c>
       <c r="D58" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="E58" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="F58" t="s">
-        <v>99</v>
-      </c>
-      <c r="G58" s="27">
-        <f>G57*10^9</f>
-        <v>2859917757757.145</v>
-      </c>
-      <c r="H58" s="27">
-        <f>H57*10^9</f>
-        <v>2471546945312.6938</v>
-      </c>
-      <c r="I58" s="27">
-        <f>I57*10^9</f>
-        <v>2859917757757.145</v>
-      </c>
-      <c r="J58" s="27">
-        <f>J57*10^9</f>
-        <v>2471546945312.6938</v>
+        <v>84</v>
+      </c>
+      <c r="G58">
+        <v>4373730</v>
+      </c>
+      <c r="H58">
+        <v>4373730</v>
+      </c>
+      <c r="I58">
+        <v>4373730</v>
+      </c>
+      <c r="J58">
+        <v>4373730</v>
       </c>
     </row>
     <row r="59" spans="2:13" x14ac:dyDescent="0.2">
@@ -6824,29 +6982,29 @@
         <v>1</v>
       </c>
       <c r="D59" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="E59" t="s">
         <v>13</v>
       </c>
       <c r="F59" t="s">
-        <v>102</v>
-      </c>
-      <c r="G59" s="4">
-        <f>G58*G$29</f>
-        <v>20553494.30992835</v>
-      </c>
-      <c r="H59" s="4">
-        <f>H58*H$29</f>
-        <v>11732677.766477879</v>
-      </c>
-      <c r="I59" s="4">
-        <f>I58*I$29</f>
-        <v>43162338.050849527</v>
-      </c>
-      <c r="J59" s="4">
-        <f>J58*J$29</f>
-        <v>8212874.4365345165</v>
+        <v>87</v>
+      </c>
+      <c r="G59" s="5">
+        <f>(G57*G$46)/(G58*G$42*10^9)</f>
+        <v>14299.588788785724</v>
+      </c>
+      <c r="H59" s="5">
+        <f>(H57*H$46)/(H58*H$42*10^9)</f>
+        <v>11764.563459688423</v>
+      </c>
+      <c r="I59" s="5">
+        <f>(I57*I$46)/(I58*I$42*10^9)</f>
+        <v>14299.588788785724</v>
+      </c>
+      <c r="J59" s="5">
+        <f>(J57*J$46)/(J58*J$42*10^9)</f>
+        <v>11764.563459688423</v>
       </c>
     </row>
     <row r="60" spans="2:13" x14ac:dyDescent="0.2">
@@ -6857,29 +7015,29 @@
         <v>1</v>
       </c>
       <c r="D60" t="s">
-        <v>270</v>
+        <v>95</v>
       </c>
       <c r="E60" t="s">
         <v>13</v>
       </c>
       <c r="F60" t="s">
-        <v>271</v>
-      </c>
-      <c r="G60" s="4">
-        <f>G58*G$30</f>
-        <v>2859.9177577571454</v>
-      </c>
-      <c r="H60" s="4">
-        <f>H58*H$30</f>
-        <v>2306.7771489585143</v>
-      </c>
-      <c r="I60" s="4">
-        <f>I58*I$30</f>
-        <v>6005.8272912900047</v>
-      </c>
-      <c r="J60" s="4">
-        <f>J58*J$30</f>
-        <v>1614.74400427096</v>
+        <v>96</v>
+      </c>
+      <c r="G60">
+        <f>G59/G$34</f>
+        <v>2859.917757757145</v>
+      </c>
+      <c r="H60">
+        <f>H59/H$34</f>
+        <v>2471.5469453126939</v>
+      </c>
+      <c r="I60">
+        <f>I59/I$34</f>
+        <v>2859.917757757145</v>
+      </c>
+      <c r="J60">
+        <f>J59/J$34</f>
+        <v>2471.5469453126939</v>
       </c>
     </row>
     <row r="61" spans="2:13" x14ac:dyDescent="0.2">
@@ -6890,180 +7048,184 @@
         <v>1</v>
       </c>
       <c r="D61" t="s">
-        <v>272</v>
+        <v>98</v>
       </c>
       <c r="E61" t="s">
         <v>13</v>
       </c>
       <c r="F61" t="s">
+        <v>99</v>
+      </c>
+      <c r="G61" s="27">
+        <f>G60*10^9</f>
+        <v>2859917757757.145</v>
+      </c>
+      <c r="H61" s="27">
+        <f>H60*10^9</f>
+        <v>2471546945312.6938</v>
+      </c>
+      <c r="I61" s="27">
+        <f>I60*10^9</f>
+        <v>2859917757757.145</v>
+      </c>
+      <c r="J61" s="27">
+        <f>J60*10^9</f>
+        <v>2471546945312.6938</v>
+      </c>
+    </row>
+    <row r="62" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B62" t="s">
+        <v>82</v>
+      </c>
+      <c r="C62" t="b">
+        <v>1</v>
+      </c>
+      <c r="D62" t="s">
+        <v>101</v>
+      </c>
+      <c r="E62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F62" t="s">
+        <v>102</v>
+      </c>
+      <c r="G62" s="4">
+        <f>G61*G$29</f>
+        <v>20553494.30992835</v>
+      </c>
+      <c r="H62" s="4">
+        <f>H61*H$29</f>
+        <v>11732677.766477879</v>
+      </c>
+      <c r="I62" s="4">
+        <f>I61*I$29</f>
+        <v>43162338.050849527</v>
+      </c>
+      <c r="J62" s="4">
+        <f>J61*J$29</f>
+        <v>8212874.4365345165</v>
+      </c>
+    </row>
+    <row r="63" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B63" t="s">
+        <v>82</v>
+      </c>
+      <c r="C63" t="b">
+        <v>1</v>
+      </c>
+      <c r="D63" t="s">
+        <v>270</v>
+      </c>
+      <c r="E63" t="s">
+        <v>13</v>
+      </c>
+      <c r="F63" t="s">
+        <v>271</v>
+      </c>
+      <c r="G63" s="4">
+        <f>G61*G$30</f>
+        <v>2859.9177577571454</v>
+      </c>
+      <c r="H63" s="4">
+        <f>H61*H$30</f>
+        <v>2306.7771489585143</v>
+      </c>
+      <c r="I63" s="4">
+        <f>I61*I$30</f>
+        <v>6005.8272912900047</v>
+      </c>
+      <c r="J63" s="4">
+        <f>J61*J$30</f>
+        <v>1614.74400427096</v>
+      </c>
+    </row>
+    <row r="64" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B64" t="s">
+        <v>82</v>
+      </c>
+      <c r="C64" t="b">
+        <v>1</v>
+      </c>
+      <c r="D64" t="s">
+        <v>272</v>
+      </c>
+      <c r="E64" t="s">
+        <v>13</v>
+      </c>
+      <c r="F64" t="s">
         <v>273</v>
       </c>
-      <c r="G61" s="4">
-        <f>G58*G$31</f>
+      <c r="G64" s="4">
+        <f>G61*G$31</f>
         <v>142995.88788785727</v>
       </c>
-      <c r="H61" s="4">
-        <f>H58*H$31</f>
+      <c r="H64" s="4">
+        <f>H61*H$31</f>
         <v>57669.428723962861</v>
       </c>
-      <c r="I61" s="4">
-        <f>I58*I$31</f>
+      <c r="I64" s="4">
+        <f>I61*I$31</f>
         <v>300291.36456450023</v>
       </c>
-      <c r="J61" s="4">
-        <f>J58*J$31</f>
+      <c r="J64" s="4">
+        <f>J61*J$31</f>
         <v>40368.600106774</v>
       </c>
     </row>
-    <row r="62" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="G62" s="4"/>
-      <c r="H62" s="4"/>
-      <c r="I62" s="4"/>
-      <c r="J62" s="4"/>
-    </row>
-    <row r="63" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="G63" s="4" t="s">
+    <row r="65" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="G65" s="4"/>
+      <c r="H65" s="4"/>
+      <c r="I65" s="4"/>
+      <c r="J65" s="4"/>
+    </row>
+    <row r="66" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="G66" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="H63" s="4" t="s">
+      <c r="H66" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="I63" s="4" t="s">
+      <c r="I66" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="J63" s="4" t="s">
+      <c r="J66" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="L63" s="2" t="s">
+      <c r="L66" s="2" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="64" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B64" s="6" t="s">
+    <row r="67" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B67" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="C64" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="D64" s="7" t="s">
+      <c r="C67" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D67" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="E64" s="7" t="s">
+      <c r="E67" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F64" s="7" t="s">
+      <c r="F67" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="G64" s="8">
+      <c r="G67" s="8">
         <f>'linear regressions counts'!M48</f>
         <v>5.5800097113146443E-4</v>
       </c>
-      <c r="H64" s="8">
+      <c r="H67" s="8">
         <f>'linear regressions counts'!M71</f>
         <v>4.5576142039897643E-4</v>
       </c>
-      <c r="I64" s="8">
+      <c r="I67" s="8">
         <f>'linear regressions counts'!M48</f>
         <v>5.5800097113146443E-4</v>
       </c>
-      <c r="J64" s="8">
+      <c r="J67" s="8">
         <f>'linear regressions counts'!M71</f>
         <v>4.5576142039897643E-4</v>
-      </c>
-    </row>
-    <row r="65" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B65" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="C65" t="b">
-        <v>1</v>
-      </c>
-      <c r="D65" t="s">
-        <v>85</v>
-      </c>
-      <c r="E65" t="s">
-        <v>8</v>
-      </c>
-      <c r="F65" t="s">
-        <v>84</v>
-      </c>
-      <c r="G65" s="10">
-        <v>89264</v>
-      </c>
-      <c r="H65" s="10">
-        <v>89264</v>
-      </c>
-      <c r="I65" s="10">
-        <v>89264</v>
-      </c>
-      <c r="J65" s="10">
-        <v>89264</v>
-      </c>
-    </row>
-    <row r="66" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B66" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="C66" t="b">
-        <v>1</v>
-      </c>
-      <c r="D66" t="s">
-        <v>86</v>
-      </c>
-      <c r="E66" t="s">
-        <v>13</v>
-      </c>
-      <c r="F66" t="s">
-        <v>87</v>
-      </c>
-      <c r="G66" s="11">
-        <f>(G64*G$43)/(G65*G$39*10^9)</f>
-        <v>5791.432583992304</v>
-      </c>
-      <c r="H66" s="11">
-        <f>(H64*H$43)/(H65*H$39*10^9)</f>
-        <v>4730.2991879621313</v>
-      </c>
-      <c r="I66" s="11">
-        <f>(I64*I$43)/(I65*I$39*10^9)</f>
-        <v>5791.432583992304</v>
-      </c>
-      <c r="J66" s="11">
-        <f>(J64*J$43)/(J65*J$39*10^9)</f>
-        <v>4730.2991879621313</v>
-      </c>
-    </row>
-    <row r="67" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B67" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="C67" t="b">
-        <v>1</v>
-      </c>
-      <c r="D67" t="s">
-        <v>95</v>
-      </c>
-      <c r="E67" t="s">
-        <v>13</v>
-      </c>
-      <c r="F67" t="s">
-        <v>96</v>
-      </c>
-      <c r="G67" s="10">
-        <f>G66/G$34</f>
-        <v>1158.2865167984608</v>
-      </c>
-      <c r="H67" s="10">
-        <f>H66/H$34</f>
-        <v>993.76033360548979</v>
-      </c>
-      <c r="I67" s="10">
-        <f>I66/I$34</f>
-        <v>1158.2865167984608</v>
-      </c>
-      <c r="J67" s="10">
-        <f>J66/J$34</f>
-        <v>993.76033360548979</v>
       </c>
     </row>
     <row r="68" spans="2:12" x14ac:dyDescent="0.2">
@@ -7074,29 +7236,25 @@
         <v>1</v>
       </c>
       <c r="D68" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="E68" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="F68" t="s">
-        <v>99</v>
-      </c>
-      <c r="G68" s="28">
-        <f>G67*10^9</f>
-        <v>1158286516798.4607</v>
-      </c>
-      <c r="H68" s="28">
-        <f>H67*10^9</f>
-        <v>993760333605.48975</v>
-      </c>
-      <c r="I68" s="28">
-        <f>I67*10^9</f>
-        <v>1158286516798.4607</v>
-      </c>
-      <c r="J68" s="28">
-        <f>J67*10^9</f>
-        <v>993760333605.48975</v>
+        <v>84</v>
+      </c>
+      <c r="G68" s="10">
+        <v>89264</v>
+      </c>
+      <c r="H68" s="10">
+        <v>89264</v>
+      </c>
+      <c r="I68" s="10">
+        <v>89264</v>
+      </c>
+      <c r="J68" s="10">
+        <v>89264</v>
       </c>
     </row>
     <row r="69" spans="2:12" x14ac:dyDescent="0.2">
@@ -7107,29 +7265,29 @@
         <v>1</v>
       </c>
       <c r="D69" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="E69" t="s">
         <v>13</v>
       </c>
       <c r="F69" t="s">
-        <v>102</v>
-      </c>
-      <c r="G69" s="46">
-        <f>G68*G$29</f>
-        <v>8324307.6720339339</v>
-      </c>
-      <c r="H69" s="46">
-        <f>H68*H$29</f>
-        <v>4717478.5789171578</v>
-      </c>
-      <c r="I69" s="46">
-        <f>I68*I$29</f>
-        <v>17481046.111271258</v>
-      </c>
-      <c r="J69" s="46">
-        <f>J68*J$29</f>
-        <v>3302235.005242011</v>
+        <v>87</v>
+      </c>
+      <c r="G69" s="11">
+        <f>(G67*G$46)/(G68*G$42*10^9)</f>
+        <v>5791.432583992304</v>
+      </c>
+      <c r="H69" s="11">
+        <f>(H67*H$46)/(H68*H$42*10^9)</f>
+        <v>4730.2991879621313</v>
+      </c>
+      <c r="I69" s="11">
+        <f>(I67*I$46)/(I68*I$42*10^9)</f>
+        <v>5791.432583992304</v>
+      </c>
+      <c r="J69" s="11">
+        <f>(J67*J$46)/(J68*J$42*10^9)</f>
+        <v>4730.2991879621313</v>
       </c>
     </row>
     <row r="70" spans="2:12" x14ac:dyDescent="0.2">
@@ -7140,264 +7298,266 @@
         <v>1</v>
       </c>
       <c r="D70" t="s">
-        <v>270</v>
+        <v>95</v>
       </c>
       <c r="E70" t="s">
         <v>13</v>
       </c>
       <c r="F70" t="s">
+        <v>96</v>
+      </c>
+      <c r="G70" s="10">
+        <f>G69/G$34</f>
+        <v>1158.2865167984608</v>
+      </c>
+      <c r="H70" s="10">
+        <f>H69/H$34</f>
+        <v>993.76033360548979</v>
+      </c>
+      <c r="I70" s="10">
+        <f>I69/I$34</f>
+        <v>1158.2865167984608</v>
+      </c>
+      <c r="J70" s="10">
+        <f>J69/J$34</f>
+        <v>993.76033360548979</v>
+      </c>
+    </row>
+    <row r="71" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B71" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C71" t="b">
+        <v>1</v>
+      </c>
+      <c r="D71" t="s">
+        <v>98</v>
+      </c>
+      <c r="E71" t="s">
+        <v>13</v>
+      </c>
+      <c r="F71" t="s">
+        <v>99</v>
+      </c>
+      <c r="G71" s="28">
+        <f>G70*10^9</f>
+        <v>1158286516798.4607</v>
+      </c>
+      <c r="H71" s="28">
+        <f>H70*10^9</f>
+        <v>993760333605.48975</v>
+      </c>
+      <c r="I71" s="28">
+        <f>I70*10^9</f>
+        <v>1158286516798.4607</v>
+      </c>
+      <c r="J71" s="28">
+        <f>J70*10^9</f>
+        <v>993760333605.48975</v>
+      </c>
+    </row>
+    <row r="72" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B72" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C72" t="b">
+        <v>1</v>
+      </c>
+      <c r="D72" t="s">
+        <v>101</v>
+      </c>
+      <c r="E72" t="s">
+        <v>13</v>
+      </c>
+      <c r="F72" t="s">
+        <v>102</v>
+      </c>
+      <c r="G72" s="46">
+        <f>G71*G$29</f>
+        <v>8324307.6720339339</v>
+      </c>
+      <c r="H72" s="46">
+        <f>H71*H$29</f>
+        <v>4717478.5789171578</v>
+      </c>
+      <c r="I72" s="46">
+        <f>I71*I$29</f>
+        <v>17481046.111271258</v>
+      </c>
+      <c r="J72" s="46">
+        <f>J71*J$29</f>
+        <v>3302235.005242011</v>
+      </c>
+    </row>
+    <row r="73" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B73" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C73" t="b">
+        <v>1</v>
+      </c>
+      <c r="D73" t="s">
+        <v>270</v>
+      </c>
+      <c r="E73" t="s">
+        <v>13</v>
+      </c>
+      <c r="F73" t="s">
         <v>271</v>
       </c>
-      <c r="G70" s="4">
-        <f>G68*G$30</f>
+      <c r="G73" s="4">
+        <f>G71*G$30</f>
         <v>1158.2865167984608</v>
       </c>
-      <c r="H70" s="4">
-        <f>H68*H$30</f>
+      <c r="H73" s="4">
+        <f>H71*H$30</f>
         <v>927.50964469845724</v>
       </c>
-      <c r="I70" s="4">
-        <f>I68*I$30</f>
+      <c r="I73" s="4">
+        <f>I71*I$30</f>
         <v>2432.4016852767677</v>
       </c>
-      <c r="J70" s="4">
-        <f>J68*J$30</f>
+      <c r="J73" s="4">
+        <f>J71*J$30</f>
         <v>649.25675128891999</v>
       </c>
     </row>
-    <row r="71" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B71" s="12" t="s">
+    <row r="74" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B74" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="C71" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="D71" s="13" t="s">
+      <c r="C74" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="D74" s="13" t="s">
         <v>272</v>
       </c>
-      <c r="E71" s="13" t="s">
+      <c r="E74" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F71" s="13" t="s">
+      <c r="F74" s="13" t="s">
         <v>273</v>
       </c>
-      <c r="G71" s="36">
-        <f>G68*G$31</f>
+      <c r="G74" s="36">
+        <f>G71*G$31</f>
         <v>57914.32583992304</v>
       </c>
-      <c r="H71" s="36">
-        <f>H68*H$31</f>
+      <c r="H74" s="36">
+        <f>H71*H$31</f>
         <v>23187.741117461428</v>
       </c>
-      <c r="I71" s="36">
-        <f>I68*I$31</f>
+      <c r="I74" s="36">
+        <f>I71*I$31</f>
         <v>121620.08426383838</v>
       </c>
-      <c r="J71" s="36">
-        <f>J68*J$31</f>
+      <c r="J74" s="36">
+        <f>J71*J$31</f>
         <v>16231.418782223</v>
       </c>
     </row>
-    <row r="72" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="G72" s="4"/>
-      <c r="H72" s="4"/>
-      <c r="I72" s="4"/>
-      <c r="J72" s="4"/>
-    </row>
-    <row r="73" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="G73" s="4"/>
-      <c r="H73" s="4"/>
-      <c r="I73" s="4"/>
-      <c r="J73" s="4"/>
-    </row>
-    <row r="74" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="G74" t="s">
+    <row r="75" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="G75" s="4"/>
+      <c r="H75" s="4"/>
+      <c r="I75" s="4"/>
+      <c r="J75" s="4"/>
+    </row>
+    <row r="76" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="G76" s="4"/>
+      <c r="H76" s="4"/>
+      <c r="I76" s="4"/>
+      <c r="J76" s="4"/>
+    </row>
+    <row r="77" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="G77" t="s">
         <v>255</v>
       </c>
-      <c r="H74" t="s">
+      <c r="H77" t="s">
         <v>256</v>
       </c>
-      <c r="I74" t="s">
+      <c r="I77" t="s">
         <v>177</v>
       </c>
-      <c r="J74" t="s">
+      <c r="J77" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="75" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="G75" t="s">
+    <row r="78" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="G78" t="s">
         <v>195</v>
       </c>
-      <c r="H75" t="s">
+      <c r="H78" t="s">
         <v>195</v>
       </c>
-      <c r="I75" t="s">
+      <c r="I78" t="s">
         <v>195</v>
       </c>
-      <c r="J75" t="s">
+      <c r="J78" t="s">
         <v>195</v>
       </c>
-      <c r="L75" t="s">
+      <c r="L78" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="76" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B76" s="23" t="s">
+    <row r="79" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B79" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="C76" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="D76" s="19" t="s">
+      <c r="C79" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="D79" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="E76" s="19" t="s">
+      <c r="E79" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="F76" s="19" t="s">
+      <c r="F79" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="G76" s="26">
+      <c r="G79" s="26">
         <v>6.0221407599999999E+23</v>
       </c>
-      <c r="H76" s="26">
+      <c r="H79" s="26">
         <v>6.0221407599999999E+23</v>
       </c>
-      <c r="I76" s="26">
+      <c r="I79" s="26">
         <v>6.0221407599999999E+23</v>
       </c>
-      <c r="J76" s="26">
+      <c r="J79" s="26">
         <v>6.0221407599999999E+23</v>
       </c>
     </row>
-    <row r="77" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B77" s="16" t="s">
+    <row r="80" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B80" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="C77" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="D77" s="17" t="s">
+      <c r="C80" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="D80" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="E77" s="17" t="s">
+      <c r="E80" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="F77" s="17" t="s">
+      <c r="F80" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="G77" s="17">
+      <c r="G80" s="17">
         <f>'linear regressions counts'!M42</f>
         <v>5.5906776314467152E-2</v>
       </c>
-      <c r="H77" s="17">
+      <c r="H80" s="17">
         <f>'linear regressions counts'!M65</f>
         <v>4.5983249626623479E-2</v>
       </c>
-      <c r="I77" s="17">
+      <c r="I80" s="17">
         <f>'linear regressions counts'!M42</f>
         <v>5.5906776314467152E-2</v>
       </c>
-      <c r="J77" s="17">
+      <c r="J80" s="17">
         <f>'linear regressions counts'!M65</f>
         <v>4.5983249626623479E-2</v>
-      </c>
-    </row>
-    <row r="78" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B78" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="C78" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="D78" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="E78" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="F78" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="G78" s="19">
-        <v>1904788.3330000001</v>
-      </c>
-      <c r="H78" s="19">
-        <v>1904788.3330000001</v>
-      </c>
-      <c r="I78" s="19">
-        <v>1904788.3330000001</v>
-      </c>
-      <c r="J78" s="19">
-        <v>1904788.3330000001</v>
-      </c>
-      <c r="L78" s="45"/>
-    </row>
-    <row r="79" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B79" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="C79" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="D79" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="E79" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="F79" s="19" t="s">
-        <v>87</v>
-      </c>
-      <c r="G79" s="20">
-        <f>(G77*G$76)/(G78*G$39*10^9)</f>
-        <v>27192.884259161423</v>
-      </c>
-      <c r="H79" s="20">
-        <f>(H77*H$76)/(H78*H$39*10^9)</f>
-        <v>22366.111362305932</v>
-      </c>
-      <c r="I79" s="20">
-        <f>(I77*I$76)/(I78*I$39*10^9)</f>
-        <v>27192.884259161423</v>
-      </c>
-      <c r="J79" s="20">
-        <f>(J77*J$76)/(J78*J$39*10^9)</f>
-        <v>22366.111362305932</v>
-      </c>
-      <c r="L79" s="45"/>
-    </row>
-    <row r="80" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B80" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="C80" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="D80" s="19" t="s">
-        <v>95</v>
-      </c>
-      <c r="E80" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="F80" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="G80" s="19">
-        <f>G79/G$34</f>
-        <v>5438.5768518322848</v>
-      </c>
-      <c r="H80" s="19">
-        <f>H79/H$34</f>
-        <v>4698.7628912407426</v>
-      </c>
-      <c r="I80" s="19">
-        <f>I79/I$34</f>
-        <v>5438.5768518322848</v>
-      </c>
-      <c r="J80" s="19">
-        <f>J79/J$34</f>
-        <v>4698.7628912407426</v>
       </c>
     </row>
     <row r="81" spans="2:12" x14ac:dyDescent="0.2">
@@ -7408,30 +7568,27 @@
         <v>1</v>
       </c>
       <c r="D81" s="19" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="E81" s="19" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="F81" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="G81" s="33">
-        <f>G80*10^9</f>
-        <v>5438576851832.2852</v>
-      </c>
-      <c r="H81" s="33">
-        <f>H80*10^9</f>
-        <v>4698762891240.7422</v>
-      </c>
-      <c r="I81" s="33">
-        <f>I80*10^9</f>
-        <v>5438576851832.2852</v>
-      </c>
-      <c r="J81" s="33">
-        <f>J80*10^9</f>
-        <v>4698762891240.7422</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="G81" s="19">
+        <v>1904788.3330000001</v>
+      </c>
+      <c r="H81" s="19">
+        <v>1904788.3330000001</v>
+      </c>
+      <c r="I81" s="19">
+        <v>1904788.3330000001</v>
+      </c>
+      <c r="J81" s="19">
+        <v>1904788.3330000001</v>
+      </c>
+      <c r="L81" s="45"/>
     </row>
     <row r="82" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B82" s="18" t="s">
@@ -7441,30 +7598,31 @@
         <v>1</v>
       </c>
       <c r="D82" s="19" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="E82" s="19" t="s">
         <v>13</v>
       </c>
       <c r="F82" s="19" t="s">
-        <v>102</v>
-      </c>
-      <c r="G82" s="39">
-        <f>G81*G$29</f>
-        <v>39085654.849706717</v>
-      </c>
-      <c r="H82" s="39">
-        <f>H81*H$29</f>
-        <v>22305492.116410837</v>
-      </c>
-      <c r="I82" s="39">
-        <f>I81*I$29</f>
-        <v>82079875.184384093</v>
-      </c>
-      <c r="J82" s="39">
-        <f>J81*J$29</f>
-        <v>15613844.481487585</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="G82" s="20">
+        <f>(G80*G$79)/(G81*G$42*10^9)</f>
+        <v>27192.884259161423</v>
+      </c>
+      <c r="H82" s="20">
+        <f>(H80*H$79)/(H81*H$42*10^9)</f>
+        <v>22366.111362305932</v>
+      </c>
+      <c r="I82" s="20">
+        <f>(I80*I$79)/(I81*I$42*10^9)</f>
+        <v>27192.884259161423</v>
+      </c>
+      <c r="J82" s="20">
+        <f>(J80*J$79)/(J81*J$42*10^9)</f>
+        <v>22366.111362305932</v>
+      </c>
+      <c r="L82" s="45"/>
     </row>
     <row r="83" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B83" s="18" t="s">
@@ -7474,213 +7632,217 @@
         <v>1</v>
       </c>
       <c r="D83" s="19" t="s">
-        <v>270</v>
+        <v>95</v>
       </c>
       <c r="E83" s="19" t="s">
         <v>13</v>
       </c>
       <c r="F83" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="G83" s="19">
+        <f>G82/G$34</f>
+        <v>5438.5768518322848</v>
+      </c>
+      <c r="H83" s="19">
+        <f>H82/H$34</f>
+        <v>4698.7628912407426</v>
+      </c>
+      <c r="I83" s="19">
+        <f>I82/I$34</f>
+        <v>5438.5768518322848</v>
+      </c>
+      <c r="J83" s="19">
+        <f>J82/J$34</f>
+        <v>4698.7628912407426</v>
+      </c>
+    </row>
+    <row r="84" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B84" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="C84" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="D84" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="E84" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="F84" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="G84" s="33">
+        <f>G83*10^9</f>
+        <v>5438576851832.2852</v>
+      </c>
+      <c r="H84" s="33">
+        <f>H83*10^9</f>
+        <v>4698762891240.7422</v>
+      </c>
+      <c r="I84" s="33">
+        <f>I83*10^9</f>
+        <v>5438576851832.2852</v>
+      </c>
+      <c r="J84" s="33">
+        <f>J83*10^9</f>
+        <v>4698762891240.7422</v>
+      </c>
+    </row>
+    <row r="85" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B85" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="C85" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="D85" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="E85" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="F85" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="G85" s="39">
+        <f>G84*G$29</f>
+        <v>39085654.849706717</v>
+      </c>
+      <c r="H85" s="39">
+        <f>H84*H$29</f>
+        <v>22305492.116410837</v>
+      </c>
+      <c r="I85" s="39">
+        <f>I84*I$29</f>
+        <v>82079875.184384093</v>
+      </c>
+      <c r="J85" s="39">
+        <f>J84*J$29</f>
+        <v>15613844.481487585</v>
+      </c>
+    </row>
+    <row r="86" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B86" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="C86" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="D86" s="19" t="s">
+        <v>270</v>
+      </c>
+      <c r="E86" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="F86" s="19" t="s">
         <v>271</v>
       </c>
-      <c r="G83" s="39">
-        <f>G81*G$30</f>
+      <c r="G86" s="39">
+        <f>G84*G$30</f>
         <v>5438.5768518322857</v>
       </c>
-      <c r="H83" s="39">
-        <f>H81*H$30</f>
+      <c r="H86" s="39">
+        <f>H84*H$30</f>
         <v>4385.5120318246927</v>
       </c>
-      <c r="I83" s="39">
-        <f>I81*I$30</f>
+      <c r="I86" s="39">
+        <f>I84*I$30</f>
         <v>11421.011388847799</v>
       </c>
-      <c r="J83" s="39">
-        <f>J81*J$30</f>
+      <c r="J86" s="39">
+        <f>J84*J$30</f>
         <v>3069.8584222772852</v>
       </c>
     </row>
-    <row r="84" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B84" s="21" t="s">
+    <row r="87" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B87" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="C84" s="22" t="b">
-        <v>1</v>
-      </c>
-      <c r="D84" s="22" t="s">
+      <c r="C87" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="D87" s="22" t="s">
         <v>272</v>
       </c>
-      <c r="E84" s="22" t="s">
+      <c r="E87" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F84" s="22" t="s">
+      <c r="F87" s="22" t="s">
         <v>273</v>
       </c>
-      <c r="G84" s="38">
-        <f>G81*G$31</f>
+      <c r="G87" s="38">
+        <f>G84*G$31</f>
         <v>271928.84259161429</v>
       </c>
-      <c r="H84" s="38">
-        <f>H81*H$31</f>
+      <c r="H87" s="38">
+        <f>H84*H$31</f>
         <v>109637.80079561732</v>
       </c>
-      <c r="I84" s="38">
-        <f>I81*I$31</f>
+      <c r="I87" s="38">
+        <f>I84*I$31</f>
         <v>571050.56944239</v>
       </c>
-      <c r="J84" s="38">
-        <f>J81*J$31</f>
+      <c r="J87" s="38">
+        <f>J84*J$31</f>
         <v>76746.460556932128</v>
       </c>
     </row>
-    <row r="85" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="G85" s="4"/>
-      <c r="H85" s="4"/>
-      <c r="I85" s="4"/>
-      <c r="J85" s="4"/>
-    </row>
-    <row r="86" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="G86" s="4" t="s">
+    <row r="88" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="G88" s="4"/>
+      <c r="H88" s="4"/>
+      <c r="I88" s="4"/>
+      <c r="J88" s="4"/>
+    </row>
+    <row r="89" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="G89" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="H86" s="4" t="s">
+      <c r="H89" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="I86" s="4" t="s">
+      <c r="I89" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="J86" s="4" t="s">
+      <c r="J89" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="L86" t="s">
+      <c r="L89" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="87" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B87" s="23" t="s">
+    <row r="90" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B90" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="C87" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="D87" s="19" t="s">
+      <c r="C90" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="D90" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="E87" s="19" t="s">
+      <c r="E90" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="F87" s="19" t="s">
+      <c r="F90" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="G87" s="19">
+      <c r="G90" s="19">
         <f>'linear regressions counts'!M43</f>
         <v>6.7506893569518861E-2</v>
       </c>
-      <c r="H87" s="19">
+      <c r="H90" s="19">
         <f>'linear regressions counts'!M66</f>
         <v>5.5539298723601756E-2</v>
       </c>
-      <c r="I87" s="19">
+      <c r="I90" s="19">
         <f>'linear regressions counts'!M43</f>
         <v>6.7506893569518861E-2</v>
       </c>
-      <c r="J87" s="19">
+      <c r="J90" s="19">
         <f>'linear regressions counts'!M66</f>
         <v>5.5539298723601756E-2</v>
-      </c>
-    </row>
-    <row r="88" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B88" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="C88" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="D88" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="E88" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="F88" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="G88" s="19">
-        <v>4373730</v>
-      </c>
-      <c r="H88" s="19">
-        <v>4373730</v>
-      </c>
-      <c r="I88" s="19">
-        <v>4373730</v>
-      </c>
-      <c r="J88" s="19">
-        <v>4373730</v>
-      </c>
-    </row>
-    <row r="89" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B89" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="C89" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="D89" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="E89" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="F89" s="19" t="s">
-        <v>87</v>
-      </c>
-      <c r="G89" s="20">
-        <f>(G87*G$76)/(G88*G$39*10^9)</f>
-        <v>14299.923031581789</v>
-      </c>
-      <c r="H89" s="20">
-        <f>(H87*H$76)/(H88*H$39*10^9)</f>
-        <v>11764.838448056504</v>
-      </c>
-      <c r="I89" s="20">
-        <f>(I87*I$76)/(I88*I$39*10^9)</f>
-        <v>14299.923031581789</v>
-      </c>
-      <c r="J89" s="20">
-        <f>(J87*J$76)/(J88*J$39*10^9)</f>
-        <v>11764.838448056504</v>
-      </c>
-    </row>
-    <row r="90" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B90" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="C90" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="D90" s="19" t="s">
-        <v>95</v>
-      </c>
-      <c r="E90" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="F90" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="G90" s="19">
-        <f>G89/G$34</f>
-        <v>2859.9846063163577</v>
-      </c>
-      <c r="H90" s="19">
-        <f>H89/H$34</f>
-        <v>2471.604715978257</v>
-      </c>
-      <c r="I90" s="19">
-        <f>I89/I$34</f>
-        <v>2859.9846063163577</v>
-      </c>
-      <c r="J90" s="19">
-        <f>J89/J$34</f>
-        <v>2471.604715978257</v>
       </c>
     </row>
     <row r="91" spans="2:12" x14ac:dyDescent="0.2">
@@ -7691,29 +7853,25 @@
         <v>1</v>
       </c>
       <c r="D91" s="19" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="E91" s="19" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="F91" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="G91" s="33">
-        <f>G90*10^9</f>
-        <v>2859984606316.3579</v>
-      </c>
-      <c r="H91" s="33">
-        <f>H90*10^9</f>
-        <v>2471604715978.2568</v>
-      </c>
-      <c r="I91" s="33">
-        <f>I90*10^9</f>
-        <v>2859984606316.3579</v>
-      </c>
-      <c r="J91" s="33">
-        <f>J90*10^9</f>
-        <v>2471604715978.2568</v>
+        <v>84</v>
+      </c>
+      <c r="G91" s="19">
+        <v>4373730</v>
+      </c>
+      <c r="H91" s="19">
+        <v>4373730</v>
+      </c>
+      <c r="I91" s="19">
+        <v>4373730</v>
+      </c>
+      <c r="J91" s="19">
+        <v>4373730</v>
       </c>
     </row>
     <row r="92" spans="2:12" x14ac:dyDescent="0.2">
@@ -7724,29 +7882,29 @@
         <v>1</v>
       </c>
       <c r="D92" s="19" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="E92" s="19" t="s">
         <v>13</v>
       </c>
       <c r="F92" s="19" t="s">
-        <v>102</v>
-      </c>
-      <c r="G92" s="39">
-        <f>G91*G$29</f>
-        <v>20553974.733352304</v>
-      </c>
-      <c r="H92" s="39">
-        <f>H91*H$29</f>
-        <v>11732952.009540385</v>
-      </c>
-      <c r="I92" s="39">
-        <f>I91*I$29</f>
-        <v>43163346.940039828</v>
-      </c>
-      <c r="J92" s="39">
-        <f>J91*J$29</f>
-        <v>8213066.4066782696</v>
+        <v>87</v>
+      </c>
+      <c r="G92" s="20">
+        <f>(G90*G$79)/(G91*G$42*10^9)</f>
+        <v>14299.923031581789</v>
+      </c>
+      <c r="H92" s="20">
+        <f>(H90*H$79)/(H91*H$42*10^9)</f>
+        <v>11764.838448056504</v>
+      </c>
+      <c r="I92" s="20">
+        <f>(I90*I$79)/(I91*I$42*10^9)</f>
+        <v>14299.923031581789</v>
+      </c>
+      <c r="J92" s="20">
+        <f>(J90*J$79)/(J91*J$42*10^9)</f>
+        <v>11764.838448056504</v>
       </c>
     </row>
     <row r="93" spans="2:12" x14ac:dyDescent="0.2">
@@ -7757,29 +7915,29 @@
         <v>1</v>
       </c>
       <c r="D93" s="19" t="s">
-        <v>270</v>
+        <v>95</v>
       </c>
       <c r="E93" s="19" t="s">
         <v>13</v>
       </c>
       <c r="F93" s="19" t="s">
-        <v>271</v>
-      </c>
-      <c r="G93" s="39">
-        <f>G91*G$30</f>
-        <v>2859.9846063163582</v>
-      </c>
-      <c r="H93" s="39">
-        <f>H91*H$30</f>
-        <v>2306.8310682463734</v>
-      </c>
-      <c r="I93" s="39">
-        <f>I91*I$30</f>
-        <v>6005.967673264352</v>
-      </c>
-      <c r="J93" s="39">
-        <f>J91*J$30</f>
-        <v>1614.7817477724611</v>
+        <v>96</v>
+      </c>
+      <c r="G93" s="19">
+        <f>G92/G$34</f>
+        <v>2859.9846063163577</v>
+      </c>
+      <c r="H93" s="19">
+        <f>H92/H$34</f>
+        <v>2471.604715978257</v>
+      </c>
+      <c r="I93" s="19">
+        <f>I92/I$34</f>
+        <v>2859.9846063163577</v>
+      </c>
+      <c r="J93" s="19">
+        <f>J92/J$34</f>
+        <v>2471.604715978257</v>
       </c>
     </row>
     <row r="94" spans="2:12" x14ac:dyDescent="0.2">
@@ -7790,183 +7948,187 @@
         <v>1</v>
       </c>
       <c r="D94" s="19" t="s">
-        <v>272</v>
+        <v>98</v>
       </c>
       <c r="E94" s="19" t="s">
         <v>13</v>
       </c>
       <c r="F94" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="G94" s="33">
+        <f>G93*10^9</f>
+        <v>2859984606316.3579</v>
+      </c>
+      <c r="H94" s="33">
+        <f>H93*10^9</f>
+        <v>2471604715978.2568</v>
+      </c>
+      <c r="I94" s="33">
+        <f>I93*10^9</f>
+        <v>2859984606316.3579</v>
+      </c>
+      <c r="J94" s="33">
+        <f>J93*10^9</f>
+        <v>2471604715978.2568</v>
+      </c>
+    </row>
+    <row r="95" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B95" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C95" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="D95" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="E95" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="F95" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="G95" s="39">
+        <f>G94*G$29</f>
+        <v>20553974.733352304</v>
+      </c>
+      <c r="H95" s="39">
+        <f>H94*H$29</f>
+        <v>11732952.009540385</v>
+      </c>
+      <c r="I95" s="39">
+        <f>I94*I$29</f>
+        <v>43163346.940039828</v>
+      </c>
+      <c r="J95" s="39">
+        <f>J94*J$29</f>
+        <v>8213066.4066782696</v>
+      </c>
+    </row>
+    <row r="96" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B96" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C96" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="D96" s="19" t="s">
+        <v>270</v>
+      </c>
+      <c r="E96" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="F96" s="19" t="s">
+        <v>271</v>
+      </c>
+      <c r="G96" s="39">
+        <f>G94*G$30</f>
+        <v>2859.9846063163582</v>
+      </c>
+      <c r="H96" s="39">
+        <f>H94*H$30</f>
+        <v>2306.8310682463734</v>
+      </c>
+      <c r="I96" s="39">
+        <f>I94*I$30</f>
+        <v>6005.967673264352</v>
+      </c>
+      <c r="J96" s="39">
+        <f>J94*J$30</f>
+        <v>1614.7817477724611</v>
+      </c>
+    </row>
+    <row r="97" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B97" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C97" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="D97" s="19" t="s">
+        <v>272</v>
+      </c>
+      <c r="E97" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="F97" s="19" t="s">
         <v>273</v>
       </c>
-      <c r="G94" s="39">
-        <f>G91*G$31</f>
+      <c r="G97" s="39">
+        <f>G94*G$31</f>
         <v>142999.2303158179</v>
       </c>
-      <c r="H94" s="39">
-        <f>H91*H$31</f>
+      <c r="H97" s="39">
+        <f>H94*H$31</f>
         <v>57670.776706159326</v>
       </c>
-      <c r="I94" s="39">
-        <f>I91*I$31</f>
+      <c r="I97" s="39">
+        <f>I94*I$31</f>
         <v>300298.3836632176</v>
       </c>
-      <c r="J94" s="39">
-        <f>J91*J$31</f>
+      <c r="J97" s="39">
+        <f>J94*J$31</f>
         <v>40369.543694311527</v>
       </c>
     </row>
-    <row r="95" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="G95" s="4"/>
-      <c r="H95" s="4"/>
-      <c r="I95" s="4"/>
-      <c r="J95" s="4"/>
-    </row>
-    <row r="96" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="G96" s="4" t="s">
+    <row r="98" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="G98" s="4"/>
+      <c r="H98" s="4"/>
+      <c r="I98" s="4"/>
+      <c r="J98" s="4"/>
+    </row>
+    <row r="99" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="G99" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="H96" s="4" t="s">
+      <c r="H99" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="I96" s="4" t="s">
+      <c r="I99" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="J96" s="4" t="s">
+      <c r="J99" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="L96" t="s">
+      <c r="L99" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="97" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B97" s="16" t="s">
+    <row r="100" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B100" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="C97" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="D97" s="17" t="s">
+      <c r="C100" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="D100" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="E97" s="17" t="s">
+      <c r="E100" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="F97" s="17" t="s">
+      <c r="F100" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="G97" s="24">
+      <c r="G100" s="24">
         <f>'linear regressions counts'!M48</f>
         <v>5.5800097113146443E-4</v>
       </c>
-      <c r="H97" s="24">
+      <c r="H100" s="24">
         <f>'linear regressions counts'!M71</f>
         <v>4.5576142039897643E-4</v>
       </c>
-      <c r="I97" s="24">
+      <c r="I100" s="24">
         <f>'linear regressions counts'!M48</f>
         <v>5.5800097113146443E-4</v>
       </c>
-      <c r="J97" s="24">
+      <c r="J100" s="24">
         <f>'linear regressions counts'!M71</f>
         <v>4.5576142039897643E-4</v>
       </c>
     </row>
-    <row r="98" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B98" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="C98" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="D98" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="E98" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="F98" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="G98" s="25">
-        <v>89264</v>
-      </c>
-      <c r="H98" s="25">
-        <v>89264</v>
-      </c>
-      <c r="I98" s="25">
-        <v>89264</v>
-      </c>
-      <c r="J98" s="25">
-        <v>89264</v>
-      </c>
-    </row>
-    <row r="99" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B99" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="C99" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="D99" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="E99" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="F99" s="19" t="s">
-        <v>87</v>
-      </c>
-      <c r="G99" s="20">
-        <f>(G97*G$76)/(G98*G$39*10^9)</f>
-        <v>5791.5679546416768</v>
-      </c>
-      <c r="H99" s="20">
-        <f>(H97*H$76)/(H98*H$39*10^9)</f>
-        <v>4730.4097553672618</v>
-      </c>
-      <c r="I99" s="20">
-        <f>(I97*I$76)/(I98*I$39*10^9)</f>
-        <v>5791.5679546416768</v>
-      </c>
-      <c r="J99" s="20">
-        <f>(J97*J$76)/(J98*J$39*10^9)</f>
-        <v>4730.4097553672618</v>
-      </c>
-    </row>
-    <row r="100" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B100" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="C100" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="D100" s="19" t="s">
-        <v>95</v>
-      </c>
-      <c r="E100" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="F100" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="G100" s="25">
-        <f>G99/G$34</f>
-        <v>1158.3135909283353</v>
-      </c>
-      <c r="H100" s="25">
-        <f>H99/H$34</f>
-        <v>993.78356205194575</v>
-      </c>
-      <c r="I100" s="25">
-        <f>I99/I$34</f>
-        <v>1158.3135909283353</v>
-      </c>
-      <c r="J100" s="25">
-        <f>J99/J$34</f>
-        <v>993.78356205194575</v>
-      </c>
-    </row>
-    <row r="101" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B101" s="18" t="s">
         <v>82</v>
       </c>
@@ -7974,32 +8136,28 @@
         <v>1</v>
       </c>
       <c r="D101" s="19" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="E101" s="19" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="F101" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="G101" s="41">
-        <f>G100*10^9</f>
-        <v>1158313590928.3352</v>
-      </c>
-      <c r="H101" s="41">
-        <f>H100*10^9</f>
-        <v>993783562051.9458</v>
-      </c>
-      <c r="I101" s="41">
-        <f>I100*10^9</f>
-        <v>1158313590928.3352</v>
-      </c>
-      <c r="J101" s="41">
-        <f>J100*10^9</f>
-        <v>993783562051.9458</v>
-      </c>
-    </row>
-    <row r="102" spans="2:10" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+      <c r="G101" s="25">
+        <v>89264</v>
+      </c>
+      <c r="H101" s="25">
+        <v>89264</v>
+      </c>
+      <c r="I101" s="25">
+        <v>89264</v>
+      </c>
+      <c r="J101" s="25">
+        <v>89264</v>
+      </c>
+    </row>
+    <row r="102" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B102" s="18" t="s">
         <v>82</v>
       </c>
@@ -8007,32 +8165,32 @@
         <v>1</v>
       </c>
       <c r="D102" s="19" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="E102" s="19" t="s">
         <v>13</v>
       </c>
       <c r="F102" s="19" t="s">
-        <v>102</v>
-      </c>
-      <c r="G102" s="47">
-        <f>G101*G$29</f>
-        <v>8324502.2468509236</v>
-      </c>
-      <c r="H102" s="47">
-        <f>H101*H$29</f>
-        <v>4717588.8466496002</v>
-      </c>
-      <c r="I102" s="47">
-        <f>I101*I$29</f>
-        <v>17481454.718386941</v>
-      </c>
-      <c r="J102" s="47">
-        <f>J101*J$29</f>
-        <v>3302312.1926547205</v>
-      </c>
-    </row>
-    <row r="103" spans="2:10" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+      <c r="G102" s="20">
+        <f>(G100*G$79)/(G101*G$42*10^9)</f>
+        <v>5791.5679546416768</v>
+      </c>
+      <c r="H102" s="20">
+        <f>(H100*H$79)/(H101*H$42*10^9)</f>
+        <v>4730.4097553672618</v>
+      </c>
+      <c r="I102" s="20">
+        <f>(I100*I$79)/(I101*I$42*10^9)</f>
+        <v>5791.5679546416768</v>
+      </c>
+      <c r="J102" s="20">
+        <f>(J100*J$79)/(J101*J$42*10^9)</f>
+        <v>4730.4097553672618</v>
+      </c>
+    </row>
+    <row r="103" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B103" s="18" t="s">
         <v>82</v>
       </c>
@@ -8040,66 +8198,165 @@
         <v>1</v>
       </c>
       <c r="D103" s="19" t="s">
-        <v>270</v>
+        <v>95</v>
       </c>
       <c r="E103" s="19" t="s">
         <v>13</v>
       </c>
       <c r="F103" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="G103" s="25">
+        <f>G102/G$34</f>
+        <v>1158.3135909283353</v>
+      </c>
+      <c r="H103" s="25">
+        <f>H102/H$34</f>
+        <v>993.78356205194575</v>
+      </c>
+      <c r="I103" s="25">
+        <f>I102/I$34</f>
+        <v>1158.3135909283353</v>
+      </c>
+      <c r="J103" s="25">
+        <f>J102/J$34</f>
+        <v>993.78356205194575</v>
+      </c>
+    </row>
+    <row r="104" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B104" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="C104" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="D104" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="E104" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="F104" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="G104" s="41">
+        <f>G103*10^9</f>
+        <v>1158313590928.3352</v>
+      </c>
+      <c r="H104" s="41">
+        <f>H103*10^9</f>
+        <v>993783562051.9458</v>
+      </c>
+      <c r="I104" s="41">
+        <f>I103*10^9</f>
+        <v>1158313590928.3352</v>
+      </c>
+      <c r="J104" s="41">
+        <f>J103*10^9</f>
+        <v>993783562051.9458</v>
+      </c>
+    </row>
+    <row r="105" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B105" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="C105" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="D105" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="E105" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="F105" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="G105" s="47">
+        <f>G104*G$29</f>
+        <v>8324502.2468509236</v>
+      </c>
+      <c r="H105" s="47">
+        <f>H104*H$29</f>
+        <v>4717588.8466496002</v>
+      </c>
+      <c r="I105" s="47">
+        <f>I104*I$29</f>
+        <v>17481454.718386941</v>
+      </c>
+      <c r="J105" s="47">
+        <f>J104*J$29</f>
+        <v>3302312.1926547205</v>
+      </c>
+    </row>
+    <row r="106" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B106" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="C106" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="D106" s="19" t="s">
+        <v>270</v>
+      </c>
+      <c r="E106" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="F106" s="19" t="s">
         <v>271</v>
       </c>
-      <c r="G103" s="39">
-        <f>G101*G$30</f>
+      <c r="G106" s="39">
+        <f>G104*G$30</f>
         <v>1158.3135909283353</v>
       </c>
-      <c r="H103" s="39">
-        <f>H101*H$30</f>
+      <c r="H106" s="39">
+        <f>H104*H$30</f>
         <v>927.53132458181619</v>
       </c>
-      <c r="I103" s="39">
-        <f>I101*I$30</f>
+      <c r="I106" s="39">
+        <f>I104*I$30</f>
         <v>2432.4585409495044</v>
       </c>
-      <c r="J103" s="39">
-        <f>J101*J$30</f>
+      <c r="J106" s="39">
+        <f>J104*J$30</f>
         <v>649.27192720727123</v>
       </c>
     </row>
-    <row r="104" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B104" s="21" t="s">
+    <row r="107" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B107" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="C104" s="22" t="b">
-        <v>1</v>
-      </c>
-      <c r="D104" s="22" t="s">
+      <c r="C107" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="D107" s="22" t="s">
         <v>272</v>
       </c>
-      <c r="E104" s="22" t="s">
+      <c r="E107" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F104" s="22" t="s">
+      <c r="F107" s="22" t="s">
         <v>273</v>
       </c>
-      <c r="G104" s="38">
-        <f>G101*G$31</f>
+      <c r="G107" s="38">
+        <f>G104*G$31</f>
         <v>57915.679546416766</v>
       </c>
-      <c r="H104" s="38">
-        <f>H101*H$31</f>
+      <c r="H107" s="38">
+        <f>H104*H$31</f>
         <v>23188.283114545404</v>
       </c>
-      <c r="I104" s="38">
-        <f>I101*I$31</f>
+      <c r="I107" s="38">
+        <f>I104*I$31</f>
         <v>121622.9270474752</v>
       </c>
-      <c r="J104" s="38">
-        <f>J101*J$31</f>
+      <c r="J107" s="38">
+        <f>J104*J$31</f>
         <v>16231.798180181782</v>
       </c>
     </row>
-    <row r="106" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="G106" s="3"/>
+    <row r="109" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="G109" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8109,11 +8366,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFC0DD12-9F50-4C4C-88FA-79E5E161A3E2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFC0DD12-9F50-4C4C-88FA-79E5E161A3E2}">
   <dimension ref="A1:M146"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="J40" sqref="J40:J48"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8205,7 +8462,7 @@
         <v>121</v>
       </c>
       <c r="E16" t="s">
-        <v>122</v>
+        <v>319</v>
       </c>
       <c r="F16" t="s">
         <v>123</v>
@@ -11097,15 +11354,16 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7E102CF-57E9-CF4D-8304-DA1926A37703}">
-  <dimension ref="A1:AU58"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7E102CF-57E9-CF4D-8304-DA1926A37703}">
+  <dimension ref="A1:AT58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB29" workbookViewId="0">
-      <selection activeCell="Q43" sqref="Q43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11230,7 +11488,7 @@
         <v>121</v>
       </c>
       <c r="E16" t="s">
-        <v>122</v>
+        <v>319</v>
       </c>
       <c r="F16" t="s">
         <v>123</v>
@@ -11790,7 +12048,7 @@
         <v>1.19</v>
       </c>
     </row>
-    <row r="33" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>128</v>
       </c>
@@ -11823,7 +12081,7 @@
         <v>7.24</v>
       </c>
     </row>
-    <row r="34" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>129</v>
       </c>
@@ -11856,7 +12114,7 @@
         <v>92.65</v>
       </c>
     </row>
-    <row r="35" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>130</v>
       </c>
@@ -11886,7 +12144,7 @@
         <v>3.58</v>
       </c>
     </row>
-    <row r="36" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>131</v>
       </c>
@@ -11919,7 +12177,7 @@
         <v>4.24</v>
       </c>
     </row>
-    <row r="37" spans="1:47" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:46" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="30" t="s">
         <v>132</v>
       </c>
@@ -11952,7 +12210,7 @@
         <v>0.72</v>
       </c>
     </row>
-    <row r="38" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:46" x14ac:dyDescent="0.2">
       <c r="J38" t="s">
         <v>293</v>
       </c>
@@ -11976,7 +12234,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="39" spans="1:47" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:46" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>133</v>
       </c>
@@ -11991,7 +12249,7 @@
         <v>1.3894854164478233E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A40" s="31"/>
       <c r="B40" s="31" t="s">
         <v>138</v>
@@ -12019,7 +12277,7 @@
         <v>1.1408701284690223E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>134</v>
       </c>
@@ -12069,7 +12327,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="42" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>135</v>
       </c>
@@ -12129,7 +12387,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="43" spans="1:47" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:46" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="30" t="s">
         <v>136</v>
       </c>
@@ -12163,7 +12421,7 @@
         <v>287</v>
       </c>
       <c r="Z43" s="51">
-        <f>'full_calcs on correct masses '!G78</f>
+        <f>'full_calcs on correct masses '!G81</f>
         <v>1904788.3330000001</v>
       </c>
       <c r="AB43" t="s">
@@ -12173,7 +12431,7 @@
         <v>287</v>
       </c>
       <c r="AJ43" s="51">
-        <f>(Q43*6.02214076E+23)/(Z43*650*1000000000)</f>
+        <f t="shared" ref="AJ43:AJ48" si="5">(Q43*6.02214076E+23)/(Z43*650*1000000000)</f>
         <v>27192.884259161423</v>
       </c>
       <c r="AL43" s="48" t="s">
@@ -12199,10 +12457,9 @@
         <f>$AM53*'full_calcs on correct masses '!$G$29</f>
         <v>39085654.849706717</v>
       </c>
-      <c r="AT43" s="54"/>
-      <c r="AU43" s="55"/>
-    </row>
-    <row r="44" spans="1:47" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AT43" s="9"/>
+    </row>
+    <row r="44" spans="1:46" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="K44" t="str">
         <v>Veillonella dispar</v>
       </c>
@@ -12224,7 +12481,7 @@
         <v>289</v>
       </c>
       <c r="Z44" s="51">
-        <f>'full_calcs on correct masses '!G88</f>
+        <f>'full_calcs on correct masses '!G91</f>
         <v>4373730</v>
       </c>
       <c r="AB44" t="s">
@@ -12234,7 +12491,7 @@
         <v>289</v>
       </c>
       <c r="AJ44" s="51">
-        <f>(Q44*6.02214076E+23)/(Z44*650*1000000000)</f>
+        <f t="shared" si="5"/>
         <v>14299.923031581789</v>
       </c>
       <c r="AL44" s="48" t="s">
@@ -12260,10 +12517,9 @@
         <f>$AM54*'full_calcs on correct masses '!$G$29</f>
         <v>20553974.733352304</v>
       </c>
-      <c r="AT44" s="54"/>
-      <c r="AU44" s="55"/>
-    </row>
-    <row r="45" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="AT44" s="9"/>
+    </row>
+    <row r="45" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A45" s="31"/>
       <c r="B45" s="31" t="s">
         <v>143</v>
@@ -12309,7 +12565,7 @@
         <v>290</v>
       </c>
       <c r="AJ45" s="51">
-        <f>(Q45*6.02214076E+23)/(Z45*650*1000000000)</f>
+        <f t="shared" si="5"/>
         <v>16299.787186793354</v>
       </c>
       <c r="AL45" s="48" t="s">
@@ -12333,9 +12589,8 @@
         <f>$AM55*'full_calcs on correct masses '!$G$29</f>
         <v>23428476.730710857</v>
       </c>
-      <c r="AU45" s="55"/>
-    </row>
-    <row r="46" spans="1:47" x14ac:dyDescent="0.2">
+    </row>
+    <row r="46" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>137</v>
       </c>
@@ -12383,7 +12638,7 @@
         <v>291</v>
       </c>
       <c r="AJ46" s="51">
-        <f>(Q46*6.02214076E+23)/(Z46*650*1000000000)</f>
+        <f t="shared" si="5"/>
         <v>1743.4155799445389</v>
       </c>
       <c r="AL46" s="48" t="s">
@@ -12407,9 +12662,8 @@
         <f>$AM56*'full_calcs on correct masses '!$G$29</f>
         <v>2505895.9898435902</v>
       </c>
-      <c r="AU46" s="55"/>
-    </row>
-    <row r="47" spans="1:47" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:46" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="30" t="s">
         <v>166</v>
       </c>
@@ -12457,7 +12711,7 @@
         <v>292</v>
       </c>
       <c r="AJ47" s="51">
-        <f>(Q47*6.02214076E+23)/(Z47*650*1000000000)</f>
+        <f t="shared" si="5"/>
         <v>1173.2048127369269</v>
       </c>
       <c r="AL47" s="48" t="s">
@@ -12481,9 +12735,8 @@
         <f>$AM57*'full_calcs on correct masses '!$G$29</f>
         <v>1686304.3265887243</v>
       </c>
-      <c r="AU47" s="55"/>
-    </row>
-    <row r="48" spans="1:47" x14ac:dyDescent="0.2">
+    </row>
+    <row r="48" spans="1:46" x14ac:dyDescent="0.2">
       <c r="P48" s="48" t="s">
         <v>293</v>
       </c>
@@ -12495,7 +12748,7 @@
         <v>293</v>
       </c>
       <c r="Z48" s="51">
-        <f>'full_calcs on correct masses '!G98</f>
+        <f>'full_calcs on correct masses '!G101</f>
         <v>89264</v>
       </c>
       <c r="AB48" t="s">
@@ -12505,7 +12758,7 @@
         <v>293</v>
       </c>
       <c r="AJ48" s="51">
-        <f>(Q48*6.02214076E+23)/(Z48*650*1000000000)</f>
+        <f t="shared" si="5"/>
         <v>5791.5679546416768</v>
       </c>
       <c r="AL48" s="48" t="s">
@@ -12531,8 +12784,7 @@
         <f>$AM58*'full_calcs on correct masses '!$G$29</f>
         <v>8324502.2468509236</v>
       </c>
-      <c r="AT48" s="54"/>
-      <c r="AU48" s="55"/>
+      <c r="AT48" s="9"/>
     </row>
     <row r="50" spans="35:46" x14ac:dyDescent="0.2">
       <c r="AI50" t="s">
@@ -12588,7 +12840,7 @@
         <v>287</v>
       </c>
       <c r="AJ53" s="51">
-        <f>'full_calcs on correct masses '!G79</f>
+        <f>'full_calcs on correct masses '!G82</f>
         <v>27192.884259161423</v>
       </c>
       <c r="AK53" t="s">
@@ -12598,7 +12850,7 @@
         <v>287</v>
       </c>
       <c r="AM53" s="52">
-        <f>'full_calcs on correct masses '!G81</f>
+        <f>'full_calcs on correct masses '!G84</f>
         <v>5438576851832.2852</v>
       </c>
       <c r="AN53" s="53" t="s">
@@ -12608,7 +12860,7 @@
         <v>287</v>
       </c>
       <c r="AP53" s="51">
-        <f>'full_calcs on correct masses '!$G$82</f>
+        <f>'full_calcs on correct masses '!$G$85</f>
         <v>39085654.849706717</v>
       </c>
       <c r="AQ53" s="53" t="s">
@@ -12618,7 +12870,7 @@
         <v>287</v>
       </c>
       <c r="AS53" s="51">
-        <f>'full_calcs on correct masses '!$G$82</f>
+        <f>'full_calcs on correct masses '!$G$85</f>
         <v>39085654.849706717</v>
       </c>
       <c r="AT53" s="53" t="s">
@@ -12630,7 +12882,7 @@
         <v>289</v>
       </c>
       <c r="AJ54" s="51">
-        <f>'full_calcs on correct masses '!G89</f>
+        <f>'full_calcs on correct masses '!G92</f>
         <v>14299.923031581789</v>
       </c>
       <c r="AK54" t="s">
@@ -12640,7 +12892,7 @@
         <v>289</v>
       </c>
       <c r="AM54" s="52">
-        <f>'full_calcs on correct masses '!G91</f>
+        <f>'full_calcs on correct masses '!G94</f>
         <v>2859984606316.3579</v>
       </c>
       <c r="AN54" s="53" t="s">
@@ -12650,7 +12902,7 @@
         <v>289</v>
       </c>
       <c r="AP54" s="51">
-        <f>'full_calcs on correct masses '!$G$92</f>
+        <f>'full_calcs on correct masses '!$G$95</f>
         <v>20553974.733352304</v>
       </c>
       <c r="AQ54" s="53" t="s">
@@ -12660,7 +12912,7 @@
         <v>289</v>
       </c>
       <c r="AS54" s="51">
-        <f>'full_calcs on correct masses '!$G$92</f>
+        <f>'full_calcs on correct masses '!$G$95</f>
         <v>20553974.733352304</v>
       </c>
       <c r="AT54" s="53" t="s">
@@ -12762,7 +13014,7 @@
         <v>293</v>
       </c>
       <c r="AJ58" s="51">
-        <f>'full_calcs on correct masses '!G99</f>
+        <f>'full_calcs on correct masses '!G102</f>
         <v>5791.5679546416768</v>
       </c>
       <c r="AK58" t="s">
@@ -12772,7 +13024,7 @@
         <v>293</v>
       </c>
       <c r="AM58" s="52">
-        <f>'full_calcs on correct masses '!G101</f>
+        <f>'full_calcs on correct masses '!G104</f>
         <v>1158313590928.3352</v>
       </c>
       <c r="AN58" s="53" t="s">
@@ -12782,7 +13034,7 @@
         <v>293</v>
       </c>
       <c r="AP58" s="51">
-        <f>'full_calcs on correct masses '!$G$102</f>
+        <f>'full_calcs on correct masses '!$G$105</f>
         <v>8324502.2468509236</v>
       </c>
       <c r="AQ58" s="53" t="s">
@@ -12792,7 +13044,7 @@
         <v>293</v>
       </c>
       <c r="AS58" s="51">
-        <f>'full_calcs on correct masses '!$G$102</f>
+        <f>'full_calcs on correct masses '!$G$105</f>
         <v>8324502.2468509236</v>
       </c>
       <c r="AT58" s="53" t="s">
@@ -12803,6 +13055,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>